<commit_message>
updated list of algos
</commit_message>
<xml_diff>
--- a/Algorithm_Topics _to_Learn.xlsx
+++ b/Algorithm_Topics _to_Learn.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="292">
   <si>
     <t>From Quora:</t>
   </si>
@@ -275,9 +275,6 @@
     <t>Data Structures:</t>
   </si>
   <si>
-    <t>Linked List</t>
-  </si>
-  <si>
     <t>Trees (Binary Tree And Binary Search Tree)</t>
   </si>
   <si>
@@ -315,12 +312,6 @@
   </si>
   <si>
     <t>Ternary Search</t>
-  </si>
-  <si>
-    <t>Selection Sort</t>
-  </si>
-  <si>
-    <t>Bubble Sort</t>
   </si>
   <si>
     <t>Insertion Sort</t>
@@ -772,11 +763,6 @@
     <t>(h) Other Important Topics On Graphs</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=7HCd074v8g8
-https://www.geeksforgeeks.org/gcd-two-array-numbers/
-https://www.geeksforgeeks.org/lcm-of-given-array-elements/</t>
-  </si>
-  <si>
     <t>&gt; Find GCD (HCF) divide the highest number with smallest, then make divisor as dividend and remainder as divisor, repeat till 0. For more than two values find answer for two value pairs and repeat
 &gt; LCM (a,b) = a*b/gcd(a,b); for more than two values find the answer for two values and repeat</t>
   </si>
@@ -814,10 +800,6 @@
   </si>
   <si>
     <t>https://www.geeksforgeeks.org/skip-list/</t>
-  </si>
-  <si>
-    <t>&gt; Codechef (Skiplist)
-&gt; Spoj (GSS6)</t>
   </si>
   <si>
     <t>&gt; To search, insert, modify big data, we can use multi level linked list (skip list)</t>
@@ -982,38 +964,10 @@
     <t>Important points/ implementation</t>
   </si>
   <si>
-    <t>&gt; We can find running median of input streams using both min and max heaps</t>
-  </si>
-  <si>
     <t>&gt; The root will be at a[1], so start indexing from 1 and carefully maintain indexing</t>
   </si>
   <si>
     <t>https://www.quora.com/How-do-I-calculate-the-median-of-given-sets-of-numbers-when-the-number-of-elements-in-a-list-are-changed</t>
-  </si>
-  <si>
-    <r>
-      <t>&gt; Spoj (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>RMID2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1172,12 +1126,254 @@
 https://www.codechef.com/certification/prepare#foundation-syllabus
 https://www.geeksforgeeks.org/top-algorithms-and-data-structures-for-competitive-programming/#algo4</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&gt; Spoj (PQUEUE, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RMID2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>&gt; Priority queues are usefull in solving scheduling problems and problems does not require complete data to be sorted
+&gt; We can find running median of input streams using both min and max heaps</t>
+  </si>
+  <si>
+    <r>
+      <t>&gt; Codeforces (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>957A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+   (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Multi cell coloring</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Practice</t>
+  </si>
+  <si>
+    <t>Learned</t>
+  </si>
+  <si>
+    <t>To learn next</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CpZh4eF8QBw</t>
+  </si>
+  <si>
+    <t>&gt; Similar complexity as kmp, but simpler to understand and implement</t>
+  </si>
+  <si>
+    <t>&gt; Codechef (TAEditor, Skiplist)
+&gt; Spoj (GSS6)</t>
+  </si>
+  <si>
+    <t>&gt; Spoj (Gcd)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7HCd074v8g8
+https://www.geeksforgeeks.org/lcm-of-given-array-elements/</t>
+  </si>
+  <si>
+    <t>Arithmetic/Geometric progression</t>
+  </si>
+  <si>
+    <r>
+      <t>&gt; GP n-th term: a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = ar</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (a=initial number, r=common ratio)
+&gt; GP fact: b</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = ac (for 3 consecutive GP series, b is called geometric mean)
+&gt; GP sum = a(1-r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)/(1-r)
+&gt; AP n-th term: a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = a + (n-1)d
+&gt; AP sum = n(a + a</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)/2</t>
+    </r>
+  </si>
+  <si>
+    <t>&gt; Spoj (ANARC05B)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1274,8 +1470,24 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1350,12 +1562,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1363,6 +1569,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1435,7 +1653,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1509,122 +1727,158 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1635,8 +1889,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCCFF"/>
       <color rgb="FF0000FF"/>
-      <color rgb="FFFFCCFF"/>
     </mruColors>
   </colors>
 </styleSheet>
@@ -1927,11 +2181,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:K256"/>
+  <dimension ref="B1:K258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="4" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -1941,1618 +2195,1639 @@
     <col min="3" max="3" width="20" style="4" customWidth="1"/>
     <col min="4" max="4" width="40.88671875" style="4" customWidth="1"/>
     <col min="5" max="5" width="22.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="77.33203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="69.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="78.77734375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="77.77734375" style="4" customWidth="1"/>
     <col min="8" max="10" width="8.88671875" style="4"/>
     <col min="11" max="11" width="18.5546875" style="4" customWidth="1"/>
     <col min="12" max="12" width="8.88671875" style="4" customWidth="1"/>
     <col min="13" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="45.6" customHeight="1">
-      <c r="C2" s="5" t="s">
+    <row r="1" spans="2:11">
+      <c r="C1" s="43" t="s">
+        <v>283</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>281</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" ht="51" customHeight="1">
+      <c r="C2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="19" t="s">
-        <v>231</v>
-      </c>
-      <c r="F2" s="35" t="s">
-        <v>284</v>
-      </c>
-      <c r="G2" s="36"/>
-    </row>
-    <row r="4" spans="2:11" s="3" customFormat="1" ht="25.2" customHeight="1">
+      <c r="E2" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>277</v>
+      </c>
+      <c r="G2" s="51"/>
+    </row>
+    <row r="4" spans="2:11" s="3" customFormat="1">
       <c r="B4" s="20" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E4" s="20"/>
       <c r="F4" s="20" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="124.8">
-      <c r="B5" s="40" t="s">
-        <v>173</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>198</v>
-      </c>
-      <c r="D5" s="55" t="s">
-        <v>249</v>
+      <c r="B5" s="63" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>245</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="9" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="40"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="5" t="s">
+      <c r="B6" s="63"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" s="63"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="K6" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11">
-      <c r="B7" s="40"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="5" t="s">
-        <v>2</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="K7" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="78">
-      <c r="B8" s="40"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="55" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" s="63"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="K8" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="78">
+      <c r="B9" s="63"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="31.2">
-      <c r="B9" s="40"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="10"/>
+      <c r="F9" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10" s="63"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="2:11" ht="31.2">
+      <c r="B11" s="63"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="2:11">
-      <c r="B10" s="40"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="2:11" ht="46.8">
-      <c r="B11" s="40"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="2:11">
-      <c r="B12" s="40"/>
-      <c r="C12" s="37"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="55"/>
       <c r="D12" s="5" t="s">
-        <v>6</v>
+        <v>184</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="2:11" ht="31.2">
-      <c r="B13" s="40"/>
-      <c r="C13" s="37"/>
+    <row r="13" spans="2:11" ht="46.8">
+      <c r="B13" s="63"/>
+      <c r="C13" s="55"/>
       <c r="D13" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="2:11">
-      <c r="B14" s="40"/>
-      <c r="C14" s="37"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="55"/>
       <c r="D14" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="2:11">
-      <c r="B15" s="40"/>
-      <c r="C15" s="37"/>
+    <row r="15" spans="2:11" ht="31.2">
+      <c r="B15" s="63"/>
+      <c r="C15" s="55"/>
       <c r="D15" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="2:11">
-      <c r="B16" s="40"/>
-      <c r="C16" s="37"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="55"/>
       <c r="D16" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="40"/>
-      <c r="C17" s="37"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="55"/>
       <c r="D17" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="40"/>
-      <c r="C18" s="37"/>
+      <c r="B18" s="63"/>
+      <c r="C18" s="55"/>
       <c r="D18" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="40"/>
-      <c r="C19" s="37"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="55"/>
       <c r="D19" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="40"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="7"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="40"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="E21" s="6"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="2:7" ht="31.2">
-      <c r="B22" s="40"/>
-      <c r="C22" s="37" t="s">
-        <v>197</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>15</v>
+    <row r="22" spans="2:7">
+      <c r="B22" s="63"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="E22" s="6"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="B23" s="40"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="5" t="s">
-        <v>16</v>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+    </row>
+    <row r="23" spans="2:7" ht="89.4">
+      <c r="B23" s="63"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="37" t="s">
+        <v>289</v>
       </c>
       <c r="E23" s="6"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="F23" s="49" t="s">
+        <v>290</v>
+      </c>
+      <c r="G23" s="48"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="40"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="5"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="7"/>
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="40"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B25" s="63"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="6"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="2:7" ht="31.2">
-      <c r="B26" s="40"/>
-      <c r="C26" s="37"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="55" t="s">
+        <v>194</v>
+      </c>
       <c r="D26" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="40"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="B27" s="63"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="E27" s="6"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="40"/>
-      <c r="C28" s="37" t="s">
-        <v>232</v>
-      </c>
+      <c r="B28" s="63"/>
+      <c r="C28" s="55"/>
       <c r="D28" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="40"/>
-      <c r="C29" s="37"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="55"/>
       <c r="D29" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="2:7" ht="46.8">
-      <c r="B30" s="40"/>
-      <c r="C30" s="37"/>
+    <row r="30" spans="2:7" ht="31.2">
+      <c r="B30" s="63"/>
+      <c r="C30" s="55"/>
       <c r="D30" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="40"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="B31" s="63"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="6"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
     <row r="32" spans="2:7">
-      <c r="B32" s="40"/>
-      <c r="C32" s="37"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="55" t="s">
+        <v>229</v>
+      </c>
       <c r="D32" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="40"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E33" s="6"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="2:7" ht="31.2">
-      <c r="B34" s="40"/>
-      <c r="C34" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="D34" s="5"/>
+    <row r="34" spans="2:7" ht="46.8">
+      <c r="B34" s="63"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E34" s="6"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="40"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E35" s="6"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="40"/>
-      <c r="C36" s="37" t="s">
-        <v>234</v>
-      </c>
+      <c r="B36" s="63"/>
+      <c r="C36" s="55"/>
       <c r="D36" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="2:7" ht="31.2">
-      <c r="B37" s="40"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="5" t="s">
-        <v>26</v>
-      </c>
+    <row r="37" spans="2:7">
+      <c r="B37" s="63"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
       <c r="E37" s="6"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="2:7" ht="46.8">
-      <c r="B38" s="40"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="5" t="s">
-        <v>27</v>
-      </c>
+    <row r="38" spans="2:7" ht="31.2">
+      <c r="B38" s="63"/>
+      <c r="C38" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="D38" s="5"/>
       <c r="E38" s="6"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="2:7" ht="46.8">
-      <c r="B39" s="40"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="5" t="s">
-        <v>28</v>
-      </c>
+    <row r="39" spans="2:7">
+      <c r="B39" s="63"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="6"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
     </row>
     <row r="40" spans="2:7">
-      <c r="B40" s="40"/>
-      <c r="C40" s="37"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="55" t="s">
+        <v>231</v>
+      </c>
       <c r="D40" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
     </row>
     <row r="41" spans="2:7" ht="31.2">
-      <c r="B41" s="40"/>
-      <c r="C41" s="37"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="55"/>
       <c r="D41" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="2:7">
-      <c r="B42" s="40"/>
-      <c r="C42" s="37"/>
+    <row r="42" spans="2:7" ht="46.8">
+      <c r="B42" s="63"/>
+      <c r="C42" s="55"/>
       <c r="D42" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
     </row>
     <row r="43" spans="2:7" ht="46.8">
-      <c r="B43" s="40"/>
-      <c r="C43" s="37"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="55"/>
       <c r="D43" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
     </row>
     <row r="44" spans="2:7">
-      <c r="B44" s="40"/>
-      <c r="C44" s="37"/>
+      <c r="B44" s="63"/>
+      <c r="C44" s="55"/>
       <c r="D44" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E44" s="6"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="2:7">
-      <c r="B45" s="40"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="53" t="s">
-        <v>188</v>
-      </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="7"/>
+    <row r="45" spans="2:7" ht="31.2">
+      <c r="B45" s="63"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" s="6"/>
+      <c r="F45" s="5"/>
       <c r="G45" s="5"/>
     </row>
     <row r="46" spans="2:7">
-      <c r="B46" s="40"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+      <c r="B46" s="63"/>
+      <c r="C46" s="55"/>
+      <c r="D46" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E46" s="6"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="2:7" ht="31.2">
-      <c r="B47" s="40"/>
-      <c r="C47" s="37" t="s">
-        <v>235</v>
-      </c>
+    <row r="47" spans="2:7" ht="46.8">
+      <c r="B47" s="63"/>
+      <c r="C47" s="55"/>
       <c r="D47" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E47" s="6"/>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
     </row>
     <row r="48" spans="2:7">
-      <c r="B48" s="40"/>
-      <c r="C48" s="37"/>
+      <c r="B48" s="63"/>
+      <c r="C48" s="55"/>
       <c r="D48" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E48" s="6"/>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
     </row>
     <row r="49" spans="2:7">
-      <c r="B49" s="40"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="5"/>
+      <c r="B49" s="63"/>
+      <c r="C49" s="55"/>
+      <c r="D49" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="E49" s="8"/>
+      <c r="F49" s="7"/>
       <c r="G49" s="5"/>
     </row>
     <row r="50" spans="2:7">
-      <c r="B50" s="40"/>
-      <c r="C50" s="37" t="s">
-        <v>236</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>36</v>
-      </c>
+      <c r="B50" s="63"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
       <c r="E50" s="6"/>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
     </row>
-    <row r="51" spans="2:7">
-      <c r="B51" s="40"/>
-      <c r="C51" s="37"/>
+    <row r="51" spans="2:7" ht="31.2">
+      <c r="B51" s="63"/>
+      <c r="C51" s="55" t="s">
+        <v>232</v>
+      </c>
       <c r="D51" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E51" s="6"/>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
     </row>
     <row r="52" spans="2:7">
-      <c r="B52" s="29"/>
-      <c r="C52" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D52" s="5"/>
+      <c r="B52" s="63"/>
+      <c r="C52" s="55"/>
+      <c r="D52" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="E52" s="6"/>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
     </row>
-    <row r="53" spans="2:7" ht="31.2">
-      <c r="B53" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="C53" s="46" t="s">
-        <v>183</v>
-      </c>
-      <c r="D53" s="16"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="30" t="s">
-        <v>253</v>
-      </c>
+    <row r="53" spans="2:7">
+      <c r="B53" s="63"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
     </row>
     <row r="54" spans="2:7">
-      <c r="B54" s="40"/>
-      <c r="C54" s="47"/>
+      <c r="B54" s="63"/>
+      <c r="C54" s="55" t="s">
+        <v>233</v>
+      </c>
       <c r="D54" s="5" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="E54" s="6"/>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
     </row>
-    <row r="55" spans="2:7" ht="31.2">
-      <c r="B55" s="40"/>
-      <c r="C55" s="47"/>
+    <row r="55" spans="2:7">
+      <c r="B55" s="63"/>
+      <c r="C55" s="55"/>
       <c r="D55" s="5" t="s">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="E55" s="6"/>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
     </row>
     <row r="56" spans="2:7">
-      <c r="B56" s="40"/>
-      <c r="C56" s="47"/>
-      <c r="D56" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="B56" s="26"/>
+      <c r="C56" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D56" s="5"/>
       <c r="E56" s="6"/>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
     </row>
-    <row r="57" spans="2:7">
-      <c r="B57" s="40"/>
-      <c r="C57" s="47"/>
-      <c r="D57" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E57" s="6"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-    </row>
-    <row r="58" spans="2:7">
-      <c r="B58" s="40"/>
-      <c r="C58" s="47"/>
+    <row r="57" spans="2:7" ht="31.2">
+      <c r="B57" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57" s="69" t="s">
+        <v>180</v>
+      </c>
+      <c r="D57" s="16"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="27" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" ht="31.2">
+      <c r="B58" s="63"/>
+      <c r="C58" s="70"/>
       <c r="D58" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E58" s="6"/>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
     </row>
-    <row r="59" spans="2:7" ht="31.2">
-      <c r="B59" s="40"/>
-      <c r="C59" s="47"/>
-      <c r="D59" s="55" t="s">
+    <row r="59" spans="2:7">
+      <c r="B59" s="63"/>
+      <c r="C59" s="70"/>
+      <c r="D59" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E59" s="6"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+    </row>
+    <row r="60" spans="2:7">
+      <c r="B60" s="63"/>
+      <c r="C60" s="70"/>
+      <c r="D60" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E60" s="6"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+    </row>
+    <row r="61" spans="2:7">
+      <c r="B61" s="63"/>
+      <c r="C61" s="70"/>
+      <c r="D61" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="E61" s="6"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+    </row>
+    <row r="62" spans="2:7" ht="31.2">
+      <c r="B62" s="63"/>
+      <c r="C62" s="70"/>
+      <c r="D62" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="E62" s="10"/>
+      <c r="F62" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="G62" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7">
+      <c r="B63" s="63"/>
+      <c r="C63" s="70"/>
+      <c r="D63" s="52" t="s">
+        <v>202</v>
+      </c>
+      <c r="E63" s="10"/>
+      <c r="F63" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="G63" s="5"/>
+    </row>
+    <row r="64" spans="2:7" ht="31.2">
+      <c r="B64" s="63"/>
+      <c r="C64" s="70"/>
+      <c r="D64" s="54"/>
+      <c r="E64" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="G64" s="5"/>
+    </row>
+    <row r="65" spans="2:7">
+      <c r="B65" s="63"/>
+      <c r="C65" s="71"/>
+      <c r="D65" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="E59" s="10"/>
-      <c r="F59" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="G59" s="11" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="60" spans="2:7">
-      <c r="B60" s="40"/>
-      <c r="C60" s="47"/>
-      <c r="D60" s="56" t="s">
-        <v>205</v>
-      </c>
-      <c r="E60" s="10"/>
-      <c r="F60" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="G60" s="5"/>
-    </row>
-    <row r="61" spans="2:7" ht="31.2">
-      <c r="B61" s="40"/>
-      <c r="C61" s="47"/>
-      <c r="D61" s="57"/>
-      <c r="E61" s="10" t="s">
+      <c r="E65" s="6"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+    </row>
+    <row r="66" spans="2:7">
+      <c r="B66" s="63"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+    </row>
+    <row r="67" spans="2:7" ht="78">
+      <c r="B67" s="63"/>
+      <c r="C67" s="69" t="s">
+        <v>181</v>
+      </c>
+      <c r="D67" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="F67" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="F61" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="G61" s="5"/>
-    </row>
-    <row r="62" spans="2:7">
-      <c r="B62" s="40"/>
-      <c r="C62" s="48"/>
-      <c r="D62" s="53" t="s">
-        <v>92</v>
-      </c>
-      <c r="E62" s="6"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
-    </row>
-    <row r="63" spans="2:7">
-      <c r="B63" s="40"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-    </row>
-    <row r="64" spans="2:7" ht="78">
-      <c r="B64" s="40"/>
-      <c r="C64" s="46" t="s">
-        <v>184</v>
-      </c>
-      <c r="D64" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="E64" s="10" t="s">
+      <c r="G67" s="11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7">
+      <c r="B68" s="63"/>
+      <c r="C68" s="70"/>
+      <c r="D68" s="53"/>
+      <c r="E68" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="F68" s="9"/>
+      <c r="G68" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="F64" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="G64" s="11" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7">
-      <c r="B65" s="40"/>
-      <c r="C65" s="47"/>
-      <c r="D65" s="58"/>
-      <c r="E65" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="F65" s="9"/>
-      <c r="G65" s="11" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" ht="62.4">
-      <c r="B66" s="40"/>
-      <c r="C66" s="47"/>
-      <c r="D66" s="57"/>
-      <c r="E66" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="G66" s="11"/>
-    </row>
-    <row r="67" spans="2:7" ht="31.2">
-      <c r="B67" s="40"/>
-      <c r="C67" s="47"/>
-      <c r="D67" s="59" t="s">
-        <v>226</v>
-      </c>
-      <c r="E67" s="10"/>
-      <c r="F67" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="G67" s="11" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7">
-      <c r="B68" s="40"/>
-      <c r="C68" s="47"/>
-      <c r="D68" s="26" t="s">
-        <v>271</v>
-      </c>
-      <c r="E68" s="8"/>
-      <c r="F68" s="7"/>
-      <c r="G68" s="11"/>
-    </row>
-    <row r="69" spans="2:7">
-      <c r="B69" s="40"/>
-      <c r="C69" s="47"/>
-      <c r="D69" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="E69" s="8"/>
-      <c r="F69" s="7"/>
-      <c r="G69" s="11" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="70" spans="2:7">
-      <c r="B70" s="40"/>
-      <c r="C70" s="47"/>
-      <c r="D70" s="53" t="s">
-        <v>215</v>
-      </c>
-      <c r="E70" s="8"/>
-      <c r="F70" s="7"/>
-      <c r="G70" s="5"/>
+    </row>
+    <row r="69" spans="2:7" ht="62.4">
+      <c r="B69" s="63"/>
+      <c r="C69" s="70"/>
+      <c r="D69" s="54"/>
+      <c r="E69" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="F69" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="G69" s="11"/>
+    </row>
+    <row r="70" spans="2:7" ht="31.2">
+      <c r="B70" s="63"/>
+      <c r="C70" s="70"/>
+      <c r="D70" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="E70" s="10"/>
+      <c r="F70" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="G70" s="11" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="71" spans="2:7">
-      <c r="B71" s="40"/>
-      <c r="C71" s="47"/>
-      <c r="D71" s="53" t="s">
-        <v>95</v>
+      <c r="B71" s="63"/>
+      <c r="C71" s="70"/>
+      <c r="D71" s="39" t="s">
+        <v>266</v>
       </c>
       <c r="E71" s="8"/>
       <c r="F71" s="7"/>
-      <c r="G71" s="5"/>
-    </row>
-    <row r="72" spans="2:7" ht="124.8">
-      <c r="B72" s="40"/>
-      <c r="C72" s="47"/>
-      <c r="D72" s="56" t="s">
-        <v>213</v>
-      </c>
-      <c r="E72" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="F72" s="9" t="s">
-        <v>263</v>
-      </c>
+      <c r="G71" s="11"/>
+    </row>
+    <row r="72" spans="2:7">
+      <c r="B72" s="63"/>
+      <c r="C72" s="70"/>
+      <c r="D72" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E72" s="8"/>
+      <c r="F72" s="7"/>
       <c r="G72" s="11" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="73" spans="2:7" ht="46.8">
-      <c r="B73" s="40"/>
-      <c r="C73" s="47"/>
-      <c r="D73" s="57"/>
-      <c r="E73" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="F73" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="G73" s="11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7">
+      <c r="B73" s="63"/>
+      <c r="C73" s="70"/>
+      <c r="D73" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="E73" s="8"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="5"/>
+    </row>
+    <row r="74" spans="2:7">
+      <c r="B74" s="63"/>
+      <c r="C74" s="70"/>
+      <c r="D74" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E74" s="8"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="5"/>
+    </row>
+    <row r="75" spans="2:7" ht="124.8">
+      <c r="B75" s="63"/>
+      <c r="C75" s="70"/>
+      <c r="D75" s="56" t="s">
+        <v>210</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="G75" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" ht="46.8">
+      <c r="B76" s="63"/>
+      <c r="C76" s="70"/>
+      <c r="D76" s="57"/>
+      <c r="E76" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="F76" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="G76" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7">
+      <c r="B77" s="63"/>
+      <c r="C77" s="70"/>
+      <c r="D77" s="31" t="s">
+        <v>259</v>
+      </c>
+      <c r="E77" s="8"/>
+      <c r="F77" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="G77" s="11"/>
+    </row>
+    <row r="78" spans="2:7">
+      <c r="B78" s="63"/>
+      <c r="C78" s="70"/>
+      <c r="D78" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="E78" s="8"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="11"/>
+    </row>
+    <row r="79" spans="2:7">
+      <c r="B79" s="63"/>
+      <c r="C79" s="70"/>
+      <c r="D79" s="58" t="s">
+        <v>252</v>
+      </c>
+      <c r="E79" s="21"/>
+      <c r="F79" s="28" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="74" spans="2:7">
-      <c r="B74" s="40"/>
-      <c r="C74" s="47"/>
-      <c r="D74" s="34" t="s">
-        <v>264</v>
-      </c>
-      <c r="E74" s="8"/>
-      <c r="F74" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="G74" s="11"/>
-    </row>
-    <row r="75" spans="2:7">
-      <c r="B75" s="40"/>
-      <c r="C75" s="47"/>
-      <c r="D75" s="53" t="s">
-        <v>214</v>
-      </c>
-      <c r="E75" s="8"/>
-      <c r="F75" s="7"/>
-      <c r="G75" s="11"/>
-    </row>
-    <row r="76" spans="2:7">
-      <c r="B76" s="40"/>
-      <c r="C76" s="47"/>
-      <c r="D76" s="61" t="s">
-        <v>256</v>
-      </c>
-      <c r="E76" s="21"/>
-      <c r="F76" s="31" t="s">
-        <v>259</v>
-      </c>
-      <c r="G76" s="32" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="77" spans="2:7" ht="31.2">
-      <c r="B77" s="40"/>
-      <c r="C77" s="47"/>
-      <c r="D77" s="61"/>
-      <c r="E77" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="F77" s="33" t="s">
-        <v>258</v>
-      </c>
-      <c r="G77" s="32"/>
-    </row>
-    <row r="78" spans="2:7" ht="31.2">
-      <c r="B78" s="40"/>
-      <c r="C78" s="48"/>
-      <c r="D78" s="60" t="s">
-        <v>230</v>
-      </c>
-      <c r="E78" s="12"/>
-      <c r="F78" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="G78" s="11"/>
-    </row>
-    <row r="79" spans="2:7">
-      <c r="B79" s="29"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="5"/>
-      <c r="G79" s="5"/>
-    </row>
-    <row r="80" spans="2:7">
-      <c r="B80" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E80" s="6"/>
-      <c r="F80" s="5"/>
-      <c r="G80" s="5"/>
-    </row>
-    <row r="81" spans="2:7">
-      <c r="B81" s="40"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E81" s="6"/>
-      <c r="F81" s="5"/>
-      <c r="G81" s="5"/>
+      <c r="G79" s="29" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" ht="31.2">
+      <c r="B80" s="63"/>
+      <c r="C80" s="70"/>
+      <c r="D80" s="58"/>
+      <c r="E80" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="F80" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="G80" s="29"/>
+    </row>
+    <row r="81" spans="2:7" ht="31.2">
+      <c r="B81" s="63"/>
+      <c r="C81" s="71"/>
+      <c r="D81" s="34" t="s">
+        <v>227</v>
+      </c>
+      <c r="E81" s="12"/>
+      <c r="F81" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="G81" s="11"/>
     </row>
     <row r="82" spans="2:7">
-      <c r="B82" s="40"/>
+      <c r="B82" s="26"/>
       <c r="C82" s="5"/>
-      <c r="D82" s="5" t="s">
-        <v>99</v>
-      </c>
+      <c r="D82" s="5"/>
       <c r="E82" s="6"/>
       <c r="F82" s="5"/>
       <c r="G82" s="5"/>
     </row>
     <row r="83" spans="2:7">
-      <c r="B83" s="40"/>
+      <c r="B83" s="63" t="s">
+        <v>95</v>
+      </c>
       <c r="C83" s="5"/>
-      <c r="D83" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E83" s="8"/>
-      <c r="F83" s="7"/>
+      <c r="D83" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E83" s="6"/>
+      <c r="F83" s="5"/>
       <c r="G83" s="5"/>
     </row>
     <row r="84" spans="2:7">
-      <c r="B84" s="40"/>
+      <c r="B84" s="63"/>
       <c r="C84" s="5"/>
-      <c r="D84" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="E84" s="6"/>
-      <c r="F84" s="5"/>
+      <c r="D84" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="E84" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="F84" s="49" t="s">
+        <v>291</v>
+      </c>
       <c r="G84" s="5"/>
     </row>
     <row r="85" spans="2:7">
-      <c r="B85" s="40"/>
+      <c r="B85" s="63"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E85" s="6"/>
       <c r="F85" s="5"/>
       <c r="G85" s="5"/>
     </row>
     <row r="86" spans="2:7">
-      <c r="B86" s="40"/>
+      <c r="B86" s="63"/>
       <c r="C86" s="5"/>
-      <c r="D86" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="E86" s="8"/>
-      <c r="F86" s="7"/>
+      <c r="D86" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E86" s="6"/>
+      <c r="F86" s="5"/>
       <c r="G86" s="5"/>
     </row>
     <row r="87" spans="2:7">
-      <c r="B87" s="40"/>
+      <c r="B87" s="63"/>
       <c r="C87" s="5"/>
-      <c r="D87" s="62" t="s">
-        <v>104</v>
+      <c r="D87" s="33" t="s">
+        <v>100</v>
       </c>
       <c r="E87" s="8"/>
       <c r="F87" s="7"/>
       <c r="G87" s="5"/>
     </row>
     <row r="88" spans="2:7">
-      <c r="B88" s="40"/>
+      <c r="B88" s="63"/>
       <c r="C88" s="5"/>
-      <c r="D88" s="7" t="s">
-        <v>105</v>
+      <c r="D88" s="35" t="s">
+        <v>101</v>
       </c>
       <c r="E88" s="8"/>
       <c r="F88" s="7"/>
       <c r="G88" s="5"/>
     </row>
-    <row r="89" spans="2:7" ht="31.2">
-      <c r="B89" s="40"/>
+    <row r="89" spans="2:7">
+      <c r="B89" s="63"/>
       <c r="C89" s="5"/>
-      <c r="D89" s="63" t="s">
-        <v>106</v>
-      </c>
-      <c r="E89" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="F89" s="9" t="s">
-        <v>276</v>
-      </c>
+      <c r="D89" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E89" s="8"/>
+      <c r="F89" s="7"/>
       <c r="G89" s="5"/>
     </row>
-    <row r="90" spans="2:7">
-      <c r="B90" s="40"/>
+    <row r="90" spans="2:7" ht="31.2">
+      <c r="B90" s="63"/>
       <c r="C90" s="5"/>
-      <c r="D90" s="57"/>
-      <c r="E90" s="10"/>
-      <c r="F90" s="9"/>
+      <c r="D90" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>270</v>
+      </c>
       <c r="G90" s="5"/>
     </row>
-    <row r="91" spans="2:7" ht="31.2">
-      <c r="B91" s="40"/>
+    <row r="91" spans="2:7">
+      <c r="B91" s="63"/>
       <c r="C91" s="5"/>
-      <c r="D91" s="63" t="s">
-        <v>273</v>
-      </c>
-      <c r="E91" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="F91" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="G91" s="11" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="92" spans="2:7">
-      <c r="B92" s="40"/>
+      <c r="D91" s="54"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="5"/>
+    </row>
+    <row r="92" spans="2:7" ht="46.8">
+      <c r="B92" s="63"/>
       <c r="C92" s="5"/>
-      <c r="D92" s="57"/>
-      <c r="E92" s="10"/>
+      <c r="D92" s="59" t="s">
+        <v>268</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>269</v>
+      </c>
       <c r="F92" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="G92" s="11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7">
+      <c r="B93" s="63"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="54"/>
+      <c r="E93" s="15"/>
+      <c r="F93" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="G92" s="5"/>
-    </row>
-    <row r="93" spans="2:7">
-      <c r="B93" s="40"/>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E93" s="6"/>
-      <c r="F93" s="5"/>
       <c r="G93" s="5"/>
     </row>
-    <row r="94" spans="2:7" ht="46.8">
-      <c r="B94" s="40"/>
+    <row r="94" spans="2:7">
+      <c r="B94" s="63"/>
       <c r="C94" s="5"/>
-      <c r="D94" s="62" t="s">
-        <v>108</v>
-      </c>
-      <c r="E94" s="21"/>
-      <c r="F94" s="22" t="s">
-        <v>262</v>
-      </c>
-      <c r="G94" s="11" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="95" spans="2:7">
-      <c r="B95" s="29"/>
+      <c r="D94" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E94" s="6"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+    </row>
+    <row r="95" spans="2:7" ht="46.8">
+      <c r="B95" s="63"/>
       <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="6"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="5"/>
+      <c r="D95" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="E95" s="21"/>
+      <c r="F95" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="G95" s="11" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="96" spans="2:7">
-      <c r="B96" s="40" t="s">
+      <c r="B96" s="26"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+    </row>
+    <row r="97" spans="2:7">
+      <c r="B97" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="C97" s="5"/>
+      <c r="D97" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="C96" s="5"/>
-      <c r="D96" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="E96" s="15"/>
-      <c r="F96" s="14"/>
-      <c r="G96" s="5"/>
-    </row>
-    <row r="97" spans="2:7">
-      <c r="B97" s="40"/>
-      <c r="C97" s="5"/>
-      <c r="D97" s="55" t="s">
-        <v>208</v>
-      </c>
-      <c r="E97" s="10"/>
-      <c r="F97" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="G97" s="11" t="s">
-        <v>207</v>
-      </c>
+      <c r="E97" s="15"/>
+      <c r="F97" s="14"/>
+      <c r="G97" s="5"/>
     </row>
     <row r="98" spans="2:7">
-      <c r="B98" s="40"/>
+      <c r="B98" s="63"/>
       <c r="C98" s="5"/>
-      <c r="D98" s="14" t="s">
+      <c r="D98" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="E98" s="10"/>
+      <c r="F98" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="E98" s="15"/>
-      <c r="F98" s="14"/>
-      <c r="G98" s="5"/>
+      <c r="G98" s="11" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="99" spans="2:7">
-      <c r="B99" s="40"/>
+      <c r="B99" s="63"/>
       <c r="C99" s="5"/>
-      <c r="D99" s="53" t="s">
-        <v>181</v>
-      </c>
-      <c r="E99" s="8"/>
-      <c r="F99" s="7"/>
+      <c r="D99" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="E99" s="15"/>
+      <c r="F99" s="14"/>
       <c r="G99" s="5"/>
     </row>
     <row r="100" spans="2:7">
-      <c r="B100" s="40"/>
+      <c r="B100" s="63"/>
       <c r="C100" s="5"/>
-      <c r="D100" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="E100" s="6"/>
-      <c r="F100" s="5"/>
-      <c r="G100" s="5"/>
+      <c r="D100" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="E100" s="8"/>
+      <c r="F100" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="G100" s="46" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="101" spans="2:7">
-      <c r="B101" s="29"/>
-      <c r="C101" s="5"/>
-      <c r="D101" s="5"/>
-      <c r="E101" s="6"/>
-      <c r="F101" s="5"/>
-      <c r="G101" s="5"/>
+      <c r="B101" s="63"/>
+      <c r="C101" s="36"/>
+      <c r="D101" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="E101" s="15"/>
+      <c r="F101" s="14"/>
+      <c r="G101" s="36"/>
     </row>
     <row r="102" spans="2:7">
-      <c r="B102" s="40" t="s">
-        <v>109</v>
-      </c>
+      <c r="B102" s="63"/>
       <c r="C102" s="5"/>
       <c r="D102" s="5" t="s">
-        <v>110</v>
+        <v>225</v>
       </c>
       <c r="E102" s="6"/>
       <c r="F102" s="5"/>
       <c r="G102" s="5"/>
     </row>
     <row r="103" spans="2:7">
-      <c r="B103" s="40"/>
+      <c r="B103" s="26"/>
       <c r="C103" s="5"/>
-      <c r="D103" s="5" t="s">
-        <v>111</v>
-      </c>
+      <c r="D103" s="5"/>
       <c r="E103" s="6"/>
       <c r="F103" s="5"/>
       <c r="G103" s="5"/>
     </row>
     <row r="104" spans="2:7">
-      <c r="B104" s="29"/>
+      <c r="B104" s="63" t="s">
+        <v>106</v>
+      </c>
       <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
+      <c r="D104" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="E104" s="6"/>
       <c r="F104" s="5"/>
       <c r="G104" s="5"/>
     </row>
     <row r="105" spans="2:7">
-      <c r="B105" s="40" t="s">
-        <v>141</v>
-      </c>
+      <c r="B105" s="63"/>
       <c r="C105" s="5"/>
       <c r="D105" s="5" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="E105" s="6"/>
       <c r="F105" s="5"/>
       <c r="G105" s="5"/>
     </row>
     <row r="106" spans="2:7">
-      <c r="B106" s="40"/>
+      <c r="B106" s="26"/>
       <c r="C106" s="5"/>
-      <c r="D106" s="5" t="s">
-        <v>103</v>
-      </c>
+      <c r="D106" s="5"/>
       <c r="E106" s="6"/>
       <c r="F106" s="5"/>
       <c r="G106" s="5"/>
     </row>
     <row r="107" spans="2:7">
-      <c r="B107" s="40"/>
+      <c r="B107" s="63" t="s">
+        <v>138</v>
+      </c>
       <c r="C107" s="5"/>
       <c r="D107" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E107" s="6"/>
       <c r="F107" s="5"/>
       <c r="G107" s="5"/>
     </row>
     <row r="108" spans="2:7">
-      <c r="B108" s="29"/>
+      <c r="B108" s="63"/>
       <c r="C108" s="5"/>
-      <c r="D108" s="5"/>
+      <c r="D108" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="E108" s="6"/>
       <c r="F108" s="5"/>
       <c r="G108" s="5"/>
     </row>
     <row r="109" spans="2:7">
-      <c r="B109" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="C109" s="37" t="s">
-        <v>237</v>
-      </c>
+      <c r="B109" s="63"/>
+      <c r="C109" s="5"/>
       <c r="D109" s="5" t="s">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="E109" s="6"/>
       <c r="F109" s="5"/>
       <c r="G109" s="5"/>
     </row>
     <row r="110" spans="2:7">
-      <c r="B110" s="49"/>
-      <c r="C110" s="37"/>
-      <c r="D110" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="B110" s="26"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
       <c r="E110" s="6"/>
       <c r="F110" s="5"/>
       <c r="G110" s="5"/>
     </row>
     <row r="111" spans="2:7">
-      <c r="B111" s="49"/>
-      <c r="C111" s="37"/>
+      <c r="B111" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="C111" s="55" t="s">
+        <v>234</v>
+      </c>
       <c r="D111" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E111" s="6"/>
       <c r="F111" s="5"/>
       <c r="G111" s="5"/>
     </row>
     <row r="112" spans="2:7">
-      <c r="B112" s="49"/>
-      <c r="C112" s="37"/>
+      <c r="B112" s="72"/>
+      <c r="C112" s="55"/>
       <c r="D112" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E112" s="6"/>
       <c r="F112" s="5"/>
       <c r="G112" s="5"/>
     </row>
     <row r="113" spans="2:7">
-      <c r="B113" s="49"/>
-      <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
+      <c r="B113" s="72"/>
+      <c r="C113" s="55"/>
+      <c r="D113" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="E113" s="6"/>
       <c r="F113" s="5"/>
       <c r="G113" s="5"/>
     </row>
     <row r="114" spans="2:7">
-      <c r="B114" s="49"/>
-      <c r="C114" s="37" t="s">
-        <v>238</v>
-      </c>
+      <c r="B114" s="72"/>
+      <c r="C114" s="55"/>
       <c r="D114" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E114" s="6"/>
       <c r="F114" s="5"/>
       <c r="G114" s="5"/>
     </row>
     <row r="115" spans="2:7">
-      <c r="B115" s="49"/>
-      <c r="C115" s="37"/>
-      <c r="D115" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="B115" s="72"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
       <c r="E115" s="6"/>
       <c r="F115" s="5"/>
       <c r="G115" s="5"/>
     </row>
     <row r="116" spans="2:7">
-      <c r="B116" s="49"/>
-      <c r="C116" s="37"/>
+      <c r="B116" s="72"/>
+      <c r="C116" s="55" t="s">
+        <v>235</v>
+      </c>
       <c r="D116" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E116" s="6"/>
       <c r="F116" s="5"/>
       <c r="G116" s="5"/>
     </row>
     <row r="117" spans="2:7">
-      <c r="B117" s="49"/>
-      <c r="C117" s="37"/>
+      <c r="B117" s="72"/>
+      <c r="C117" s="55"/>
       <c r="D117" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E117" s="6"/>
       <c r="F117" s="5"/>
       <c r="G117" s="5"/>
     </row>
     <row r="118" spans="2:7">
-      <c r="B118" s="49"/>
-      <c r="C118" s="37"/>
+      <c r="B118" s="72"/>
+      <c r="C118" s="55"/>
       <c r="D118" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E118" s="6"/>
       <c r="F118" s="5"/>
       <c r="G118" s="5"/>
     </row>
     <row r="119" spans="2:7">
-      <c r="B119" s="49"/>
-      <c r="C119" s="37"/>
+      <c r="B119" s="72"/>
+      <c r="C119" s="55"/>
       <c r="D119" s="5" t="s">
-        <v>180</v>
+        <v>47</v>
       </c>
       <c r="E119" s="6"/>
       <c r="F119" s="5"/>
       <c r="G119" s="5"/>
     </row>
     <row r="120" spans="2:7">
-      <c r="B120" s="49"/>
-      <c r="C120" s="37"/>
-      <c r="D120" s="53" t="s">
-        <v>185</v>
+      <c r="B120" s="72"/>
+      <c r="C120" s="55"/>
+      <c r="D120" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="E120" s="6"/>
       <c r="F120" s="5"/>
       <c r="G120" s="5"/>
     </row>
     <row r="121" spans="2:7">
-      <c r="B121" s="49"/>
-      <c r="C121" s="37"/>
+      <c r="B121" s="72"/>
+      <c r="C121" s="55"/>
       <c r="D121" s="5" t="s">
-        <v>49</v>
+        <v>177</v>
       </c>
       <c r="E121" s="6"/>
       <c r="F121" s="5"/>
       <c r="G121" s="5"/>
     </row>
     <row r="122" spans="2:7">
-      <c r="B122" s="49"/>
-      <c r="C122" s="37"/>
-      <c r="D122" s="5" t="s">
-        <v>50</v>
+      <c r="B122" s="72"/>
+      <c r="C122" s="55"/>
+      <c r="D122" s="32" t="s">
+        <v>182</v>
       </c>
       <c r="E122" s="6"/>
       <c r="F122" s="5"/>
       <c r="G122" s="5"/>
     </row>
     <row r="123" spans="2:7">
-      <c r="B123" s="49"/>
-      <c r="C123" s="5"/>
-      <c r="D123" s="5"/>
+      <c r="B123" s="72"/>
+      <c r="C123" s="55"/>
+      <c r="D123" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="E123" s="6"/>
       <c r="F123" s="5"/>
       <c r="G123" s="5"/>
     </row>
-    <row r="124" spans="2:7" ht="31.2">
-      <c r="B124" s="49"/>
-      <c r="C124" s="37" t="s">
-        <v>239</v>
-      </c>
-      <c r="E124" s="10" t="s">
+    <row r="124" spans="2:7">
+      <c r="B124" s="72"/>
+      <c r="C124" s="55"/>
+      <c r="D124" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E124" s="6"/>
+      <c r="F124" s="5"/>
+      <c r="G124" s="5"/>
+    </row>
+    <row r="125" spans="2:7">
+      <c r="B125" s="72"/>
+      <c r="C125" s="5"/>
+      <c r="D125" s="5"/>
+      <c r="E125" s="6"/>
+      <c r="F125" s="5"/>
+      <c r="G125" s="5"/>
+    </row>
+    <row r="126" spans="2:7" ht="31.2">
+      <c r="B126" s="72"/>
+      <c r="C126" s="55" t="s">
+        <v>236</v>
+      </c>
+      <c r="E126" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="F126" s="30" t="s">
         <v>274</v>
       </c>
-      <c r="F124" s="33" t="s">
-        <v>281</v>
-      </c>
-      <c r="G124" s="5"/>
-    </row>
-    <row r="125" spans="2:7">
-      <c r="B125" s="49"/>
-      <c r="C125" s="37"/>
-      <c r="E125" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="F125" s="33" t="s">
-        <v>280</v>
-      </c>
-      <c r="G125" s="5"/>
-    </row>
-    <row r="126" spans="2:7">
-      <c r="B126" s="49"/>
-      <c r="C126" s="37"/>
-      <c r="D126" s="5" t="s">
+      <c r="G126" s="5"/>
+    </row>
+    <row r="127" spans="2:7">
+      <c r="B127" s="72"/>
+      <c r="C127" s="55"/>
+      <c r="E127" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="F127" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="G127" s="5"/>
+    </row>
+    <row r="128" spans="2:7">
+      <c r="B128" s="72"/>
+      <c r="C128" s="55"/>
+      <c r="D128" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="E126" s="6"/>
-      <c r="F126" s="5"/>
-      <c r="G126" s="5"/>
-    </row>
-    <row r="127" spans="2:7">
-      <c r="B127" s="49"/>
-      <c r="C127" s="37"/>
-      <c r="D127" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E127" s="6"/>
-      <c r="F127" s="5"/>
-      <c r="G127" s="5"/>
-    </row>
-    <row r="128" spans="2:7">
-      <c r="B128" s="49"/>
-      <c r="C128" s="37"/>
-      <c r="D128" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="E128" s="6"/>
       <c r="F128" s="5"/>
       <c r="G128" s="5"/>
     </row>
     <row r="129" spans="2:7">
-      <c r="B129" s="49"/>
-      <c r="C129" s="37"/>
+      <c r="B129" s="72"/>
+      <c r="C129" s="55"/>
       <c r="D129" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E129" s="6"/>
       <c r="F129" s="5"/>
       <c r="G129" s="5"/>
     </row>
     <row r="130" spans="2:7">
-      <c r="B130" s="49"/>
-      <c r="C130" s="37"/>
-      <c r="D130" s="53" t="s">
-        <v>55</v>
+      <c r="B130" s="72"/>
+      <c r="C130" s="55"/>
+      <c r="D130" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="E130" s="6"/>
       <c r="F130" s="5"/>
       <c r="G130" s="5"/>
     </row>
     <row r="131" spans="2:7">
-      <c r="B131" s="49"/>
-      <c r="C131" s="37"/>
+      <c r="B131" s="72"/>
+      <c r="C131" s="55"/>
       <c r="D131" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E131" s="6"/>
       <c r="F131" s="5"/>
       <c r="G131" s="5"/>
     </row>
     <row r="132" spans="2:7">
-      <c r="B132" s="49"/>
-      <c r="C132" s="37"/>
-      <c r="D132" s="5" t="s">
-        <v>168</v>
+      <c r="B132" s="72"/>
+      <c r="C132" s="55"/>
+      <c r="D132" s="32" t="s">
+        <v>55</v>
       </c>
       <c r="E132" s="6"/>
       <c r="F132" s="5"/>
       <c r="G132" s="5"/>
     </row>
     <row r="133" spans="2:7">
-      <c r="B133" s="49"/>
-      <c r="C133" s="37"/>
+      <c r="B133" s="72"/>
+      <c r="C133" s="55"/>
       <c r="D133" s="5" t="s">
-        <v>169</v>
+        <v>56</v>
       </c>
       <c r="E133" s="6"/>
       <c r="F133" s="5"/>
       <c r="G133" s="5"/>
     </row>
     <row r="134" spans="2:7">
-      <c r="B134" s="49"/>
-      <c r="C134" s="37"/>
+      <c r="B134" s="72"/>
+      <c r="C134" s="55"/>
       <c r="D134" s="5" t="s">
-        <v>57</v>
+        <v>165</v>
       </c>
       <c r="E134" s="6"/>
       <c r="F134" s="5"/>
       <c r="G134" s="5"/>
     </row>
     <row r="135" spans="2:7">
-      <c r="B135" s="49"/>
-      <c r="C135" s="37"/>
+      <c r="B135" s="72"/>
+      <c r="C135" s="55"/>
       <c r="D135" s="5" t="s">
-        <v>58</v>
+        <v>166</v>
       </c>
       <c r="E135" s="6"/>
       <c r="F135" s="5"/>
       <c r="G135" s="5"/>
     </row>
     <row r="136" spans="2:7">
-      <c r="B136" s="49"/>
-      <c r="C136" s="37"/>
+      <c r="B136" s="72"/>
+      <c r="C136" s="55"/>
       <c r="D136" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E136" s="6"/>
       <c r="F136" s="5"/>
       <c r="G136" s="5"/>
     </row>
     <row r="137" spans="2:7">
-      <c r="B137" s="49"/>
-      <c r="C137" s="37"/>
-      <c r="D137" s="53" t="s">
-        <v>60</v>
+      <c r="B137" s="72"/>
+      <c r="C137" s="55"/>
+      <c r="D137" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="E137" s="6"/>
       <c r="F137" s="5"/>
       <c r="G137" s="5"/>
     </row>
     <row r="138" spans="2:7">
-      <c r="B138" s="49"/>
-      <c r="C138" s="5"/>
-      <c r="D138" s="5"/>
+      <c r="B138" s="72"/>
+      <c r="C138" s="55"/>
+      <c r="D138" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E138" s="6"/>
       <c r="F138" s="5"/>
       <c r="G138" s="5"/>
     </row>
     <row r="139" spans="2:7">
-      <c r="B139" s="49"/>
-      <c r="C139" s="37" t="s">
-        <v>240</v>
-      </c>
-      <c r="E139" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="F139" s="33" t="s">
-        <v>283</v>
-      </c>
+      <c r="B139" s="72"/>
+      <c r="C139" s="55"/>
+      <c r="D139" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E139" s="6"/>
+      <c r="F139" s="5"/>
       <c r="G139" s="5"/>
     </row>
     <row r="140" spans="2:7">
-      <c r="B140" s="49"/>
-      <c r="C140" s="37"/>
-      <c r="D140" s="5" t="s">
-        <v>170</v>
-      </c>
+      <c r="B140" s="72"/>
+      <c r="C140" s="5"/>
+      <c r="D140" s="5"/>
       <c r="E140" s="6"/>
       <c r="F140" s="5"/>
       <c r="G140" s="5"/>
     </row>
     <row r="141" spans="2:7">
-      <c r="B141" s="49"/>
-      <c r="C141" s="37"/>
-      <c r="D141" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="E141" s="6"/>
-      <c r="F141" s="5"/>
+      <c r="B141" s="72"/>
+      <c r="C141" s="55" t="s">
+        <v>237</v>
+      </c>
+      <c r="E141" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="F141" s="47" t="s">
+        <v>276</v>
+      </c>
       <c r="G141" s="5"/>
     </row>
     <row r="142" spans="2:7">
-      <c r="B142" s="49"/>
-      <c r="C142" s="37"/>
+      <c r="B142" s="72"/>
+      <c r="C142" s="55"/>
       <c r="D142" s="5" t="s">
-        <v>58</v>
+        <v>167</v>
       </c>
       <c r="E142" s="6"/>
       <c r="F142" s="5"/>
       <c r="G142" s="5"/>
     </row>
     <row r="143" spans="2:7">
-      <c r="B143" s="49"/>
-      <c r="C143" s="37"/>
+      <c r="B143" s="72"/>
+      <c r="C143" s="55"/>
       <c r="D143" s="5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E143" s="6"/>
       <c r="F143" s="5"/>
       <c r="G143" s="5"/>
     </row>
     <row r="144" spans="2:7">
-      <c r="B144" s="49"/>
-      <c r="C144" s="5"/>
-      <c r="D144" s="5"/>
+      <c r="B144" s="72"/>
+      <c r="C144" s="55"/>
+      <c r="D144" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="E144" s="6"/>
       <c r="F144" s="5"/>
       <c r="G144" s="5"/>
     </row>
     <row r="145" spans="2:7">
-      <c r="B145" s="49"/>
-      <c r="C145" s="37" t="s">
-        <v>241</v>
-      </c>
-      <c r="D145" s="54" t="s">
+      <c r="B145" s="72"/>
+      <c r="C145" s="55"/>
+      <c r="D145" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E145" s="6"/>
+      <c r="F145" s="5"/>
+      <c r="G145" s="5"/>
+    </row>
+    <row r="146" spans="2:7">
+      <c r="B146" s="72"/>
+      <c r="C146" s="5"/>
+      <c r="D146" s="5"/>
+      <c r="E146" s="6"/>
+      <c r="F146" s="5"/>
+      <c r="G146" s="5"/>
+    </row>
+    <row r="147" spans="2:7">
+      <c r="B147" s="72"/>
+      <c r="C147" s="55" t="s">
+        <v>238</v>
+      </c>
+      <c r="D147" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="E145" s="8"/>
-      <c r="F145" s="7"/>
-      <c r="G145" s="5"/>
-    </row>
-    <row r="146" spans="2:7">
-      <c r="B146" s="49"/>
-      <c r="C146" s="37"/>
-      <c r="D146" s="54" t="s">
+      <c r="E147" s="8"/>
+      <c r="F147" s="7"/>
+      <c r="G147" s="5"/>
+    </row>
+    <row r="148" spans="2:7">
+      <c r="B148" s="72"/>
+      <c r="C148" s="55"/>
+      <c r="D148" s="40" t="s">
         <v>62</v>
-      </c>
-      <c r="E146" s="8"/>
-      <c r="F146" s="7"/>
-      <c r="G146" s="5"/>
-    </row>
-    <row r="147" spans="2:7">
-      <c r="B147" s="49"/>
-      <c r="C147" s="5"/>
-      <c r="D147" s="5"/>
-      <c r="E147" s="6"/>
-      <c r="F147" s="5"/>
-      <c r="G147" s="5"/>
-    </row>
-    <row r="148" spans="2:7">
-      <c r="B148" s="49"/>
-      <c r="C148" s="37" t="s">
-        <v>242</v>
-      </c>
-      <c r="D148" s="54" t="s">
-        <v>63</v>
       </c>
       <c r="E148" s="8"/>
       <c r="F148" s="7"/>
       <c r="G148" s="5"/>
     </row>
     <row r="149" spans="2:7">
-      <c r="B149" s="49"/>
-      <c r="C149" s="37"/>
-      <c r="D149" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="B149" s="72"/>
+      <c r="C149" s="5"/>
+      <c r="D149" s="5"/>
       <c r="E149" s="6"/>
       <c r="F149" s="5"/>
       <c r="G149" s="5"/>
     </row>
     <row r="150" spans="2:7">
-      <c r="B150" s="49"/>
-      <c r="C150" s="5"/>
-      <c r="D150" s="5"/>
-      <c r="E150" s="6"/>
-      <c r="F150" s="5"/>
+      <c r="B150" s="72"/>
+      <c r="C150" s="55" t="s">
+        <v>239</v>
+      </c>
+      <c r="D150" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E150" s="8"/>
+      <c r="F150" s="7"/>
       <c r="G150" s="5"/>
     </row>
-    <row r="151" spans="2:7" ht="31.2">
-      <c r="B151" s="49"/>
-      <c r="C151" s="28" t="s">
-        <v>243</v>
-      </c>
-      <c r="D151" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E151" s="8"/>
-      <c r="F151" s="7"/>
+    <row r="151" spans="2:7">
+      <c r="B151" s="72"/>
+      <c r="C151" s="55"/>
+      <c r="D151" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E151" s="6"/>
+      <c r="F151" s="5"/>
       <c r="G151" s="5"/>
     </row>
     <row r="152" spans="2:7">
-      <c r="B152" s="49"/>
+      <c r="B152" s="72"/>
       <c r="C152" s="5"/>
       <c r="D152" s="5"/>
       <c r="E152" s="6"/>
       <c r="F152" s="5"/>
       <c r="G152" s="5"/>
     </row>
-    <row r="153" spans="2:7">
-      <c r="B153" s="49"/>
-      <c r="C153" s="28" t="s">
-        <v>244</v>
-      </c>
-      <c r="D153" s="5"/>
-      <c r="E153" s="6"/>
-      <c r="F153" s="5"/>
+    <row r="153" spans="2:7" ht="31.2">
+      <c r="B153" s="72"/>
+      <c r="C153" s="25" t="s">
+        <v>240</v>
+      </c>
+      <c r="D153" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E153" s="8"/>
+      <c r="F153" s="7"/>
       <c r="G153" s="5"/>
     </row>
     <row r="154" spans="2:7">
-      <c r="B154" s="49"/>
+      <c r="B154" s="72"/>
       <c r="C154" s="5"/>
       <c r="D154" s="5"/>
       <c r="E154" s="6"/>
@@ -3560,676 +3835,678 @@
       <c r="G154" s="5"/>
     </row>
     <row r="155" spans="2:7">
-      <c r="B155" s="49"/>
-      <c r="C155" s="37" t="s">
-        <v>245</v>
-      </c>
-      <c r="D155" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E155" s="15"/>
-      <c r="F155" s="14"/>
+      <c r="B155" s="72"/>
+      <c r="C155" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="D155" s="5"/>
+      <c r="E155" s="6"/>
+      <c r="F155" s="5"/>
       <c r="G155" s="5"/>
     </row>
     <row r="156" spans="2:7">
-      <c r="B156" s="49"/>
-      <c r="C156" s="37"/>
-      <c r="D156" s="5" t="s">
-        <v>67</v>
-      </c>
+      <c r="B156" s="72"/>
+      <c r="C156" s="5"/>
+      <c r="D156" s="5"/>
       <c r="E156" s="6"/>
       <c r="F156" s="5"/>
       <c r="G156" s="5"/>
     </row>
-    <row r="157" spans="2:7" ht="31.2">
-      <c r="B157" s="49"/>
-      <c r="C157" s="37"/>
-      <c r="D157" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E157" s="6"/>
-      <c r="F157" s="5"/>
+    <row r="157" spans="2:7">
+      <c r="B157" s="72"/>
+      <c r="C157" s="55" t="s">
+        <v>242</v>
+      </c>
+      <c r="D157" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E157" s="15"/>
+      <c r="F157" s="14"/>
       <c r="G157" s="5"/>
     </row>
-    <row r="158" spans="2:7" ht="31.2">
-      <c r="B158" s="49"/>
-      <c r="C158" s="37"/>
+    <row r="158" spans="2:7">
+      <c r="B158" s="72"/>
+      <c r="C158" s="55"/>
       <c r="D158" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E158" s="6"/>
       <c r="F158" s="5"/>
       <c r="G158" s="5"/>
     </row>
-    <row r="159" spans="2:7">
-      <c r="B159" s="49"/>
-      <c r="C159" s="37"/>
+    <row r="159" spans="2:7" ht="31.2">
+      <c r="B159" s="72"/>
+      <c r="C159" s="55"/>
       <c r="D159" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E159" s="6"/>
       <c r="F159" s="5"/>
       <c r="G159" s="5"/>
     </row>
-    <row r="160" spans="2:7">
-      <c r="B160" s="49"/>
-      <c r="C160" s="37"/>
+    <row r="160" spans="2:7" ht="31.2">
+      <c r="B160" s="72"/>
+      <c r="C160" s="55"/>
       <c r="D160" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E160" s="6"/>
       <c r="F160" s="5"/>
       <c r="G160" s="5"/>
     </row>
     <row r="161" spans="2:7">
-      <c r="B161" s="49"/>
-      <c r="C161" s="37"/>
+      <c r="B161" s="72"/>
+      <c r="C161" s="55"/>
       <c r="D161" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E161" s="6"/>
       <c r="F161" s="5"/>
       <c r="G161" s="5"/>
     </row>
     <row r="162" spans="2:7">
-      <c r="B162" s="49"/>
-      <c r="C162" s="5"/>
-      <c r="D162" s="5"/>
+      <c r="B162" s="72"/>
+      <c r="C162" s="55"/>
+      <c r="D162" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="E162" s="6"/>
       <c r="F162" s="5"/>
       <c r="G162" s="5"/>
     </row>
     <row r="163" spans="2:7">
-      <c r="B163" s="49"/>
-      <c r="C163" s="37" t="s">
-        <v>246</v>
-      </c>
+      <c r="B163" s="72"/>
+      <c r="C163" s="55"/>
       <c r="D163" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E163" s="6"/>
       <c r="F163" s="5"/>
       <c r="G163" s="5"/>
     </row>
     <row r="164" spans="2:7">
-      <c r="B164" s="49"/>
-      <c r="C164" s="37"/>
-      <c r="D164" s="5" t="s">
-        <v>272</v>
-      </c>
+      <c r="B164" s="72"/>
+      <c r="C164" s="5"/>
+      <c r="D164" s="5"/>
       <c r="E164" s="6"/>
       <c r="F164" s="5"/>
       <c r="G164" s="5"/>
     </row>
     <row r="165" spans="2:7">
-      <c r="B165" s="49"/>
-      <c r="C165" s="37"/>
+      <c r="B165" s="72"/>
+      <c r="C165" s="55" t="s">
+        <v>243</v>
+      </c>
       <c r="D165" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E165" s="6"/>
       <c r="F165" s="5"/>
       <c r="G165" s="5"/>
     </row>
     <row r="166" spans="2:7">
-      <c r="B166" s="49"/>
-      <c r="C166" s="37"/>
+      <c r="B166" s="72"/>
+      <c r="C166" s="55"/>
       <c r="D166" s="5" t="s">
-        <v>75</v>
+        <v>267</v>
       </c>
       <c r="E166" s="6"/>
       <c r="F166" s="5"/>
       <c r="G166" s="5"/>
     </row>
     <row r="167" spans="2:7">
-      <c r="B167" s="49"/>
-      <c r="C167" s="37"/>
+      <c r="B167" s="72"/>
+      <c r="C167" s="55"/>
       <c r="D167" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E167" s="6"/>
       <c r="F167" s="5"/>
       <c r="G167" s="5"/>
     </row>
     <row r="168" spans="2:7">
-      <c r="B168" s="49"/>
-      <c r="C168" s="37"/>
+      <c r="B168" s="72"/>
+      <c r="C168" s="55"/>
       <c r="D168" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E168" s="6"/>
       <c r="F168" s="5"/>
       <c r="G168" s="5"/>
     </row>
     <row r="169" spans="2:7">
-      <c r="B169" s="49"/>
-      <c r="C169" s="37"/>
+      <c r="B169" s="72"/>
+      <c r="C169" s="55"/>
       <c r="D169" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E169" s="6"/>
       <c r="F169" s="5"/>
       <c r="G169" s="5"/>
     </row>
     <row r="170" spans="2:7">
-      <c r="B170" s="49"/>
-      <c r="C170" s="37"/>
+      <c r="B170" s="72"/>
+      <c r="C170" s="55"/>
       <c r="D170" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E170" s="6"/>
       <c r="F170" s="5"/>
       <c r="G170" s="5"/>
     </row>
     <row r="171" spans="2:7">
-      <c r="B171" s="49"/>
-      <c r="C171" s="37"/>
-      <c r="D171" s="5"/>
+      <c r="B171" s="72"/>
+      <c r="C171" s="55"/>
+      <c r="D171" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="E171" s="6"/>
       <c r="F171" s="5"/>
       <c r="G171" s="5"/>
     </row>
     <row r="172" spans="2:7">
-      <c r="B172" s="49"/>
-      <c r="C172" s="37"/>
+      <c r="B172" s="72"/>
+      <c r="C172" s="55"/>
       <c r="D172" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E172" s="6"/>
       <c r="F172" s="5"/>
       <c r="G172" s="5"/>
     </row>
     <row r="173" spans="2:7">
-      <c r="B173" s="49"/>
-      <c r="C173" s="37"/>
-      <c r="D173" s="24" t="s">
-        <v>81</v>
-      </c>
+      <c r="B173" s="72"/>
+      <c r="C173" s="55"/>
+      <c r="D173" s="5"/>
       <c r="E173" s="6"/>
       <c r="F173" s="5"/>
       <c r="G173" s="5"/>
     </row>
     <row r="174" spans="2:7">
-      <c r="B174" s="49"/>
-      <c r="C174" s="37"/>
+      <c r="B174" s="72"/>
+      <c r="C174" s="55"/>
       <c r="D174" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E174" s="6"/>
       <c r="F174" s="5"/>
       <c r="G174" s="5"/>
     </row>
     <row r="175" spans="2:7">
-      <c r="B175" s="49"/>
-      <c r="C175" s="37"/>
-      <c r="D175" s="5" t="s">
-        <v>83</v>
+      <c r="B175" s="72"/>
+      <c r="C175" s="55"/>
+      <c r="D175" s="24" t="s">
+        <v>81</v>
       </c>
       <c r="E175" s="6"/>
       <c r="F175" s="5"/>
       <c r="G175" s="5"/>
     </row>
     <row r="176" spans="2:7">
-      <c r="B176" s="49"/>
-      <c r="C176" s="37"/>
-      <c r="D176" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E176" s="8"/>
-      <c r="F176" s="7"/>
+      <c r="B176" s="72"/>
+      <c r="C176" s="55"/>
+      <c r="D176" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E176" s="6"/>
+      <c r="F176" s="5"/>
       <c r="G176" s="5"/>
     </row>
     <row r="177" spans="2:7">
-      <c r="B177" s="29"/>
-      <c r="C177" s="5"/>
-      <c r="D177" s="5"/>
+      <c r="B177" s="72"/>
+      <c r="C177" s="55"/>
+      <c r="D177" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="E177" s="6"/>
       <c r="F177" s="5"/>
       <c r="G177" s="5"/>
     </row>
     <row r="178" spans="2:7">
-      <c r="B178" s="40" t="s">
-        <v>174</v>
-      </c>
-      <c r="C178" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="D178" s="16"/>
-      <c r="E178" s="17"/>
-      <c r="F178" s="30" t="s">
-        <v>252</v>
-      </c>
+      <c r="B178" s="72"/>
+      <c r="C178" s="55"/>
+      <c r="D178" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E178" s="8"/>
+      <c r="F178" s="7"/>
+      <c r="G178" s="5"/>
     </row>
     <row r="179" spans="2:7">
-      <c r="B179" s="40"/>
-      <c r="C179" s="37"/>
-      <c r="D179" s="5" t="s">
-        <v>113</v>
-      </c>
+      <c r="B179" s="26"/>
+      <c r="C179" s="5"/>
+      <c r="D179" s="5"/>
       <c r="E179" s="6"/>
       <c r="F179" s="5"/>
       <c r="G179" s="5"/>
     </row>
     <row r="180" spans="2:7">
-      <c r="B180" s="40"/>
-      <c r="C180" s="37"/>
-      <c r="D180" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E180" s="6"/>
-      <c r="F180" s="5"/>
-      <c r="G180" s="5"/>
+      <c r="B180" s="63" t="s">
+        <v>171</v>
+      </c>
+      <c r="C180" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="D180" s="16"/>
+      <c r="E180" s="17"/>
+      <c r="F180" s="27" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="181" spans="2:7">
-      <c r="B181" s="40"/>
-      <c r="C181" s="37"/>
+      <c r="B181" s="63"/>
+      <c r="C181" s="55"/>
       <c r="D181" s="5" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E181" s="6"/>
       <c r="F181" s="5"/>
       <c r="G181" s="5"/>
     </row>
     <row r="182" spans="2:7">
-      <c r="B182" s="40"/>
-      <c r="C182" s="37"/>
+      <c r="B182" s="63"/>
+      <c r="C182" s="55"/>
       <c r="D182" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E182" s="6"/>
       <c r="F182" s="5"/>
       <c r="G182" s="5"/>
     </row>
     <row r="183" spans="2:7">
-      <c r="B183" s="40"/>
-      <c r="C183" s="37"/>
+      <c r="B183" s="63"/>
+      <c r="C183" s="55"/>
       <c r="D183" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E183" s="6"/>
       <c r="F183" s="5"/>
       <c r="G183" s="5"/>
     </row>
     <row r="184" spans="2:7">
-      <c r="B184" s="40"/>
-      <c r="C184" s="37"/>
+      <c r="B184" s="63"/>
+      <c r="C184" s="55"/>
       <c r="D184" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E184" s="6"/>
       <c r="F184" s="5"/>
       <c r="G184" s="5"/>
     </row>
     <row r="185" spans="2:7">
-      <c r="B185" s="40"/>
-      <c r="C185" s="37"/>
+      <c r="B185" s="63"/>
+      <c r="C185" s="55"/>
       <c r="D185" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E185" s="6"/>
       <c r="F185" s="5"/>
       <c r="G185" s="5"/>
     </row>
     <row r="186" spans="2:7">
-      <c r="B186" s="40"/>
-      <c r="C186" s="37"/>
+      <c r="B186" s="63"/>
+      <c r="C186" s="55"/>
       <c r="D186" s="5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E186" s="6"/>
       <c r="F186" s="5"/>
       <c r="G186" s="5"/>
     </row>
     <row r="187" spans="2:7">
-      <c r="B187" s="40"/>
-      <c r="C187" s="37"/>
+      <c r="B187" s="63"/>
+      <c r="C187" s="55"/>
       <c r="D187" s="5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E187" s="6"/>
       <c r="F187" s="5"/>
       <c r="G187" s="5"/>
     </row>
     <row r="188" spans="2:7">
-      <c r="B188" s="40"/>
-      <c r="C188" s="37"/>
+      <c r="B188" s="63"/>
+      <c r="C188" s="55"/>
       <c r="D188" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E188" s="6"/>
       <c r="F188" s="5"/>
       <c r="G188" s="5"/>
     </row>
-    <row r="189" spans="2:7" ht="31.2">
-      <c r="B189" s="40"/>
-      <c r="C189" s="37"/>
+    <row r="189" spans="2:7">
+      <c r="B189" s="63"/>
+      <c r="C189" s="55"/>
       <c r="D189" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E189" s="6"/>
       <c r="F189" s="5"/>
       <c r="G189" s="5"/>
     </row>
     <row r="190" spans="2:7">
-      <c r="B190" s="40"/>
-      <c r="C190" s="37"/>
+      <c r="B190" s="63"/>
+      <c r="C190" s="55"/>
       <c r="D190" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E190" s="6"/>
       <c r="F190" s="5"/>
       <c r="G190" s="5"/>
     </row>
-    <row r="191" spans="2:7">
-      <c r="B191" s="40"/>
-      <c r="C191" s="37"/>
+    <row r="191" spans="2:7" ht="31.2">
+      <c r="B191" s="63"/>
+      <c r="C191" s="55"/>
       <c r="D191" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E191" s="6"/>
       <c r="F191" s="5"/>
       <c r="G191" s="5"/>
     </row>
     <row r="192" spans="2:7">
-      <c r="B192" s="40"/>
-      <c r="C192" s="37"/>
+      <c r="B192" s="63"/>
+      <c r="C192" s="55"/>
       <c r="D192" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E192" s="6"/>
       <c r="F192" s="5"/>
       <c r="G192" s="5"/>
     </row>
     <row r="193" spans="2:7">
-      <c r="B193" s="40"/>
-      <c r="C193" s="37"/>
+      <c r="B193" s="63"/>
+      <c r="C193" s="55"/>
       <c r="D193" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E193" s="6"/>
       <c r="F193" s="5"/>
       <c r="G193" s="5"/>
     </row>
     <row r="194" spans="2:7">
-      <c r="B194" s="40"/>
-      <c r="C194" s="37"/>
+      <c r="B194" s="63"/>
+      <c r="C194" s="55"/>
       <c r="D194" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E194" s="6"/>
       <c r="F194" s="5"/>
       <c r="G194" s="5"/>
     </row>
     <row r="195" spans="2:7">
-      <c r="B195" s="40"/>
-      <c r="C195" s="37"/>
+      <c r="B195" s="63"/>
+      <c r="C195" s="55"/>
       <c r="D195" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E195" s="6"/>
       <c r="F195" s="5"/>
       <c r="G195" s="5"/>
     </row>
     <row r="196" spans="2:7">
-      <c r="B196" s="40"/>
-      <c r="C196" s="37"/>
+      <c r="B196" s="63"/>
+      <c r="C196" s="55"/>
       <c r="D196" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E196" s="6"/>
       <c r="F196" s="5"/>
       <c r="G196" s="5"/>
     </row>
     <row r="197" spans="2:7">
-      <c r="B197" s="40"/>
-      <c r="C197" s="37"/>
+      <c r="B197" s="63"/>
+      <c r="C197" s="55"/>
       <c r="D197" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E197" s="6"/>
       <c r="F197" s="5"/>
       <c r="G197" s="5"/>
     </row>
     <row r="198" spans="2:7">
-      <c r="B198" s="40"/>
-      <c r="C198" s="37"/>
+      <c r="B198" s="63"/>
+      <c r="C198" s="55"/>
       <c r="D198" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E198" s="6"/>
       <c r="F198" s="5"/>
       <c r="G198" s="5"/>
     </row>
     <row r="199" spans="2:7">
-      <c r="B199" s="40"/>
-      <c r="C199" s="5"/>
-      <c r="D199" s="5"/>
+      <c r="B199" s="63"/>
+      <c r="C199" s="55"/>
+      <c r="D199" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="E199" s="6"/>
       <c r="F199" s="5"/>
       <c r="G199" s="5"/>
     </row>
     <row r="200" spans="2:7">
-      <c r="B200" s="40"/>
-      <c r="C200" s="37" t="s">
-        <v>133</v>
-      </c>
+      <c r="B200" s="63"/>
+      <c r="C200" s="55"/>
       <c r="D200" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E200" s="6"/>
       <c r="F200" s="5"/>
       <c r="G200" s="5"/>
     </row>
     <row r="201" spans="2:7">
-      <c r="B201" s="40"/>
-      <c r="C201" s="37"/>
-      <c r="D201" s="5" t="s">
-        <v>135</v>
-      </c>
+      <c r="B201" s="63"/>
+      <c r="C201" s="5"/>
+      <c r="D201" s="5"/>
       <c r="E201" s="6"/>
       <c r="F201" s="5"/>
       <c r="G201" s="5"/>
     </row>
     <row r="202" spans="2:7">
-      <c r="B202" s="40"/>
-      <c r="C202" s="37"/>
+      <c r="B202" s="63"/>
+      <c r="C202" s="55" t="s">
+        <v>130</v>
+      </c>
       <c r="D202" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E202" s="6"/>
       <c r="F202" s="5"/>
       <c r="G202" s="5"/>
     </row>
     <row r="203" spans="2:7">
-      <c r="B203" s="40"/>
-      <c r="C203" s="37"/>
+      <c r="B203" s="63"/>
+      <c r="C203" s="55"/>
       <c r="D203" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E203" s="6"/>
       <c r="F203" s="5"/>
       <c r="G203" s="5"/>
     </row>
     <row r="204" spans="2:7">
-      <c r="B204" s="40"/>
-      <c r="C204" s="37"/>
+      <c r="B204" s="63"/>
+      <c r="C204" s="55"/>
       <c r="D204" s="5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E204" s="6"/>
       <c r="F204" s="5"/>
       <c r="G204" s="5"/>
     </row>
     <row r="205" spans="2:7">
-      <c r="B205" s="40"/>
-      <c r="C205" s="37"/>
+      <c r="B205" s="63"/>
+      <c r="C205" s="55"/>
       <c r="D205" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E205" s="6"/>
       <c r="F205" s="5"/>
       <c r="G205" s="5"/>
     </row>
     <row r="206" spans="2:7">
-      <c r="B206" s="40"/>
-      <c r="C206" s="37"/>
+      <c r="B206" s="63"/>
+      <c r="C206" s="55"/>
       <c r="D206" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E206" s="6"/>
       <c r="F206" s="5"/>
       <c r="G206" s="5"/>
     </row>
     <row r="207" spans="2:7">
-      <c r="B207" s="29"/>
-      <c r="C207" s="5"/>
-      <c r="D207" s="5"/>
+      <c r="B207" s="63"/>
+      <c r="C207" s="55"/>
+      <c r="D207" s="5" t="s">
+        <v>136</v>
+      </c>
       <c r="E207" s="6"/>
       <c r="F207" s="5"/>
       <c r="G207" s="5"/>
     </row>
-    <row r="208" spans="2:7" ht="31.2">
-      <c r="B208" s="41" t="s">
-        <v>144</v>
-      </c>
-      <c r="C208" s="5"/>
-      <c r="D208" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="E208" s="10"/>
-      <c r="F208" s="9"/>
-      <c r="G208" s="11" t="s">
-        <v>251</v>
-      </c>
+    <row r="208" spans="2:7">
+      <c r="B208" s="63"/>
+      <c r="C208" s="55"/>
+      <c r="D208" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E208" s="6"/>
+      <c r="F208" s="5"/>
+      <c r="G208" s="5"/>
     </row>
     <row r="209" spans="2:7">
-      <c r="B209" s="41"/>
+      <c r="B209" s="26"/>
       <c r="C209" s="5"/>
-      <c r="D209" s="5" t="s">
-        <v>146</v>
-      </c>
+      <c r="D209" s="5"/>
       <c r="E209" s="6"/>
       <c r="F209" s="5"/>
       <c r="G209" s="5"/>
     </row>
-    <row r="210" spans="2:7">
-      <c r="B210" s="41"/>
+    <row r="210" spans="2:7" ht="31.2">
+      <c r="B210" s="64" t="s">
+        <v>141</v>
+      </c>
       <c r="C210" s="5"/>
-      <c r="D210" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E210" s="6"/>
-      <c r="F210" s="5"/>
-      <c r="G210" s="5"/>
+      <c r="D210" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="E210" s="10"/>
+      <c r="F210" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="G210" s="11" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="211" spans="2:7">
-      <c r="B211" s="41"/>
+      <c r="B211" s="64"/>
       <c r="C211" s="5"/>
       <c r="D211" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E211" s="6"/>
       <c r="F211" s="5"/>
       <c r="G211" s="5"/>
     </row>
     <row r="212" spans="2:7">
-      <c r="B212" s="41"/>
+      <c r="B212" s="64"/>
       <c r="C212" s="5"/>
       <c r="D212" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E212" s="6"/>
       <c r="F212" s="5"/>
       <c r="G212" s="5"/>
     </row>
     <row r="213" spans="2:7">
-      <c r="B213" s="41"/>
+      <c r="B213" s="64"/>
       <c r="C213" s="5"/>
       <c r="D213" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E213" s="6"/>
       <c r="F213" s="5"/>
       <c r="G213" s="5"/>
     </row>
     <row r="214" spans="2:7">
-      <c r="B214" s="41"/>
+      <c r="B214" s="64"/>
       <c r="C214" s="5"/>
-      <c r="D214" s="53" t="s">
-        <v>222</v>
+      <c r="D214" s="5" t="s">
+        <v>146</v>
       </c>
       <c r="E214" s="6"/>
       <c r="F214" s="5"/>
       <c r="G214" s="5"/>
     </row>
     <row r="215" spans="2:7">
-      <c r="B215" s="41"/>
+      <c r="B215" s="64"/>
       <c r="C215" s="5"/>
       <c r="D215" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E215" s="6"/>
       <c r="F215" s="5"/>
       <c r="G215" s="5"/>
     </row>
     <row r="216" spans="2:7">
-      <c r="B216" s="29"/>
+      <c r="B216" s="64"/>
       <c r="C216" s="5"/>
-      <c r="D216" s="5"/>
+      <c r="D216" s="32" t="s">
+        <v>219</v>
+      </c>
       <c r="E216" s="6"/>
       <c r="F216" s="5"/>
       <c r="G216" s="5"/>
     </row>
     <row r="217" spans="2:7">
-      <c r="B217" s="38" t="s">
-        <v>190</v>
-      </c>
+      <c r="B217" s="64"/>
       <c r="C217" s="5"/>
-      <c r="D217" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E217" s="15"/>
-      <c r="F217" s="14"/>
+      <c r="D217" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E217" s="6"/>
+      <c r="F217" s="5"/>
       <c r="G217" s="5"/>
     </row>
     <row r="218" spans="2:7">
-      <c r="B218" s="50"/>
+      <c r="B218" s="26"/>
       <c r="C218" s="5"/>
-      <c r="D218" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="E218" s="15"/>
-      <c r="F218" s="14"/>
+      <c r="D218" s="5"/>
+      <c r="E218" s="6"/>
+      <c r="F218" s="5"/>
       <c r="G218" s="5"/>
     </row>
     <row r="219" spans="2:7">
-      <c r="B219" s="50"/>
+      <c r="B219" s="61" t="s">
+        <v>187</v>
+      </c>
       <c r="C219" s="5"/>
       <c r="D219" s="14" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E219" s="15"/>
       <c r="F219" s="14"/>
       <c r="G219" s="5"/>
     </row>
     <row r="220" spans="2:7">
-      <c r="B220" s="50"/>
+      <c r="B220" s="73"/>
       <c r="C220" s="5"/>
-      <c r="D220" s="5"/>
-      <c r="E220" s="6"/>
-      <c r="F220" s="5"/>
+      <c r="D220" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="E220" s="15"/>
+      <c r="F220" s="14"/>
       <c r="G220" s="5"/>
     </row>
     <row r="221" spans="2:7">
-      <c r="B221" s="50"/>
+      <c r="B221" s="73"/>
       <c r="C221" s="5"/>
-      <c r="D221" s="5"/>
+      <c r="D221" s="36"/>
       <c r="E221" s="6"/>
-      <c r="F221" s="5"/>
+      <c r="F221" s="36"/>
       <c r="G221" s="5"/>
     </row>
     <row r="222" spans="2:7">
-      <c r="B222" s="50"/>
+      <c r="B222" s="73"/>
       <c r="C222" s="5"/>
       <c r="D222" s="5"/>
       <c r="E222" s="6"/>
@@ -4237,7 +4514,7 @@
       <c r="G222" s="5"/>
     </row>
     <row r="223" spans="2:7">
-      <c r="B223" s="50"/>
+      <c r="B223" s="73"/>
       <c r="C223" s="5"/>
       <c r="D223" s="5"/>
       <c r="E223" s="6"/>
@@ -4245,7 +4522,7 @@
       <c r="G223" s="5"/>
     </row>
     <row r="224" spans="2:7">
-      <c r="B224" s="50"/>
+      <c r="B224" s="73"/>
       <c r="C224" s="5"/>
       <c r="D224" s="5"/>
       <c r="E224" s="6"/>
@@ -4253,7 +4530,7 @@
       <c r="G224" s="5"/>
     </row>
     <row r="225" spans="2:7">
-      <c r="B225" s="50"/>
+      <c r="B225" s="73"/>
       <c r="C225" s="5"/>
       <c r="D225" s="5"/>
       <c r="E225" s="6"/>
@@ -4261,7 +4538,7 @@
       <c r="G225" s="5"/>
     </row>
     <row r="226" spans="2:7">
-      <c r="B226" s="50"/>
+      <c r="B226" s="73"/>
       <c r="C226" s="5"/>
       <c r="D226" s="5"/>
       <c r="E226" s="6"/>
@@ -4269,7 +4546,7 @@
       <c r="G226" s="5"/>
     </row>
     <row r="227" spans="2:7">
-      <c r="B227" s="50"/>
+      <c r="B227" s="73"/>
       <c r="C227" s="5"/>
       <c r="D227" s="5"/>
       <c r="E227" s="6"/>
@@ -4277,7 +4554,7 @@
       <c r="G227" s="5"/>
     </row>
     <row r="228" spans="2:7">
-      <c r="B228" s="50"/>
+      <c r="B228" s="73"/>
       <c r="C228" s="5"/>
       <c r="D228" s="5"/>
       <c r="E228" s="6"/>
@@ -4285,7 +4562,7 @@
       <c r="G228" s="5"/>
     </row>
     <row r="229" spans="2:7">
-      <c r="B229" s="50"/>
+      <c r="B229" s="73"/>
       <c r="C229" s="5"/>
       <c r="D229" s="5"/>
       <c r="E229" s="6"/>
@@ -4293,7 +4570,7 @@
       <c r="G229" s="5"/>
     </row>
     <row r="230" spans="2:7">
-      <c r="B230" s="50"/>
+      <c r="B230" s="73"/>
       <c r="C230" s="5"/>
       <c r="D230" s="5"/>
       <c r="E230" s="6"/>
@@ -4301,7 +4578,7 @@
       <c r="G230" s="5"/>
     </row>
     <row r="231" spans="2:7">
-      <c r="B231" s="39"/>
+      <c r="B231" s="73"/>
       <c r="C231" s="5"/>
       <c r="D231" s="5"/>
       <c r="E231" s="6"/>
@@ -4309,7 +4586,7 @@
       <c r="G231" s="5"/>
     </row>
     <row r="232" spans="2:7">
-      <c r="B232" s="29"/>
+      <c r="B232" s="73"/>
       <c r="C232" s="5"/>
       <c r="D232" s="5"/>
       <c r="E232" s="6"/>
@@ -4317,21 +4594,15 @@
       <c r="G232" s="5"/>
     </row>
     <row r="233" spans="2:7">
-      <c r="B233" s="42" t="s">
-        <v>268</v>
-      </c>
-      <c r="C233" s="24" t="s">
-        <v>269</v>
-      </c>
+      <c r="B233" s="62"/>
+      <c r="C233" s="5"/>
       <c r="D233" s="5"/>
       <c r="E233" s="6"/>
-      <c r="F233" s="5" t="s">
-        <v>270</v>
-      </c>
+      <c r="F233" s="5"/>
       <c r="G233" s="5"/>
     </row>
     <row r="234" spans="2:7">
-      <c r="B234" s="43"/>
+      <c r="B234" s="26"/>
       <c r="C234" s="5"/>
       <c r="D234" s="5"/>
       <c r="E234" s="6"/>
@@ -4339,15 +4610,21 @@
       <c r="G234" s="5"/>
     </row>
     <row r="235" spans="2:7">
-      <c r="B235" s="44"/>
-      <c r="C235" s="5"/>
+      <c r="B235" s="65" t="s">
+        <v>263</v>
+      </c>
+      <c r="C235" s="24" t="s">
+        <v>264</v>
+      </c>
       <c r="D235" s="5"/>
       <c r="E235" s="6"/>
-      <c r="F235" s="5"/>
+      <c r="F235" s="5" t="s">
+        <v>265</v>
+      </c>
       <c r="G235" s="5"/>
     </row>
     <row r="236" spans="2:7">
-      <c r="B236" s="44"/>
+      <c r="B236" s="66"/>
       <c r="C236" s="5"/>
       <c r="D236" s="5"/>
       <c r="E236" s="6"/>
@@ -4355,7 +4632,7 @@
       <c r="G236" s="5"/>
     </row>
     <row r="237" spans="2:7">
-      <c r="B237" s="45"/>
+      <c r="B237" s="67"/>
       <c r="C237" s="5"/>
       <c r="D237" s="5"/>
       <c r="E237" s="6"/>
@@ -4363,259 +4640,278 @@
       <c r="G237" s="5"/>
     </row>
     <row r="238" spans="2:7">
-      <c r="B238" s="23"/>
+      <c r="B238" s="67"/>
       <c r="C238" s="5"/>
       <c r="D238" s="5"/>
       <c r="E238" s="6"/>
       <c r="F238" s="5"/>
       <c r="G238" s="5"/>
     </row>
-    <row r="239" spans="2:7" ht="46.8">
-      <c r="B239" s="38" t="s">
-        <v>196</v>
-      </c>
+    <row r="239" spans="2:7">
+      <c r="B239" s="68"/>
       <c r="C239" s="5"/>
-      <c r="D239" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="E239" s="18"/>
-      <c r="F239" s="11"/>
+      <c r="D239" s="5"/>
+      <c r="E239" s="6"/>
+      <c r="F239" s="5"/>
       <c r="G239" s="5"/>
     </row>
-    <row r="240" spans="2:7" ht="31.2">
-      <c r="B240" s="39"/>
+    <row r="240" spans="2:7">
+      <c r="B240" s="23"/>
       <c r="C240" s="5"/>
-      <c r="D240" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="E240" s="18"/>
-      <c r="F240" s="11"/>
+      <c r="D240" s="5"/>
+      <c r="E240" s="6"/>
+      <c r="F240" s="5"/>
       <c r="G240" s="5"/>
     </row>
-    <row r="241" spans="2:7">
-      <c r="B241" s="29"/>
+    <row r="241" spans="2:7" ht="46.8">
+      <c r="B241" s="61" t="s">
+        <v>193</v>
+      </c>
       <c r="C241" s="5"/>
-      <c r="D241" s="5"/>
-      <c r="E241" s="6"/>
-      <c r="F241" s="5"/>
+      <c r="D241" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E241" s="18"/>
+      <c r="F241" s="11"/>
       <c r="G241" s="5"/>
     </row>
-    <row r="242" spans="2:7">
-      <c r="B242" s="41" t="s">
-        <v>152</v>
-      </c>
+    <row r="242" spans="2:7" ht="31.2">
+      <c r="B242" s="62"/>
       <c r="C242" s="5"/>
-      <c r="D242" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="E242" s="6"/>
-      <c r="F242" s="5"/>
+      <c r="D242" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="E242" s="18"/>
+      <c r="F242" s="11"/>
       <c r="G242" s="5"/>
     </row>
     <row r="243" spans="2:7">
-      <c r="B243" s="41"/>
+      <c r="B243" s="26"/>
       <c r="C243" s="5"/>
-      <c r="D243" s="5" t="s">
-        <v>154</v>
-      </c>
+      <c r="D243" s="5"/>
       <c r="E243" s="6"/>
       <c r="F243" s="5"/>
       <c r="G243" s="5"/>
     </row>
     <row r="244" spans="2:7">
-      <c r="B244" s="41"/>
+      <c r="B244" s="64" t="s">
+        <v>149</v>
+      </c>
       <c r="C244" s="5"/>
       <c r="D244" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E244" s="6"/>
       <c r="F244" s="5"/>
       <c r="G244" s="5"/>
     </row>
     <row r="245" spans="2:7">
-      <c r="B245" s="41"/>
+      <c r="B245" s="64"/>
       <c r="C245" s="5"/>
       <c r="D245" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E245" s="6"/>
       <c r="F245" s="5"/>
       <c r="G245" s="5"/>
     </row>
     <row r="246" spans="2:7">
-      <c r="B246" s="41"/>
+      <c r="B246" s="64"/>
       <c r="C246" s="5"/>
       <c r="D246" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E246" s="6"/>
       <c r="F246" s="5"/>
       <c r="G246" s="5"/>
     </row>
-    <row r="247" spans="2:7" ht="46.8">
-      <c r="B247" s="41"/>
+    <row r="247" spans="2:7">
+      <c r="B247" s="64"/>
       <c r="C247" s="5"/>
       <c r="D247" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E247" s="6"/>
       <c r="F247" s="5"/>
       <c r="G247" s="5"/>
     </row>
-    <row r="248" spans="2:7" ht="31.2">
-      <c r="B248" s="41"/>
+    <row r="248" spans="2:7">
+      <c r="B248" s="64"/>
       <c r="C248" s="5"/>
       <c r="D248" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E248" s="6"/>
       <c r="F248" s="5"/>
       <c r="G248" s="5"/>
     </row>
-    <row r="249" spans="2:7">
-      <c r="B249" s="41"/>
+    <row r="249" spans="2:7" ht="46.8">
+      <c r="B249" s="64"/>
       <c r="C249" s="5"/>
       <c r="D249" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E249" s="6"/>
       <c r="F249" s="5"/>
       <c r="G249" s="5"/>
     </row>
-    <row r="250" spans="2:7">
-      <c r="B250" s="41"/>
+    <row r="250" spans="2:7" ht="31.2">
+      <c r="B250" s="64"/>
       <c r="C250" s="5"/>
       <c r="D250" s="5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E250" s="6"/>
       <c r="F250" s="5"/>
       <c r="G250" s="5"/>
     </row>
     <row r="251" spans="2:7">
-      <c r="B251" s="41"/>
+      <c r="B251" s="64"/>
       <c r="C251" s="5"/>
       <c r="D251" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E251" s="6"/>
       <c r="F251" s="5"/>
       <c r="G251" s="5"/>
     </row>
-    <row r="252" spans="2:7" ht="31.2">
-      <c r="B252" s="41"/>
+    <row r="252" spans="2:7">
+      <c r="B252" s="64"/>
       <c r="C252" s="5"/>
       <c r="D252" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E252" s="6"/>
       <c r="F252" s="5"/>
       <c r="G252" s="5"/>
     </row>
-    <row r="253" spans="2:7" ht="31.2">
-      <c r="B253" s="41"/>
+    <row r="253" spans="2:7">
+      <c r="B253" s="64"/>
       <c r="C253" s="5"/>
       <c r="D253" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E253" s="6"/>
       <c r="F253" s="5"/>
       <c r="G253" s="5"/>
     </row>
     <row r="254" spans="2:7" ht="31.2">
-      <c r="B254" s="41"/>
+      <c r="B254" s="64"/>
       <c r="C254" s="5"/>
       <c r="D254" s="5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E254" s="6"/>
       <c r="F254" s="5"/>
       <c r="G254" s="5"/>
     </row>
     <row r="255" spans="2:7" ht="31.2">
-      <c r="B255" s="41"/>
+      <c r="B255" s="64"/>
       <c r="C255" s="5"/>
       <c r="D255" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E255" s="6"/>
       <c r="F255" s="5"/>
       <c r="G255" s="5"/>
     </row>
-    <row r="256" spans="2:7">
-      <c r="B256" s="41"/>
+    <row r="256" spans="2:7" ht="31.2">
+      <c r="B256" s="64"/>
       <c r="C256" s="5"/>
       <c r="D256" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E256" s="6"/>
       <c r="F256" s="5"/>
       <c r="G256" s="5"/>
     </row>
+    <row r="257" spans="2:7" ht="31.2">
+      <c r="B257" s="64"/>
+      <c r="C257" s="5"/>
+      <c r="D257" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E257" s="6"/>
+      <c r="F257" s="5"/>
+      <c r="G257" s="5"/>
+    </row>
+    <row r="258" spans="2:7">
+      <c r="B258" s="64"/>
+      <c r="C258" s="5"/>
+      <c r="D258" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E258" s="6"/>
+      <c r="F258" s="5"/>
+      <c r="G258" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="B242:B256"/>
-    <mergeCell ref="B96:B100"/>
-    <mergeCell ref="C53:C62"/>
-    <mergeCell ref="C64:C78"/>
-    <mergeCell ref="B53:B78"/>
-    <mergeCell ref="B80:B94"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="B178:B206"/>
-    <mergeCell ref="C178:C198"/>
-    <mergeCell ref="C200:C206"/>
-    <mergeCell ref="B109:B176"/>
-    <mergeCell ref="C109:C112"/>
-    <mergeCell ref="C114:C122"/>
-    <mergeCell ref="C124:C137"/>
-    <mergeCell ref="B217:B231"/>
-    <mergeCell ref="C155:C161"/>
-    <mergeCell ref="B239:B240"/>
-    <mergeCell ref="B5:B51"/>
-    <mergeCell ref="C5:C20"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="C36:C45"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="B105:B107"/>
-    <mergeCell ref="B208:B215"/>
-    <mergeCell ref="C163:C176"/>
-    <mergeCell ref="B233:B237"/>
+  <mergeCells count="40">
+    <mergeCell ref="B244:B258"/>
+    <mergeCell ref="B97:B102"/>
+    <mergeCell ref="C57:C65"/>
+    <mergeCell ref="C67:C81"/>
+    <mergeCell ref="B57:B81"/>
+    <mergeCell ref="B83:B95"/>
+    <mergeCell ref="B104:B105"/>
+    <mergeCell ref="B180:B208"/>
+    <mergeCell ref="C180:C200"/>
+    <mergeCell ref="C202:C208"/>
+    <mergeCell ref="B111:B178"/>
+    <mergeCell ref="C111:C114"/>
+    <mergeCell ref="C116:C124"/>
+    <mergeCell ref="C126:C139"/>
+    <mergeCell ref="B219:B233"/>
+    <mergeCell ref="C157:C163"/>
+    <mergeCell ref="B241:B242"/>
+    <mergeCell ref="B5:B55"/>
+    <mergeCell ref="C5:C24"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="C40:C49"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="B107:B109"/>
+    <mergeCell ref="B210:B217"/>
+    <mergeCell ref="C165:C178"/>
+    <mergeCell ref="B235:B239"/>
     <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D64:D66"/>
-    <mergeCell ref="C139:C143"/>
-    <mergeCell ref="C145:C146"/>
-    <mergeCell ref="C148:C149"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="D67:D69"/>
+    <mergeCell ref="C141:C145"/>
+    <mergeCell ref="C147:C148"/>
+    <mergeCell ref="C150:C151"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="D92:D93"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D5:D6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D239" r:id="rId1"/>
-    <hyperlink ref="D240" r:id="rId2"/>
-    <hyperlink ref="G64" r:id="rId3"/>
-    <hyperlink ref="G65" r:id="rId4"/>
-    <hyperlink ref="G97" r:id="rId5"/>
-    <hyperlink ref="G69" r:id="rId6"/>
-    <hyperlink ref="G59" r:id="rId7"/>
-    <hyperlink ref="G67" r:id="rId8"/>
+    <hyperlink ref="D241" r:id="rId1"/>
+    <hyperlink ref="D242" r:id="rId2"/>
+    <hyperlink ref="G67" r:id="rId3"/>
+    <hyperlink ref="G68" r:id="rId4"/>
+    <hyperlink ref="G98" r:id="rId5"/>
+    <hyperlink ref="G72" r:id="rId6"/>
+    <hyperlink ref="G62" r:id="rId7"/>
+    <hyperlink ref="G70" r:id="rId8"/>
     <hyperlink ref="F2" r:id="rId9" location="foundation-syllabus" display="https://www.codechef.com/certification/prepare#foundation-syllabus"/>
-    <hyperlink ref="G8" r:id="rId10" display="https://www.youtube.com/watch?v=7HCd074v8g8"/>
+    <hyperlink ref="G9" r:id="rId10" display="https://www.youtube.com/watch?v=7HCd074v8g8"/>
     <hyperlink ref="G5" r:id="rId11" location="1039525" display="https://math.stackexchange.com/questions/1039519/finding-prime-factors-by-taking-the-square-root/1039525#1039525"/>
-    <hyperlink ref="G208" r:id="rId12"/>
-    <hyperlink ref="F178" r:id="rId13"/>
-    <hyperlink ref="F53" r:id="rId14" display="https://www.geeksforgeeks.org/advanced-data-structures/"/>
-    <hyperlink ref="G73" r:id="rId15"/>
-    <hyperlink ref="G72" r:id="rId16" display="https://www.youtube.com/watch?v=uxA__b23t2w"/>
-    <hyperlink ref="G76" r:id="rId17"/>
-    <hyperlink ref="G94" r:id="rId18"/>
-    <hyperlink ref="G91" r:id="rId19"/>
+    <hyperlink ref="G210" r:id="rId12"/>
+    <hyperlink ref="F180" r:id="rId13"/>
+    <hyperlink ref="F57" r:id="rId14" display="https://www.geeksforgeeks.org/advanced-data-structures/"/>
+    <hyperlink ref="G76" r:id="rId15"/>
+    <hyperlink ref="G75" r:id="rId16" display="https://www.youtube.com/watch?v=uxA__b23t2w"/>
+    <hyperlink ref="G79" r:id="rId17"/>
+    <hyperlink ref="G95" r:id="rId18"/>
+    <hyperlink ref="G92" r:id="rId19"/>
+    <hyperlink ref="G100" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -4637,51 +4933,51 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="74" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" s="75"/>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="75"/>
+    </row>
+    <row r="5" spans="2:4" ht="31.2">
+      <c r="B5" s="75"/>
+      <c r="C5" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="28.8">
+      <c r="B6" s="75"/>
+      <c r="C6" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4">
-      <c r="B3" s="52"/>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4" s="52"/>
-    </row>
-    <row r="5" spans="2:4" ht="31.2">
-      <c r="B5" s="52"/>
-      <c r="C5" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="28.8">
-      <c r="B6" s="52"/>
-      <c r="C6" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D6" s="2" t="s">
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="75"/>
+      <c r="C7" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="52"/>
-      <c r="C7" s="1" t="s">
-        <v>224</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="52"/>
+      <c r="B8" s="75"/>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="52"/>
+      <c r="B9" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
latst changes are updated
</commit_message>
<xml_diff>
--- a/Algorithm_Topics _to_Learn.xlsx
+++ b/Algorithm_Topics _to_Learn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="242" yWindow="104" windowWidth="14803" windowHeight="8018"/>
   </bookViews>
   <sheets>
     <sheet name="Algorithms" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="305">
   <si>
     <t>Euler Totient Theorem</t>
   </si>
@@ -624,11 +624,6 @@
     <t>https://www.youtube.com/watch?v=AXjmTQ8LEoI</t>
   </si>
   <si>
-    <t>&gt; Tries are an extremely special and useful data-structure that are based on the prefix of a string.
-&gt; Need to create proper base data structure with appropriate elements.
-&gt; Lexographic order of strings is possible by searching the char array alphabetically, can use the count of chars to optimize search</t>
-  </si>
-  <si>
     <t>Rolling hash</t>
   </si>
   <si>
@@ -659,41 +654,16 @@
     <t>https://www.youtube.com/watch?v=Ke_tII6Y0GE&amp;list=PLTZbNwgO5ebqw1v0ODk8cPLW9dQ99Te8f</t>
   </si>
   <si>
-    <t>Codeforces (372B, )</t>
-  </si>
-  <si>
-    <t>Grid/Matrix Problems/Concepts</t>
-  </si>
-  <si>
     <t>Maximum size rectangle binary sub-matrix with all 1s</t>
   </si>
   <si>
-    <t>maximum sum rectangle in 2D matrix</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?time_continue=4&amp;v=yCQN096CwWM</t>
-  </si>
-  <si>
     <t>https://www.geeksforgeeks.org/maximum-size-sub-matrix-with-all-1s-in-a-binary-matrix/</t>
   </si>
   <si>
-    <t>Number of rectangles in N*M grid</t>
-  </si>
-  <si>
-    <t>https://www.geeksforgeeks.org/number-rectangles-nm-grid/</t>
-  </si>
-  <si>
     <t>Suffix Trie</t>
   </si>
   <si>
     <t>https://www.geeksforgeeks.org/count-distinct-substrings-string-using-suffix-trie/</t>
-  </si>
-  <si>
-    <t>&gt; LeetCode
-&gt; Word Search II: search words in a grid</t>
-  </si>
-  <si>
-    <t>Good problems</t>
   </si>
   <si>
     <t>© Counting</t>
@@ -1186,53 +1156,9 @@
     </r>
   </si>
   <si>
-    <t>https://stackoverflow.com/questions/36814088/understanding-how-rolling-hash-works-with-modulus-in-rabin-karp-algorithm</t>
-  </si>
-  <si>
     <t>&gt; Use a large prime number as mod to reduce the collisons
 &gt; For strings, multiply each character incresed power of a prime number
 &gt; djb2 hash function (initial value: 5381, then hash = (hash * 33 + c )%P)</t>
-  </si>
-  <si>
-    <t>&gt; Re-use previously computed hash function to find the next sub-string hash
-&gt; Using position powers as decreasing powers to avoid divison
-&gt; next_h = (((prev_h - 1st_char * (p^len)%q)*p)+nxt_char*p)%q
-&gt; for -ve add q (example string: 2345, len=3, p=7, q=101)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">&gt; Codeforces (319D, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, 407D, 444D, 271D, 869E, 228C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)
-&gt; Spoj (ADACLEAN)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1285,53 +1211,6 @@
   </si>
   <si>
     <t>&gt; For fixed links without delete use a mapping of link address in array to avoid searching</t>
-  </si>
-  <si>
-    <r>
-      <t>&gt; SPOJ (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>good_DICT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>good_PHONELST</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)
-&gt; topcoder (3972, 7694, 6215)
-&gt; Codeforces (633C, 665E, 514C, 858D)</t>
-    </r>
   </si>
   <si>
     <t>https://www.topcoder.com/community/data-science/data-science-tutorials/mathematics-for-topcoders/
@@ -1452,12 +1331,215 @@
   <si>
     <t>&gt; Can use bfs and indegree, it also gives lexographically small order with min priority queue</t>
   </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=H4VrKHVG5qI&amp;t=877s
+https://stackoverflow.com/questions/36814088/understanding-how-rolling-hash-works-with-modulus-in-rabin-karp-algorithm</t>
+  </si>
+  <si>
+    <t>&gt; Re-use previously computed hash function to find the next sub-string hash
+&gt; Using position powers as decreasing powers to avoid divison
+&gt; next_h = (((prev_h - 1st_char * (p^len)%q)*p)+nxt_char*p)%q
+&gt; for -ve hash result add q to make +ve (example string: 2345, len=3, p=7, q=101)</t>
+  </si>
+  <si>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>Directory commands</t>
+  </si>
+  <si>
+    <t>http://codeforces.com/contest/158/problem/C</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Algorithm(s) required</t>
+  </si>
+  <si>
+    <r>
+      <t>&gt; Codeforces (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, 319D, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>407D, 444D, 271D, 869E, 228C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+&gt; Spoj (ADACLEAN)
+&gt; HackerEarth (Needle in Haystack, )</t>
+    </r>
+  </si>
+  <si>
+    <t>Password registration</t>
+  </si>
+  <si>
+    <t>http://codeforces.com/problemset/problem/4/C</t>
+  </si>
+  <si>
+    <t>File system</t>
+  </si>
+  <si>
+    <t>http://codeforces.com/contest/66/problem/C</t>
+  </si>
+  <si>
+    <r>
+      <t>&gt; SPOJ (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>good_DICT</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>good_PHONELST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+&gt; topcoder (3972, 7694, 6215)
+&gt; Codeforces (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>158C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>66C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>633C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 514C, 858D)
+&gt; LeetCode (Word Search II)</t>
+    </r>
+  </si>
+  <si>
+    <t>&gt; Tries is a useful data-structure that are based on the prefix of a string.
+&gt; Need to create proper base data structure with appropriate elements.
+&gt; Lexographic order of strings is possible by searching the char array alphabetically, can use the count of chars to optimize search</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1570,6 +1652,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -1599,12 +1689,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1665,6 +1749,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1737,7 +1827,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1772,206 +1862,194 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1983,6 +2061,7 @@
   <colors>
     <mruColors>
       <color rgb="FF0000FF"/>
+      <color rgb="FFFF99FF"/>
       <color rgb="FFFFCCFF"/>
     </mruColors>
   </colors>
@@ -2274,88 +2353,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:K268"/>
+  <dimension ref="B1:K267"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F133" sqref="F133"/>
+      <pane ySplit="3" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="16.149999999999999"/>
   <cols>
     <col min="1" max="1" width="4" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="40.88671875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="78.77734375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="77.77734375" style="4" customWidth="1"/>
-    <col min="8" max="10" width="8.88671875" style="4"/>
-    <col min="11" max="11" width="18.5546875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="13.8984375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.59765625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="40.8984375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="19.69921875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="78.796875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="77.796875" style="4" customWidth="1"/>
+    <col min="8" max="10" width="8.8984375" style="4"/>
+    <col min="11" max="11" width="18.59765625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="8.8984375" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="8.8984375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11">
-      <c r="C1" s="40" t="s">
-        <v>268</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>266</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" s="3" customFormat="1" ht="30.6" customHeight="1">
-      <c r="B3" s="20" t="s">
+      <c r="C1" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" s="3" customFormat="1" ht="30.7" customHeight="1">
+      <c r="B3" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20" t="s">
+      <c r="E3" s="18"/>
+      <c r="F3" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="18" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="124.8">
-      <c r="B4" s="65" t="s">
+    <row r="4" spans="2:11" ht="129.05000000000001">
+      <c r="B4" s="53" t="s">
         <v>168</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="57" t="s">
         <v>193</v>
       </c>
-      <c r="D4" s="59" t="s">
-        <v>237</v>
+      <c r="D4" s="66" t="s">
+        <v>228</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="65"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="50"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="47"/>
       <c r="G5" s="11"/>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="65"/>
-      <c r="C6" s="66"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="5" t="s">
         <v>0</v>
       </c>
@@ -2367,8 +2446,8 @@
       </c>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="65"/>
-      <c r="C7" s="66"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="5" t="s">
         <v>1</v>
       </c>
@@ -2379,37 +2458,37 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="78">
-      <c r="B8" s="65"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="59" t="s">
+    <row r="8" spans="2:11" ht="80.650000000000006">
+      <c r="B8" s="53"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="66" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" s="65"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="49" t="s">
+      <c r="B9" s="53"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="46" t="s">
         <v>196</v>
       </c>
-      <c r="F9" s="50" t="s">
-        <v>272</v>
+      <c r="F9" s="47" t="s">
+        <v>263</v>
       </c>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="2:11" ht="31.2">
-      <c r="B10" s="65"/>
-      <c r="C10" s="66"/>
+    <row r="10" spans="2:11" ht="32.25">
+      <c r="B10" s="53"/>
+      <c r="C10" s="57"/>
       <c r="D10" s="7" t="s">
         <v>3</v>
       </c>
@@ -2417,31 +2496,31 @@
       <c r="F10" s="7"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="2:11" ht="46.8">
-      <c r="B11" s="65"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="53" t="s">
+    <row r="11" spans="2:11" ht="48.4">
+      <c r="B11" s="53"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="50" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="56" t="s">
-        <v>298</v>
+      <c r="G11" s="73" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="2:11">
-      <c r="B12" s="65"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="53" t="s">
+      <c r="B12" s="53"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="50" t="s">
         <v>182</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="57"/>
+      <c r="G12" s="67"/>
     </row>
     <row r="13" spans="2:11">
-      <c r="B13" s="65"/>
-      <c r="C13" s="66"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="57"/>
       <c r="D13" s="5" t="s">
         <v>5</v>
       </c>
@@ -2449,9 +2528,9 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="2:11" ht="31.2">
-      <c r="B14" s="65"/>
-      <c r="C14" s="66"/>
+    <row r="14" spans="2:11" ht="32.25">
+      <c r="B14" s="53"/>
+      <c r="C14" s="57"/>
       <c r="D14" s="5" t="s">
         <v>6</v>
       </c>
@@ -2460,8 +2539,8 @@
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="2:11">
-      <c r="B15" s="65"/>
-      <c r="C15" s="66"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="57"/>
       <c r="D15" s="5" t="s">
         <v>7</v>
       </c>
@@ -2470,8 +2549,8 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="2:11">
-      <c r="B16" s="65"/>
-      <c r="C16" s="66"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="57"/>
       <c r="D16" s="5" t="s">
         <v>8</v>
       </c>
@@ -2480,8 +2559,8 @@
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="65"/>
-      <c r="C17" s="66"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="57"/>
       <c r="D17" s="5" t="s">
         <v>9</v>
       </c>
@@ -2490,8 +2569,8 @@
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="65"/>
-      <c r="C18" s="66"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="5" t="s">
         <v>10</v>
       </c>
@@ -2500,8 +2579,8 @@
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="65"/>
-      <c r="C19" s="66"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="57"/>
       <c r="D19" s="5" t="s">
         <v>11</v>
       </c>
@@ -2510,8 +2589,8 @@
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="65"/>
-      <c r="C20" s="66"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="57"/>
       <c r="D20" s="5" t="s">
         <v>12</v>
       </c>
@@ -2520,48 +2599,48 @@
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="65"/>
-      <c r="C21" s="66"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="57"/>
       <c r="D21" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E21" s="6"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-    </row>
-    <row r="22" spans="2:7" ht="89.4">
-      <c r="B22" s="65"/>
-      <c r="C22" s="66"/>
-      <c r="D22" s="36" t="s">
-        <v>273</v>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+    </row>
+    <row r="22" spans="2:7" ht="91.6">
+      <c r="B22" s="53"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="33" t="s">
+        <v>264</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="G22" s="44"/>
+        <v>265</v>
+      </c>
+      <c r="G22" s="41"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="65"/>
-      <c r="C23" s="66"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="57"/>
       <c r="D23" s="7"/>
       <c r="E23" s="8"/>
       <c r="F23" s="7"/>
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="65"/>
+      <c r="B24" s="53"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="2:7" ht="31.2">
-      <c r="B25" s="65"/>
-      <c r="C25" s="66" t="s">
+    <row r="25" spans="2:7">
+      <c r="B25" s="53"/>
+      <c r="C25" s="57" t="s">
         <v>192</v>
       </c>
       <c r="D25" s="5" t="s">
@@ -2572,8 +2651,8 @@
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="65"/>
-      <c r="C26" s="66"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="57"/>
       <c r="D26" s="5" t="s">
         <v>15</v>
       </c>
@@ -2582,8 +2661,8 @@
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="65"/>
-      <c r="C27" s="66"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="57"/>
       <c r="D27" s="5" t="s">
         <v>16</v>
       </c>
@@ -2592,8 +2671,8 @@
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="65"/>
-      <c r="C28" s="66"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="57"/>
       <c r="D28" s="5" t="s">
         <v>17</v>
       </c>
@@ -2601,9 +2680,9 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="2:7" ht="31.2">
-      <c r="B29" s="65"/>
-      <c r="C29" s="66"/>
+    <row r="29" spans="2:7" ht="32.25">
+      <c r="B29" s="53"/>
+      <c r="C29" s="57"/>
       <c r="D29" s="5" t="s">
         <v>18</v>
       </c>
@@ -2612,7 +2691,7 @@
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="65"/>
+      <c r="B30" s="53"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="6"/>
@@ -2620,9 +2699,9 @@
       <c r="G30" s="5"/>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="65"/>
-      <c r="C31" s="66" t="s">
-        <v>222</v>
+      <c r="B31" s="53"/>
+      <c r="C31" s="57" t="s">
+        <v>213</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>19</v>
@@ -2631,21 +2710,21 @@
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="2:7" ht="28.8">
-      <c r="B32" s="65"/>
-      <c r="C32" s="66"/>
-      <c r="D32" s="53" t="s">
-        <v>299</v>
+    <row r="32" spans="2:7">
+      <c r="B32" s="53"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="50" t="s">
+        <v>286</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="9"/>
-      <c r="G32" s="43" t="s">
-        <v>300</v>
+      <c r="G32" s="40" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="65"/>
-      <c r="C33" s="66"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="57"/>
       <c r="D33" s="5" t="s">
         <v>20</v>
       </c>
@@ -2653,9 +2732,9 @@
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="2:7" ht="46.8">
-      <c r="B34" s="65"/>
-      <c r="C34" s="66"/>
+    <row r="34" spans="2:7" ht="32.25">
+      <c r="B34" s="53"/>
+      <c r="C34" s="57"/>
       <c r="D34" s="5" t="s">
         <v>21</v>
       </c>
@@ -2664,8 +2743,8 @@
       <c r="G34" s="5"/>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="65"/>
-      <c r="C35" s="66"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="57"/>
       <c r="D35" s="5" t="s">
         <v>22</v>
       </c>
@@ -2674,8 +2753,8 @@
       <c r="G35" s="5"/>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="65"/>
-      <c r="C36" s="66"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="57"/>
       <c r="D36" s="5" t="s">
         <v>23</v>
       </c>
@@ -2684,17 +2763,17 @@
       <c r="G36" s="5"/>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="65"/>
+      <c r="B37" s="53"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="6"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="2:7" ht="31.2">
-      <c r="B38" s="65"/>
-      <c r="C38" s="25" t="s">
-        <v>223</v>
+    <row r="38" spans="2:7" ht="32.25">
+      <c r="B38" s="53"/>
+      <c r="C38" s="23" t="s">
+        <v>214</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="6"/>
@@ -2702,7 +2781,7 @@
       <c r="G38" s="5"/>
     </row>
     <row r="39" spans="2:7">
-      <c r="B39" s="65"/>
+      <c r="B39" s="53"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="6"/>
@@ -2710,9 +2789,9 @@
       <c r="G39" s="5"/>
     </row>
     <row r="40" spans="2:7">
-      <c r="B40" s="65"/>
-      <c r="C40" s="66" t="s">
-        <v>224</v>
+      <c r="B40" s="53"/>
+      <c r="C40" s="57" t="s">
+        <v>215</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>24</v>
@@ -2721,9 +2800,9 @@
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="2:7" ht="31.2">
-      <c r="B41" s="65"/>
-      <c r="C41" s="66"/>
+    <row r="41" spans="2:7" ht="32.25">
+      <c r="B41" s="53"/>
+      <c r="C41" s="57"/>
       <c r="D41" s="5" t="s">
         <v>25</v>
       </c>
@@ -2731,9 +2810,9 @@
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="2:7" ht="46.8">
-      <c r="B42" s="65"/>
-      <c r="C42" s="66"/>
+    <row r="42" spans="2:7" ht="48.4">
+      <c r="B42" s="53"/>
+      <c r="C42" s="57"/>
       <c r="D42" s="5" t="s">
         <v>26</v>
       </c>
@@ -2741,9 +2820,9 @@
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="2:7" ht="46.8">
-      <c r="B43" s="65"/>
-      <c r="C43" s="66"/>
+    <row r="43" spans="2:7" ht="48.4">
+      <c r="B43" s="53"/>
+      <c r="C43" s="57"/>
       <c r="D43" s="5" t="s">
         <v>27</v>
       </c>
@@ -2752,8 +2831,8 @@
       <c r="G43" s="5"/>
     </row>
     <row r="44" spans="2:7">
-      <c r="B44" s="65"/>
-      <c r="C44" s="66"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="57"/>
       <c r="D44" s="5" t="s">
         <v>28</v>
       </c>
@@ -2761,9 +2840,9 @@
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="2:7" ht="31.2">
-      <c r="B45" s="65"/>
-      <c r="C45" s="66"/>
+    <row r="45" spans="2:7">
+      <c r="B45" s="53"/>
+      <c r="C45" s="57"/>
       <c r="D45" s="5" t="s">
         <v>29</v>
       </c>
@@ -2772,8 +2851,8 @@
       <c r="G45" s="5"/>
     </row>
     <row r="46" spans="2:7">
-      <c r="B46" s="65"/>
-      <c r="C46" s="66"/>
+      <c r="B46" s="53"/>
+      <c r="C46" s="57"/>
       <c r="D46" s="5" t="s">
         <v>30</v>
       </c>
@@ -2781,9 +2860,9 @@
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="2:7" ht="46.8">
-      <c r="B47" s="65"/>
-      <c r="C47" s="66"/>
+    <row r="47" spans="2:7" ht="32.25">
+      <c r="B47" s="53"/>
+      <c r="C47" s="57"/>
       <c r="D47" s="5" t="s">
         <v>31</v>
       </c>
@@ -2792,8 +2871,8 @@
       <c r="G47" s="5"/>
     </row>
     <row r="48" spans="2:7">
-      <c r="B48" s="65"/>
-      <c r="C48" s="66"/>
+      <c r="B48" s="53"/>
+      <c r="C48" s="57"/>
       <c r="D48" s="5" t="s">
         <v>32</v>
       </c>
@@ -2802,9 +2881,9 @@
       <c r="G48" s="5"/>
     </row>
     <row r="49" spans="2:7">
-      <c r="B49" s="65"/>
-      <c r="C49" s="66"/>
-      <c r="D49" s="19" t="s">
+      <c r="B49" s="53"/>
+      <c r="C49" s="57"/>
+      <c r="D49" s="17" t="s">
         <v>183</v>
       </c>
       <c r="E49" s="8"/>
@@ -2812,17 +2891,17 @@
       <c r="G49" s="5"/>
     </row>
     <row r="50" spans="2:7">
-      <c r="B50" s="65"/>
+      <c r="B50" s="53"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="6"/>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
     </row>
-    <row r="51" spans="2:7" ht="31.2">
-      <c r="B51" s="65"/>
-      <c r="C51" s="66" t="s">
-        <v>225</v>
+    <row r="51" spans="2:7" ht="32.25">
+      <c r="B51" s="53"/>
+      <c r="C51" s="57" t="s">
+        <v>216</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>33</v>
@@ -2832,8 +2911,8 @@
       <c r="G51" s="5"/>
     </row>
     <row r="52" spans="2:7">
-      <c r="B52" s="65"/>
-      <c r="C52" s="66"/>
+      <c r="B52" s="53"/>
+      <c r="C52" s="57"/>
       <c r="D52" s="5" t="s">
         <v>34</v>
       </c>
@@ -2842,7 +2921,7 @@
       <c r="G52" s="5"/>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="65"/>
+      <c r="B53" s="53"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="6"/>
@@ -2850,9 +2929,9 @@
       <c r="G53" s="5"/>
     </row>
     <row r="54" spans="2:7">
-      <c r="B54" s="65"/>
-      <c r="C54" s="66" t="s">
-        <v>226</v>
+      <c r="B54" s="53"/>
+      <c r="C54" s="57" t="s">
+        <v>217</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>35</v>
@@ -2862,8 +2941,8 @@
       <c r="G54" s="5"/>
     </row>
     <row r="55" spans="2:7">
-      <c r="B55" s="65"/>
-      <c r="C55" s="66"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="57"/>
       <c r="D55" s="5" t="s">
         <v>36</v>
       </c>
@@ -2872,7 +2951,7 @@
       <c r="G55" s="5"/>
     </row>
     <row r="56" spans="2:7">
-      <c r="B56" s="26"/>
+      <c r="B56" s="24"/>
       <c r="C56" s="5" t="s">
         <v>37</v>
       </c>
@@ -2881,23 +2960,23 @@
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
     </row>
-    <row r="57" spans="2:7" ht="31.2">
-      <c r="B57" s="65" t="s">
+    <row r="57" spans="2:7" ht="32.25">
+      <c r="B57" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="C57" s="72" t="s">
+      <c r="C57" s="54" t="s">
         <v>178</v>
       </c>
-      <c r="D57" s="16"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="27" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" ht="31.2">
-      <c r="B58" s="65"/>
-      <c r="C58" s="73"/>
-      <c r="D58" s="5" t="s">
+      <c r="D57" s="14"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="25" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7">
+      <c r="B58" s="53"/>
+      <c r="C58" s="55"/>
+      <c r="D58" s="17" t="s">
         <v>85</v>
       </c>
       <c r="E58" s="6"/>
@@ -2905,8 +2984,8 @@
       <c r="G58" s="5"/>
     </row>
     <row r="59" spans="2:7">
-      <c r="B59" s="65"/>
-      <c r="C59" s="73"/>
+      <c r="B59" s="53"/>
+      <c r="C59" s="55"/>
       <c r="D59" s="5" t="s">
         <v>86</v>
       </c>
@@ -2915,8 +2994,8 @@
       <c r="G59" s="5"/>
     </row>
     <row r="60" spans="2:7">
-      <c r="B60" s="65"/>
-      <c r="C60" s="73"/>
+      <c r="B60" s="53"/>
+      <c r="C60" s="55"/>
       <c r="D60" s="5" t="s">
         <v>87</v>
       </c>
@@ -2925,75 +3004,75 @@
       <c r="G60" s="5"/>
     </row>
     <row r="61" spans="2:7">
-      <c r="B61" s="65"/>
-      <c r="C61" s="73"/>
-      <c r="D61" s="45" t="s">
-        <v>276</v>
+      <c r="B61" s="53"/>
+      <c r="C61" s="55"/>
+      <c r="D61" s="42" t="s">
+        <v>267</v>
       </c>
       <c r="E61" s="6"/>
-      <c r="F61" s="45" t="s">
-        <v>277</v>
-      </c>
-      <c r="G61" s="45"/>
+      <c r="F61" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="G61" s="42"/>
     </row>
     <row r="62" spans="2:7">
-      <c r="B62" s="65"/>
-      <c r="C62" s="73"/>
-      <c r="D62" s="36" t="s">
+      <c r="B62" s="53"/>
+      <c r="C62" s="55"/>
+      <c r="D62" s="33" t="s">
         <v>88</v>
       </c>
       <c r="E62" s="6"/>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
     </row>
-    <row r="63" spans="2:7" ht="46.8">
-      <c r="B63" s="65"/>
-      <c r="C63" s="73"/>
-      <c r="D63" s="32" t="s">
+    <row r="63" spans="2:7" ht="48.4">
+      <c r="B63" s="53"/>
+      <c r="C63" s="55"/>
+      <c r="D63" s="30" t="s">
         <v>89</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" ht="62.4">
-      <c r="B64" s="65"/>
-      <c r="C64" s="73"/>
-      <c r="D64" s="54" t="s">
-        <v>200</v>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" ht="64.55">
+      <c r="B64" s="53"/>
+      <c r="C64" s="55"/>
+      <c r="D64" s="68" t="s">
+        <v>199</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="G64" s="43" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" ht="31.2">
-      <c r="B65" s="65"/>
-      <c r="C65" s="73"/>
-      <c r="D65" s="55"/>
-      <c r="E65" s="49" t="s">
+        <v>292</v>
+      </c>
+      <c r="G64" s="40" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" ht="48.4">
+      <c r="B65" s="53"/>
+      <c r="C65" s="55"/>
+      <c r="D65" s="70"/>
+      <c r="E65" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="F65" s="50" t="s">
-        <v>289</v>
+      <c r="F65" s="47" t="s">
+        <v>298</v>
       </c>
       <c r="G65" s="5"/>
     </row>
     <row r="66" spans="2:7">
-      <c r="B66" s="65"/>
-      <c r="C66" s="74"/>
-      <c r="D66" s="19" t="s">
+      <c r="B66" s="53"/>
+      <c r="C66" s="56"/>
+      <c r="D66" s="17" t="s">
         <v>90</v>
       </c>
       <c r="E66" s="6"/>
@@ -3001,35 +3080,35 @@
       <c r="G66" s="5"/>
     </row>
     <row r="67" spans="2:7">
-      <c r="B67" s="65"/>
+      <c r="B67" s="53"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
       <c r="E67" s="6"/>
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
     </row>
-    <row r="68" spans="2:7" ht="78">
-      <c r="B68" s="65"/>
-      <c r="C68" s="72" t="s">
+    <row r="68" spans="2:7" ht="64.55">
+      <c r="B68" s="53"/>
+      <c r="C68" s="54" t="s">
         <v>179</v>
       </c>
-      <c r="D68" s="54" t="s">
+      <c r="D68" s="68" t="s">
         <v>91</v>
       </c>
       <c r="E68" s="10" t="s">
         <v>194</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>199</v>
+        <v>304</v>
       </c>
       <c r="G68" s="11" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="69" spans="2:7">
-      <c r="B69" s="65"/>
-      <c r="C69" s="73"/>
-      <c r="D69" s="60"/>
+      <c r="B69" s="53"/>
+      <c r="C69" s="55"/>
+      <c r="D69" s="69"/>
       <c r="E69" s="10" t="s">
         <v>195</v>
       </c>
@@ -3038,1648 +3117,1644 @@
         <v>197</v>
       </c>
     </row>
-    <row r="70" spans="2:7" ht="46.8">
-      <c r="B70" s="65"/>
-      <c r="C70" s="73"/>
-      <c r="D70" s="55"/>
-      <c r="E70" s="49" t="s">
+    <row r="70" spans="2:7" ht="64.55">
+      <c r="B70" s="53"/>
+      <c r="C70" s="55"/>
+      <c r="D70" s="70"/>
+      <c r="E70" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="F70" s="50" t="s">
-        <v>294</v>
+      <c r="F70" s="47" t="s">
+        <v>303</v>
       </c>
       <c r="G70" s="11"/>
     </row>
-    <row r="71" spans="2:7" ht="31.2">
-      <c r="B71" s="65"/>
-      <c r="C71" s="73"/>
-      <c r="D71" s="37" t="s">
-        <v>218</v>
+    <row r="71" spans="2:7" ht="32.25">
+      <c r="B71" s="53"/>
+      <c r="C71" s="55"/>
+      <c r="D71" s="34" t="s">
+        <v>211</v>
       </c>
       <c r="E71" s="10"/>
       <c r="F71" s="9" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="72" spans="2:7">
-      <c r="B72" s="65"/>
-      <c r="C72" s="73"/>
-      <c r="D72" s="38" t="s">
-        <v>256</v>
+      <c r="B72" s="53"/>
+      <c r="C72" s="55"/>
+      <c r="D72" s="35" t="s">
+        <v>247</v>
       </c>
       <c r="E72" s="8"/>
       <c r="F72" s="7"/>
       <c r="G72" s="11"/>
     </row>
     <row r="73" spans="2:7">
-      <c r="B73" s="65"/>
-      <c r="C73" s="73"/>
-      <c r="D73" s="19" t="s">
+      <c r="B73" s="53"/>
+      <c r="C73" s="55"/>
+      <c r="D73" s="17" t="s">
         <v>92</v>
       </c>
       <c r="E73" s="8"/>
       <c r="F73" s="7"/>
       <c r="G73" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="74" spans="2:7">
-      <c r="B74" s="65"/>
-      <c r="C74" s="73"/>
-      <c r="D74" s="19" t="s">
-        <v>208</v>
+      <c r="B74" s="53"/>
+      <c r="C74" s="55"/>
+      <c r="D74" s="17" t="s">
+        <v>207</v>
       </c>
       <c r="E74" s="8"/>
       <c r="F74" s="7"/>
       <c r="G74" s="5"/>
     </row>
     <row r="75" spans="2:7">
-      <c r="B75" s="65"/>
-      <c r="C75" s="73"/>
-      <c r="D75" s="19" t="s">
+      <c r="B75" s="53"/>
+      <c r="C75" s="55"/>
+      <c r="D75" s="17" t="s">
         <v>93</v>
       </c>
       <c r="E75" s="8"/>
       <c r="F75" s="7"/>
       <c r="G75" s="5"/>
     </row>
-    <row r="76" spans="2:7" ht="124.8">
-      <c r="B76" s="65"/>
-      <c r="C76" s="73"/>
-      <c r="D76" s="59" t="s">
-        <v>206</v>
+    <row r="76" spans="2:7" ht="129.05000000000001">
+      <c r="B76" s="53"/>
+      <c r="C76" s="55"/>
+      <c r="D76" s="66" t="s">
+        <v>205</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>195</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="77" spans="2:7" ht="46.8">
-      <c r="B77" s="65"/>
-      <c r="C77" s="73"/>
-      <c r="D77" s="61"/>
-      <c r="E77" s="49" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" ht="48.4">
+      <c r="B77" s="53"/>
+      <c r="C77" s="55"/>
+      <c r="D77" s="71"/>
+      <c r="E77" s="46" t="s">
         <v>196</v>
       </c>
-      <c r="F77" s="50" t="s">
-        <v>250</v>
+      <c r="F77" s="47" t="s">
+        <v>241</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="78" spans="2:7">
-      <c r="B78" s="65"/>
-      <c r="C78" s="73"/>
-      <c r="D78" s="30" t="s">
-        <v>249</v>
+      <c r="B78" s="53"/>
+      <c r="C78" s="55"/>
+      <c r="D78" s="28" t="s">
+        <v>240</v>
       </c>
       <c r="E78" s="8"/>
       <c r="F78" s="7" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="G78" s="11"/>
     </row>
     <row r="79" spans="2:7">
-      <c r="B79" s="65"/>
-      <c r="C79" s="73"/>
-      <c r="D79" s="19" t="s">
-        <v>207</v>
+      <c r="B79" s="53"/>
+      <c r="C79" s="55"/>
+      <c r="D79" s="17" t="s">
+        <v>206</v>
       </c>
       <c r="E79" s="8"/>
       <c r="F79" s="7"/>
       <c r="G79" s="11"/>
     </row>
     <row r="80" spans="2:7">
-      <c r="B80" s="65"/>
-      <c r="C80" s="73"/>
-      <c r="D80" s="62" t="s">
-        <v>243</v>
-      </c>
-      <c r="E80" s="21"/>
-      <c r="F80" s="28" t="s">
-        <v>245</v>
-      </c>
-      <c r="G80" s="29" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" ht="31.2">
-      <c r="B81" s="65"/>
-      <c r="C81" s="73"/>
-      <c r="D81" s="62"/>
-      <c r="E81" s="49" t="s">
+      <c r="B80" s="53"/>
+      <c r="C80" s="55"/>
+      <c r="D80" s="72" t="s">
+        <v>234</v>
+      </c>
+      <c r="E80" s="19"/>
+      <c r="F80" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="G80" s="27" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" ht="32.25">
+      <c r="B81" s="53"/>
+      <c r="C81" s="55"/>
+      <c r="D81" s="72"/>
+      <c r="E81" s="46" t="s">
         <v>196</v>
       </c>
-      <c r="F81" s="51" t="s">
-        <v>271</v>
-      </c>
-      <c r="G81" s="29"/>
-    </row>
-    <row r="82" spans="2:7" ht="31.2">
-      <c r="B82" s="65"/>
-      <c r="C82" s="74"/>
-      <c r="D82" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="E82" s="12"/>
-      <c r="F82" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="G82" s="11"/>
+      <c r="F81" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="G81" s="27"/>
+    </row>
+    <row r="82" spans="2:7">
+      <c r="B82" s="24"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
     </row>
     <row r="83" spans="2:7">
-      <c r="B83" s="26"/>
+      <c r="B83" s="53" t="s">
+        <v>94</v>
+      </c>
       <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
+      <c r="D83" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="E83" s="6"/>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
     </row>
     <row r="84" spans="2:7">
-      <c r="B84" s="65" t="s">
-        <v>94</v>
-      </c>
+      <c r="B84" s="53"/>
       <c r="C84" s="5"/>
-      <c r="D84" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E84" s="6"/>
-      <c r="F84" s="5"/>
+      <c r="D84" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="E84" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="F84" s="47" t="s">
+        <v>266</v>
+      </c>
       <c r="G84" s="5"/>
     </row>
     <row r="85" spans="2:7">
-      <c r="B85" s="65"/>
+      <c r="B85" s="53"/>
       <c r="C85" s="5"/>
-      <c r="D85" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="E85" s="49" t="s">
-        <v>196</v>
-      </c>
-      <c r="F85" s="50" t="s">
-        <v>275</v>
-      </c>
+      <c r="D85" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E85" s="6"/>
+      <c r="F85" s="5"/>
       <c r="G85" s="5"/>
     </row>
     <row r="86" spans="2:7">
-      <c r="B86" s="65"/>
+      <c r="B86" s="53"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E86" s="6"/>
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
     </row>
     <row r="87" spans="2:7">
-      <c r="B87" s="65"/>
+      <c r="B87" s="53"/>
       <c r="C87" s="5"/>
-      <c r="D87" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E87" s="6"/>
-      <c r="F87" s="5"/>
+      <c r="D87" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E87" s="8"/>
+      <c r="F87" s="7"/>
       <c r="G87" s="5"/>
     </row>
     <row r="88" spans="2:7">
-      <c r="B88" s="65"/>
+      <c r="B88" s="53"/>
       <c r="C88" s="5"/>
-      <c r="D88" s="32" t="s">
-        <v>99</v>
+      <c r="D88" s="31" t="s">
+        <v>100</v>
       </c>
       <c r="E88" s="8"/>
       <c r="F88" s="7"/>
       <c r="G88" s="5"/>
     </row>
     <row r="89" spans="2:7">
-      <c r="B89" s="65"/>
+      <c r="B89" s="53"/>
       <c r="C89" s="5"/>
-      <c r="D89" s="34" t="s">
-        <v>100</v>
+      <c r="D89" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="E89" s="8"/>
       <c r="F89" s="7"/>
       <c r="G89" s="5"/>
     </row>
-    <row r="90" spans="2:7">
-      <c r="B90" s="65"/>
+    <row r="90" spans="2:7" ht="32.25">
+      <c r="B90" s="53"/>
       <c r="C90" s="5"/>
-      <c r="D90" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E90" s="8"/>
-      <c r="F90" s="7"/>
+      <c r="D90" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>251</v>
+      </c>
       <c r="G90" s="5"/>
     </row>
-    <row r="91" spans="2:7" ht="31.2">
-      <c r="B91" s="65"/>
+    <row r="91" spans="2:7">
+      <c r="B91" s="53"/>
       <c r="C91" s="5"/>
-      <c r="D91" s="58" t="s">
-        <v>102</v>
-      </c>
-      <c r="E91" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="F91" s="9" t="s">
-        <v>260</v>
-      </c>
+      <c r="D91" s="70"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="9"/>
       <c r="G91" s="5"/>
     </row>
-    <row r="92" spans="2:7">
-      <c r="B92" s="65"/>
+    <row r="92" spans="2:7" ht="48.4">
+      <c r="B92" s="53"/>
       <c r="C92" s="5"/>
-      <c r="D92" s="55"/>
-      <c r="E92" s="10"/>
-      <c r="F92" s="9"/>
-      <c r="G92" s="5"/>
-    </row>
-    <row r="93" spans="2:7" ht="46.8">
-      <c r="B93" s="65"/>
+      <c r="D92" s="74" t="s">
+        <v>249</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="G92" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7">
+      <c r="B93" s="53"/>
       <c r="C93" s="5"/>
-      <c r="D93" s="58" t="s">
-        <v>258</v>
-      </c>
-      <c r="E93" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="F93" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="G93" s="11" t="s">
-        <v>261</v>
-      </c>
+      <c r="D93" s="70"/>
+      <c r="E93" s="46"/>
+      <c r="F93" s="47" t="s">
+        <v>254</v>
+      </c>
+      <c r="G93" s="5"/>
     </row>
     <row r="94" spans="2:7">
-      <c r="B94" s="65"/>
+      <c r="B94" s="53"/>
       <c r="C94" s="5"/>
-      <c r="D94" s="55"/>
-      <c r="E94" s="49"/>
-      <c r="F94" s="50" t="s">
-        <v>263</v>
-      </c>
+      <c r="D94" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E94" s="6"/>
+      <c r="F94" s="5"/>
       <c r="G94" s="5"/>
     </row>
-    <row r="95" spans="2:7">
-      <c r="B95" s="65"/>
+    <row r="95" spans="2:7" ht="32.25">
+      <c r="B95" s="53"/>
       <c r="C95" s="5"/>
-      <c r="D95" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E95" s="6"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="5"/>
-    </row>
-    <row r="96" spans="2:7" ht="46.8">
-      <c r="B96" s="65"/>
+      <c r="D95" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="E95" s="10"/>
+      <c r="F95" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="G95" s="11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7">
+      <c r="B96" s="24"/>
       <c r="C96" s="5"/>
-      <c r="D96" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="E96" s="10"/>
-      <c r="F96" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="G96" s="11" t="s">
-        <v>246</v>
-      </c>
+      <c r="D96" s="5"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
     </row>
     <row r="97" spans="2:7">
-      <c r="B97" s="26"/>
+      <c r="B97" s="53" t="s">
+        <v>174</v>
+      </c>
       <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="6"/>
-      <c r="F97" s="5"/>
+      <c r="D97" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="E97" s="13"/>
+      <c r="F97" s="12"/>
       <c r="G97" s="5"/>
     </row>
     <row r="98" spans="2:7">
-      <c r="B98" s="65" t="s">
-        <v>174</v>
-      </c>
+      <c r="B98" s="53"/>
       <c r="C98" s="5"/>
-      <c r="D98" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="E98" s="15"/>
-      <c r="F98" s="14"/>
-      <c r="G98" s="5"/>
+      <c r="D98" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="E98" s="10"/>
+      <c r="F98" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="G98" s="11" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="99" spans="2:7">
-      <c r="B99" s="65"/>
+      <c r="B99" s="53"/>
       <c r="C99" s="5"/>
-      <c r="D99" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="E99" s="10"/>
-      <c r="F99" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="G99" s="11" t="s">
-        <v>202</v>
-      </c>
+      <c r="D99" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="E99" s="13"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="5"/>
     </row>
     <row r="100" spans="2:7">
-      <c r="B100" s="65"/>
+      <c r="B100" s="53"/>
       <c r="C100" s="5"/>
       <c r="D100" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="E100" s="15"/>
-      <c r="F100" s="14"/>
-      <c r="G100" s="5"/>
+        <v>176</v>
+      </c>
+      <c r="E100" s="10"/>
+      <c r="F100" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="G100" s="40" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="101" spans="2:7">
-      <c r="B101" s="65"/>
-      <c r="C101" s="5"/>
-      <c r="D101" s="36" t="s">
-        <v>176</v>
-      </c>
-      <c r="E101" s="10"/>
-      <c r="F101" s="9" t="s">
+      <c r="B101" s="53"/>
+      <c r="C101" s="32"/>
+      <c r="D101" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="E101" s="13"/>
+      <c r="F101" s="12"/>
+      <c r="G101" s="32"/>
+    </row>
+    <row r="102" spans="2:7">
+      <c r="B102" s="53"/>
+      <c r="C102" s="43"/>
+      <c r="D102" s="29" t="s">
         <v>270</v>
       </c>
-      <c r="G101" s="43" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="102" spans="2:7">
-      <c r="B102" s="65"/>
-      <c r="C102" s="35"/>
-      <c r="D102" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="E102" s="15"/>
-      <c r="F102" s="14"/>
-      <c r="G102" s="35"/>
+      <c r="E102" s="13"/>
+      <c r="F102" s="12"/>
+      <c r="G102" s="43"/>
     </row>
     <row r="103" spans="2:7">
-      <c r="B103" s="65"/>
-      <c r="C103" s="46"/>
-      <c r="D103" s="31" t="s">
-        <v>279</v>
-      </c>
-      <c r="E103" s="15"/>
-      <c r="F103" s="14"/>
-      <c r="G103" s="46"/>
-    </row>
-    <row r="104" spans="2:7">
-      <c r="B104" s="65"/>
-      <c r="C104" s="47"/>
-      <c r="D104" s="31" t="s">
-        <v>281</v>
-      </c>
-      <c r="E104" s="15"/>
-      <c r="F104" s="14"/>
-      <c r="G104" s="47"/>
-    </row>
-    <row r="105" spans="2:7" ht="46.8">
-      <c r="B105" s="65"/>
-      <c r="C105" s="48"/>
-      <c r="D105" s="54" t="s">
-        <v>283</v>
-      </c>
-      <c r="E105" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="F105" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="G105" s="43" t="s">
-        <v>282</v>
-      </c>
+      <c r="B103" s="53"/>
+      <c r="C103" s="44"/>
+      <c r="D103" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="E103" s="13"/>
+      <c r="F103" s="12"/>
+      <c r="G103" s="44"/>
+    </row>
+    <row r="104" spans="2:7" ht="48.4">
+      <c r="B104" s="53"/>
+      <c r="C104" s="45"/>
+      <c r="D104" s="68" t="s">
+        <v>274</v>
+      </c>
+      <c r="E104" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="F104" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="G104" s="40" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7">
+      <c r="B105" s="53"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="70"/>
+      <c r="E105" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="F105" s="47" t="s">
+        <v>276</v>
+      </c>
+      <c r="G105" s="5"/>
     </row>
     <row r="106" spans="2:7">
-      <c r="B106" s="65"/>
+      <c r="B106" s="24"/>
       <c r="C106" s="5"/>
-      <c r="D106" s="55"/>
-      <c r="E106" s="49" t="s">
-        <v>196</v>
-      </c>
-      <c r="F106" s="50" t="s">
-        <v>285</v>
-      </c>
+      <c r="D106" s="5"/>
+      <c r="E106" s="6"/>
+      <c r="F106" s="5"/>
       <c r="G106" s="5"/>
     </row>
     <row r="107" spans="2:7">
-      <c r="B107" s="26"/>
+      <c r="B107" s="53" t="s">
+        <v>105</v>
+      </c>
       <c r="C107" s="5"/>
-      <c r="D107" s="5"/>
+      <c r="D107" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="E107" s="6"/>
       <c r="F107" s="5"/>
       <c r="G107" s="5"/>
     </row>
     <row r="108" spans="2:7">
-      <c r="B108" s="65" t="s">
-        <v>105</v>
-      </c>
+      <c r="B108" s="53"/>
       <c r="C108" s="5"/>
       <c r="D108" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E108" s="6"/>
       <c r="F108" s="5"/>
       <c r="G108" s="5"/>
     </row>
     <row r="109" spans="2:7">
-      <c r="B109" s="65"/>
+      <c r="B109" s="24"/>
       <c r="C109" s="5"/>
-      <c r="D109" s="5" t="s">
-        <v>107</v>
-      </c>
+      <c r="D109" s="5"/>
       <c r="E109" s="6"/>
       <c r="F109" s="5"/>
       <c r="G109" s="5"/>
     </row>
     <row r="110" spans="2:7">
-      <c r="B110" s="26"/>
+      <c r="B110" s="53" t="s">
+        <v>136</v>
+      </c>
       <c r="C110" s="5"/>
-      <c r="D110" s="5"/>
+      <c r="D110" s="5" t="s">
+        <v>137</v>
+      </c>
       <c r="E110" s="6"/>
       <c r="F110" s="5"/>
       <c r="G110" s="5"/>
     </row>
     <row r="111" spans="2:7">
-      <c r="B111" s="65" t="s">
-        <v>136</v>
-      </c>
+      <c r="B111" s="53"/>
       <c r="C111" s="5"/>
       <c r="D111" s="5" t="s">
-        <v>137</v>
+        <v>99</v>
       </c>
       <c r="E111" s="6"/>
       <c r="F111" s="5"/>
       <c r="G111" s="5"/>
     </row>
     <row r="112" spans="2:7">
-      <c r="B112" s="65"/>
+      <c r="B112" s="53"/>
       <c r="C112" s="5"/>
       <c r="D112" s="5" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="E112" s="6"/>
       <c r="F112" s="5"/>
       <c r="G112" s="5"/>
     </row>
     <row r="113" spans="2:7">
-      <c r="B113" s="65"/>
+      <c r="B113" s="24"/>
       <c r="C113" s="5"/>
-      <c r="D113" s="5" t="s">
-        <v>138</v>
-      </c>
+      <c r="D113" s="5"/>
       <c r="E113" s="6"/>
       <c r="F113" s="5"/>
       <c r="G113" s="5"/>
     </row>
     <row r="114" spans="2:7">
-      <c r="B114" s="26"/>
-      <c r="C114" s="5"/>
-      <c r="D114" s="5"/>
+      <c r="B114" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="C114" s="57" t="s">
+        <v>218</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="E114" s="6"/>
       <c r="F114" s="5"/>
       <c r="G114" s="5"/>
     </row>
     <row r="115" spans="2:7">
-      <c r="B115" s="75" t="s">
-        <v>38</v>
-      </c>
-      <c r="C115" s="66" t="s">
-        <v>227</v>
-      </c>
+      <c r="B115" s="58"/>
+      <c r="C115" s="57"/>
       <c r="D115" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E115" s="6"/>
       <c r="F115" s="5"/>
       <c r="G115" s="5"/>
     </row>
     <row r="116" spans="2:7">
-      <c r="B116" s="75"/>
-      <c r="C116" s="66"/>
+      <c r="B116" s="58"/>
+      <c r="C116" s="57"/>
       <c r="D116" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E116" s="6"/>
       <c r="F116" s="5"/>
       <c r="G116" s="5"/>
     </row>
     <row r="117" spans="2:7">
-      <c r="B117" s="75"/>
-      <c r="C117" s="66"/>
+      <c r="B117" s="58"/>
+      <c r="C117" s="57"/>
       <c r="D117" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E117" s="6"/>
       <c r="F117" s="5"/>
       <c r="G117" s="5"/>
     </row>
     <row r="118" spans="2:7">
-      <c r="B118" s="75"/>
-      <c r="C118" s="66"/>
-      <c r="D118" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="B118" s="58"/>
+      <c r="C118" s="5"/>
+      <c r="D118" s="5"/>
       <c r="E118" s="6"/>
       <c r="F118" s="5"/>
       <c r="G118" s="5"/>
     </row>
     <row r="119" spans="2:7">
-      <c r="B119" s="75"/>
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
+      <c r="B119" s="58"/>
+      <c r="C119" s="57" t="s">
+        <v>219</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="E119" s="6"/>
       <c r="F119" s="5"/>
       <c r="G119" s="5"/>
     </row>
     <row r="120" spans="2:7">
-      <c r="B120" s="75"/>
-      <c r="C120" s="66" t="s">
-        <v>228</v>
-      </c>
+      <c r="B120" s="58"/>
+      <c r="C120" s="57"/>
       <c r="D120" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E120" s="6"/>
       <c r="F120" s="5"/>
       <c r="G120" s="5"/>
     </row>
     <row r="121" spans="2:7">
-      <c r="B121" s="75"/>
-      <c r="C121" s="66"/>
+      <c r="B121" s="58"/>
+      <c r="C121" s="57"/>
       <c r="D121" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E121" s="6"/>
       <c r="F121" s="5"/>
       <c r="G121" s="5"/>
     </row>
     <row r="122" spans="2:7">
-      <c r="B122" s="75"/>
-      <c r="C122" s="66"/>
+      <c r="B122" s="58"/>
+      <c r="C122" s="57"/>
       <c r="D122" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E122" s="6"/>
       <c r="F122" s="5"/>
       <c r="G122" s="5"/>
     </row>
     <row r="123" spans="2:7">
-      <c r="B123" s="75"/>
-      <c r="C123" s="66"/>
+      <c r="B123" s="58"/>
+      <c r="C123" s="57"/>
       <c r="D123" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E123" s="6"/>
       <c r="F123" s="5"/>
       <c r="G123" s="5"/>
     </row>
     <row r="124" spans="2:7">
-      <c r="B124" s="75"/>
-      <c r="C124" s="66"/>
+      <c r="B124" s="58"/>
+      <c r="C124" s="57"/>
       <c r="D124" s="5" t="s">
-        <v>47</v>
+        <v>175</v>
       </c>
       <c r="E124" s="6"/>
       <c r="F124" s="5"/>
       <c r="G124" s="5"/>
     </row>
     <row r="125" spans="2:7">
-      <c r="B125" s="75"/>
-      <c r="C125" s="66"/>
-      <c r="D125" s="5" t="s">
-        <v>175</v>
+      <c r="B125" s="58"/>
+      <c r="C125" s="57"/>
+      <c r="D125" s="29" t="s">
+        <v>180</v>
       </c>
       <c r="E125" s="6"/>
       <c r="F125" s="5"/>
       <c r="G125" s="5"/>
     </row>
     <row r="126" spans="2:7">
-      <c r="B126" s="75"/>
-      <c r="C126" s="66"/>
-      <c r="D126" s="31" t="s">
-        <v>180</v>
+      <c r="B126" s="58"/>
+      <c r="C126" s="57"/>
+      <c r="D126" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="E126" s="6"/>
       <c r="F126" s="5"/>
       <c r="G126" s="5"/>
     </row>
     <row r="127" spans="2:7">
-      <c r="B127" s="75"/>
-      <c r="C127" s="66"/>
+      <c r="B127" s="58"/>
+      <c r="C127" s="57"/>
       <c r="D127" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E127" s="6"/>
       <c r="F127" s="5"/>
       <c r="G127" s="5"/>
     </row>
     <row r="128" spans="2:7">
-      <c r="B128" s="75"/>
-      <c r="C128" s="66"/>
-      <c r="D128" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="B128" s="58"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="5"/>
       <c r="E128" s="6"/>
       <c r="F128" s="5"/>
       <c r="G128" s="5"/>
     </row>
-    <row r="129" spans="2:7">
-      <c r="B129" s="75"/>
-      <c r="C129" s="5"/>
-      <c r="D129" s="5"/>
-      <c r="E129" s="6"/>
-      <c r="F129" s="5"/>
+    <row r="129" spans="2:7" ht="32.25">
+      <c r="B129" s="58"/>
+      <c r="C129" s="57" t="s">
+        <v>220</v>
+      </c>
+      <c r="E129" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="F129" s="49" t="s">
+        <v>253</v>
+      </c>
       <c r="G129" s="5"/>
     </row>
-    <row r="130" spans="2:7" ht="31.2">
-      <c r="B130" s="75"/>
-      <c r="C130" s="66" t="s">
-        <v>229</v>
-      </c>
-      <c r="E130" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="F130" s="52" t="s">
-        <v>262</v>
+    <row r="130" spans="2:7">
+      <c r="B130" s="58"/>
+      <c r="C130" s="57"/>
+      <c r="E130" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="F130" s="48" t="s">
+        <v>279</v>
       </c>
       <c r="G130" s="5"/>
     </row>
-    <row r="131" spans="2:7">
-      <c r="B131" s="75"/>
-      <c r="C131" s="66"/>
-      <c r="E131" s="49" t="s">
-        <v>196</v>
-      </c>
-      <c r="F131" s="51" t="s">
-        <v>291</v>
+    <row r="131" spans="2:7" ht="32.25">
+      <c r="B131" s="58"/>
+      <c r="C131" s="57"/>
+      <c r="D131" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E131" s="6"/>
+      <c r="F131" s="45" t="s">
+        <v>290</v>
       </c>
       <c r="G131" s="5"/>
     </row>
-    <row r="132" spans="2:7" ht="31.2">
-      <c r="B132" s="75"/>
-      <c r="C132" s="66"/>
+    <row r="132" spans="2:7">
+      <c r="B132" s="58"/>
+      <c r="C132" s="57"/>
       <c r="D132" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E132" s="6"/>
-      <c r="F132" s="48" t="s">
-        <v>303</v>
-      </c>
+      <c r="F132" s="5"/>
       <c r="G132" s="5"/>
     </row>
     <row r="133" spans="2:7">
-      <c r="B133" s="75"/>
-      <c r="C133" s="66"/>
+      <c r="B133" s="58"/>
+      <c r="C133" s="57"/>
       <c r="D133" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E133" s="6"/>
-      <c r="F133" s="5"/>
+      <c r="F133" s="45"/>
       <c r="G133" s="5"/>
     </row>
-    <row r="134" spans="2:7">
-      <c r="B134" s="75"/>
-      <c r="C134" s="66"/>
+    <row r="134" spans="2:7" ht="32.25">
+      <c r="B134" s="58"/>
+      <c r="C134" s="57"/>
       <c r="D134" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E134" s="6"/>
-      <c r="F134" s="48"/>
+      <c r="F134" s="45" t="s">
+        <v>289</v>
+      </c>
       <c r="G134" s="5"/>
     </row>
-    <row r="135" spans="2:7" ht="31.2">
-      <c r="B135" s="75"/>
-      <c r="C135" s="66"/>
-      <c r="D135" s="5" t="s">
-        <v>53</v>
+    <row r="135" spans="2:7">
+      <c r="B135" s="58"/>
+      <c r="C135" s="57"/>
+      <c r="D135" s="29" t="s">
+        <v>54</v>
       </c>
       <c r="E135" s="6"/>
-      <c r="F135" s="48" t="s">
-        <v>302</v>
-      </c>
+      <c r="F135" s="5"/>
       <c r="G135" s="5"/>
     </row>
     <row r="136" spans="2:7">
-      <c r="B136" s="75"/>
-      <c r="C136" s="66"/>
-      <c r="D136" s="31" t="s">
-        <v>54</v>
+      <c r="B136" s="58"/>
+      <c r="C136" s="57"/>
+      <c r="D136" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="E136" s="6"/>
       <c r="F136" s="5"/>
       <c r="G136" s="5"/>
     </row>
     <row r="137" spans="2:7">
-      <c r="B137" s="75"/>
-      <c r="C137" s="66"/>
+      <c r="B137" s="58"/>
+      <c r="C137" s="57"/>
       <c r="D137" s="5" t="s">
-        <v>55</v>
+        <v>163</v>
       </c>
       <c r="E137" s="6"/>
       <c r="F137" s="5"/>
       <c r="G137" s="5"/>
     </row>
     <row r="138" spans="2:7">
-      <c r="B138" s="75"/>
-      <c r="C138" s="66"/>
+      <c r="B138" s="58"/>
+      <c r="C138" s="57"/>
       <c r="D138" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E138" s="6"/>
       <c r="F138" s="5"/>
       <c r="G138" s="5"/>
     </row>
     <row r="139" spans="2:7">
-      <c r="B139" s="75"/>
-      <c r="C139" s="66"/>
+      <c r="B139" s="58"/>
+      <c r="C139" s="57"/>
       <c r="D139" s="5" t="s">
-        <v>164</v>
+        <v>56</v>
       </c>
       <c r="E139" s="6"/>
       <c r="F139" s="5"/>
       <c r="G139" s="5"/>
     </row>
     <row r="140" spans="2:7">
-      <c r="B140" s="75"/>
-      <c r="C140" s="66"/>
+      <c r="B140" s="58"/>
+      <c r="C140" s="57"/>
       <c r="D140" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E140" s="6"/>
       <c r="F140" s="5"/>
       <c r="G140" s="5"/>
     </row>
     <row r="141" spans="2:7">
-      <c r="B141" s="75"/>
-      <c r="C141" s="66"/>
+      <c r="B141" s="58"/>
+      <c r="C141" s="57"/>
       <c r="D141" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E141" s="6"/>
       <c r="F141" s="5"/>
       <c r="G141" s="5"/>
     </row>
     <row r="142" spans="2:7">
-      <c r="B142" s="75"/>
-      <c r="C142" s="66"/>
-      <c r="D142" s="5" t="s">
-        <v>58</v>
+      <c r="B142" s="58"/>
+      <c r="C142" s="57"/>
+      <c r="D142" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="E142" s="6"/>
       <c r="F142" s="5"/>
       <c r="G142" s="5"/>
     </row>
     <row r="143" spans="2:7">
-      <c r="B143" s="75"/>
-      <c r="C143" s="66"/>
-      <c r="D143" s="19" t="s">
-        <v>59</v>
-      </c>
+      <c r="B143" s="58"/>
+      <c r="C143" s="5"/>
+      <c r="D143" s="5"/>
       <c r="E143" s="6"/>
       <c r="F143" s="5"/>
       <c r="G143" s="5"/>
     </row>
     <row r="144" spans="2:7">
-      <c r="B144" s="75"/>
-      <c r="C144" s="5"/>
-      <c r="D144" s="5"/>
-      <c r="E144" s="6"/>
-      <c r="F144" s="5"/>
+      <c r="B144" s="58"/>
+      <c r="C144" s="57" t="s">
+        <v>221</v>
+      </c>
+      <c r="E144" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="F144" s="48" t="s">
+        <v>278</v>
+      </c>
       <c r="G144" s="5"/>
     </row>
     <row r="145" spans="2:7">
-      <c r="B145" s="75"/>
-      <c r="C145" s="66" t="s">
-        <v>230</v>
-      </c>
-      <c r="E145" s="49" t="s">
-        <v>196</v>
-      </c>
-      <c r="F145" s="51" t="s">
-        <v>290</v>
-      </c>
+      <c r="B145" s="58"/>
+      <c r="C145" s="57"/>
+      <c r="D145" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E145" s="6"/>
+      <c r="F145" s="5"/>
       <c r="G145" s="5"/>
     </row>
     <row r="146" spans="2:7">
-      <c r="B146" s="75"/>
-      <c r="C146" s="66"/>
+      <c r="B146" s="58"/>
+      <c r="C146" s="57"/>
       <c r="D146" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E146" s="6"/>
       <c r="F146" s="5"/>
       <c r="G146" s="5"/>
     </row>
     <row r="147" spans="2:7">
-      <c r="B147" s="75"/>
-      <c r="C147" s="66"/>
+      <c r="B147" s="58"/>
+      <c r="C147" s="57"/>
       <c r="D147" s="5" t="s">
-        <v>166</v>
+        <v>57</v>
       </c>
       <c r="E147" s="6"/>
       <c r="F147" s="5"/>
       <c r="G147" s="5"/>
     </row>
     <row r="148" spans="2:7">
-      <c r="B148" s="75"/>
-      <c r="C148" s="66"/>
+      <c r="B148" s="58"/>
+      <c r="C148" s="57"/>
       <c r="D148" s="5" t="s">
-        <v>57</v>
+        <v>167</v>
       </c>
       <c r="E148" s="6"/>
       <c r="F148" s="5"/>
       <c r="G148" s="5"/>
     </row>
     <row r="149" spans="2:7">
-      <c r="B149" s="75"/>
-      <c r="C149" s="66"/>
-      <c r="D149" s="5" t="s">
-        <v>167</v>
-      </c>
+      <c r="B149" s="58"/>
+      <c r="C149" s="5"/>
+      <c r="D149" s="5"/>
       <c r="E149" s="6"/>
       <c r="F149" s="5"/>
       <c r="G149" s="5"/>
     </row>
     <row r="150" spans="2:7">
-      <c r="B150" s="75"/>
-      <c r="C150" s="5"/>
-      <c r="D150" s="5"/>
-      <c r="E150" s="6"/>
-      <c r="F150" s="5"/>
+      <c r="B150" s="58"/>
+      <c r="C150" s="57" t="s">
+        <v>222</v>
+      </c>
+      <c r="D150" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="E150" s="8"/>
+      <c r="F150" s="7"/>
       <c r="G150" s="5"/>
     </row>
     <row r="151" spans="2:7">
-      <c r="B151" s="75"/>
-      <c r="C151" s="66" t="s">
-        <v>231</v>
-      </c>
-      <c r="D151" s="39" t="s">
-        <v>60</v>
+      <c r="B151" s="58"/>
+      <c r="C151" s="57"/>
+      <c r="D151" s="36" t="s">
+        <v>61</v>
       </c>
       <c r="E151" s="8"/>
       <c r="F151" s="7"/>
       <c r="G151" s="5"/>
     </row>
     <row r="152" spans="2:7">
-      <c r="B152" s="75"/>
-      <c r="C152" s="66"/>
-      <c r="D152" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="E152" s="8"/>
-      <c r="F152" s="7"/>
+      <c r="B152" s="58"/>
+      <c r="C152" s="5"/>
+      <c r="D152" s="5"/>
+      <c r="E152" s="6"/>
+      <c r="F152" s="5"/>
       <c r="G152" s="5"/>
     </row>
     <row r="153" spans="2:7">
-      <c r="B153" s="75"/>
-      <c r="C153" s="5"/>
-      <c r="D153" s="5"/>
-      <c r="E153" s="6"/>
-      <c r="F153" s="5"/>
+      <c r="B153" s="58"/>
+      <c r="C153" s="57" t="s">
+        <v>223</v>
+      </c>
+      <c r="D153" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E153" s="8"/>
+      <c r="F153" s="7"/>
       <c r="G153" s="5"/>
     </row>
     <row r="154" spans="2:7">
-      <c r="B154" s="75"/>
-      <c r="C154" s="66" t="s">
-        <v>232</v>
-      </c>
-      <c r="D154" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="E154" s="8"/>
-      <c r="F154" s="7"/>
+      <c r="B154" s="58"/>
+      <c r="C154" s="57"/>
+      <c r="D154" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E154" s="6"/>
+      <c r="F154" s="5"/>
       <c r="G154" s="5"/>
     </row>
     <row r="155" spans="2:7">
-      <c r="B155" s="75"/>
-      <c r="C155" s="66"/>
-      <c r="D155" s="5" t="s">
-        <v>63</v>
-      </c>
+      <c r="B155" s="58"/>
+      <c r="C155" s="5"/>
+      <c r="D155" s="5"/>
       <c r="E155" s="6"/>
       <c r="F155" s="5"/>
       <c r="G155" s="5"/>
     </row>
-    <row r="156" spans="2:7">
-      <c r="B156" s="75"/>
-      <c r="C156" s="5"/>
-      <c r="D156" s="5"/>
-      <c r="E156" s="6"/>
-      <c r="F156" s="5"/>
+    <row r="156" spans="2:7" ht="32.25">
+      <c r="B156" s="58"/>
+      <c r="C156" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="D156" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E156" s="8"/>
+      <c r="F156" s="7"/>
       <c r="G156" s="5"/>
     </row>
-    <row r="157" spans="2:7" ht="31.2">
-      <c r="B157" s="75"/>
-      <c r="C157" s="25" t="s">
-        <v>233</v>
-      </c>
-      <c r="D157" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E157" s="8"/>
-      <c r="F157" s="7"/>
+    <row r="157" spans="2:7">
+      <c r="B157" s="58"/>
+      <c r="C157" s="5"/>
+      <c r="D157" s="5"/>
+      <c r="E157" s="6"/>
+      <c r="F157" s="5"/>
       <c r="G157" s="5"/>
     </row>
     <row r="158" spans="2:7">
-      <c r="B158" s="75"/>
-      <c r="C158" s="5"/>
+      <c r="B158" s="58"/>
+      <c r="C158" s="23" t="s">
+        <v>225</v>
+      </c>
       <c r="D158" s="5"/>
       <c r="E158" s="6"/>
       <c r="F158" s="5"/>
       <c r="G158" s="5"/>
     </row>
     <row r="159" spans="2:7">
-      <c r="B159" s="75"/>
-      <c r="C159" s="25" t="s">
-        <v>234</v>
-      </c>
+      <c r="B159" s="58"/>
+      <c r="C159" s="5"/>
       <c r="D159" s="5"/>
       <c r="E159" s="6"/>
       <c r="F159" s="5"/>
       <c r="G159" s="5"/>
     </row>
     <row r="160" spans="2:7">
-      <c r="B160" s="75"/>
-      <c r="C160" s="5"/>
-      <c r="D160" s="5"/>
-      <c r="E160" s="6"/>
-      <c r="F160" s="5"/>
+      <c r="B160" s="58"/>
+      <c r="C160" s="57" t="s">
+        <v>226</v>
+      </c>
+      <c r="D160" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E160" s="13"/>
+      <c r="F160" s="12"/>
       <c r="G160" s="5"/>
     </row>
     <row r="161" spans="2:7">
-      <c r="B161" s="75"/>
-      <c r="C161" s="66" t="s">
-        <v>235</v>
-      </c>
-      <c r="D161" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="E161" s="15"/>
-      <c r="F161" s="14"/>
+      <c r="B161" s="58"/>
+      <c r="C161" s="57"/>
+      <c r="D161" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E161" s="6"/>
+      <c r="F161" s="5"/>
       <c r="G161" s="5"/>
     </row>
-    <row r="162" spans="2:7">
-      <c r="B162" s="75"/>
-      <c r="C162" s="66"/>
+    <row r="162" spans="2:7" ht="32.25">
+      <c r="B162" s="58"/>
+      <c r="C162" s="57"/>
       <c r="D162" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E162" s="6"/>
       <c r="F162" s="5"/>
       <c r="G162" s="5"/>
     </row>
-    <row r="163" spans="2:7" ht="31.2">
-      <c r="B163" s="75"/>
-      <c r="C163" s="66"/>
+    <row r="163" spans="2:7" ht="32.25">
+      <c r="B163" s="58"/>
+      <c r="C163" s="57"/>
       <c r="D163" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E163" s="6"/>
       <c r="F163" s="5"/>
       <c r="G163" s="5"/>
     </row>
-    <row r="164" spans="2:7" ht="31.2">
-      <c r="B164" s="75"/>
-      <c r="C164" s="66"/>
+    <row r="164" spans="2:7">
+      <c r="B164" s="58"/>
+      <c r="C164" s="57"/>
       <c r="D164" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E164" s="6"/>
       <c r="F164" s="5"/>
       <c r="G164" s="5"/>
     </row>
     <row r="165" spans="2:7">
-      <c r="B165" s="75"/>
-      <c r="C165" s="66"/>
+      <c r="B165" s="58"/>
+      <c r="C165" s="57"/>
       <c r="D165" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E165" s="6"/>
       <c r="F165" s="5"/>
       <c r="G165" s="5"/>
     </row>
     <row r="166" spans="2:7">
-      <c r="B166" s="75"/>
-      <c r="C166" s="66"/>
+      <c r="B166" s="58"/>
+      <c r="C166" s="57"/>
       <c r="D166" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E166" s="6"/>
       <c r="F166" s="5"/>
       <c r="G166" s="5"/>
     </row>
     <row r="167" spans="2:7">
-      <c r="B167" s="75"/>
-      <c r="C167" s="66"/>
-      <c r="D167" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="B167" s="58"/>
+      <c r="C167" s="5"/>
+      <c r="D167" s="5"/>
       <c r="E167" s="6"/>
       <c r="F167" s="5"/>
       <c r="G167" s="5"/>
     </row>
     <row r="168" spans="2:7">
-      <c r="B168" s="75"/>
-      <c r="C168" s="5"/>
-      <c r="D168" s="5"/>
+      <c r="B168" s="58"/>
+      <c r="C168" s="57" t="s">
+        <v>227</v>
+      </c>
+      <c r="D168" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="E168" s="6"/>
       <c r="F168" s="5"/>
       <c r="G168" s="5"/>
     </row>
     <row r="169" spans="2:7">
-      <c r="B169" s="75"/>
-      <c r="C169" s="66" t="s">
-        <v>236</v>
-      </c>
+      <c r="B169" s="58"/>
+      <c r="C169" s="57"/>
       <c r="D169" s="5" t="s">
-        <v>72</v>
+        <v>248</v>
       </c>
       <c r="E169" s="6"/>
       <c r="F169" s="5"/>
       <c r="G169" s="5"/>
     </row>
     <row r="170" spans="2:7">
-      <c r="B170" s="75"/>
-      <c r="C170" s="66"/>
+      <c r="B170" s="58"/>
+      <c r="C170" s="57"/>
       <c r="D170" s="5" t="s">
-        <v>257</v>
+        <v>73</v>
       </c>
       <c r="E170" s="6"/>
       <c r="F170" s="5"/>
       <c r="G170" s="5"/>
     </row>
     <row r="171" spans="2:7">
-      <c r="B171" s="75"/>
-      <c r="C171" s="66"/>
+      <c r="B171" s="58"/>
+      <c r="C171" s="57"/>
       <c r="D171" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E171" s="6"/>
       <c r="F171" s="5"/>
       <c r="G171" s="5"/>
     </row>
     <row r="172" spans="2:7">
-      <c r="B172" s="75"/>
-      <c r="C172" s="66"/>
+      <c r="B172" s="58"/>
+      <c r="C172" s="57"/>
       <c r="D172" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E172" s="6"/>
       <c r="F172" s="5"/>
       <c r="G172" s="5"/>
     </row>
     <row r="173" spans="2:7">
-      <c r="B173" s="75"/>
-      <c r="C173" s="66"/>
+      <c r="B173" s="58"/>
+      <c r="C173" s="57"/>
       <c r="D173" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E173" s="6"/>
       <c r="F173" s="5"/>
       <c r="G173" s="5"/>
     </row>
     <row r="174" spans="2:7">
-      <c r="B174" s="75"/>
-      <c r="C174" s="66"/>
+      <c r="B174" s="58"/>
+      <c r="C174" s="57"/>
       <c r="D174" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E174" s="6"/>
       <c r="F174" s="5"/>
       <c r="G174" s="5"/>
     </row>
     <row r="175" spans="2:7">
-      <c r="B175" s="75"/>
-      <c r="C175" s="66"/>
+      <c r="B175" s="58"/>
+      <c r="C175" s="57"/>
       <c r="D175" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E175" s="6"/>
       <c r="F175" s="5"/>
       <c r="G175" s="5"/>
     </row>
     <row r="176" spans="2:7">
-      <c r="B176" s="75"/>
-      <c r="C176" s="66"/>
-      <c r="D176" s="5" t="s">
-        <v>78</v>
-      </c>
+      <c r="B176" s="58"/>
+      <c r="C176" s="57"/>
+      <c r="D176" s="5"/>
       <c r="E176" s="6"/>
       <c r="F176" s="5"/>
       <c r="G176" s="5"/>
     </row>
     <row r="177" spans="2:7">
-      <c r="B177" s="75"/>
-      <c r="C177" s="66"/>
-      <c r="D177" s="5"/>
+      <c r="B177" s="58"/>
+      <c r="C177" s="57"/>
+      <c r="D177" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="E177" s="6"/>
       <c r="F177" s="5"/>
       <c r="G177" s="5"/>
     </row>
     <row r="178" spans="2:7">
-      <c r="B178" s="75"/>
-      <c r="C178" s="66"/>
-      <c r="D178" s="5" t="s">
-        <v>79</v>
+      <c r="B178" s="58"/>
+      <c r="C178" s="57"/>
+      <c r="D178" s="22" t="s">
+        <v>80</v>
       </c>
       <c r="E178" s="6"/>
       <c r="F178" s="5"/>
       <c r="G178" s="5"/>
     </row>
     <row r="179" spans="2:7">
-      <c r="B179" s="75"/>
-      <c r="C179" s="66"/>
-      <c r="D179" s="24" t="s">
-        <v>80</v>
+      <c r="B179" s="58"/>
+      <c r="C179" s="57"/>
+      <c r="D179" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="E179" s="6"/>
       <c r="F179" s="5"/>
       <c r="G179" s="5"/>
     </row>
     <row r="180" spans="2:7">
-      <c r="B180" s="75"/>
-      <c r="C180" s="66"/>
+      <c r="B180" s="58"/>
+      <c r="C180" s="57"/>
       <c r="D180" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E180" s="6"/>
       <c r="F180" s="5"/>
       <c r="G180" s="5"/>
     </row>
     <row r="181" spans="2:7">
-      <c r="B181" s="75"/>
-      <c r="C181" s="66"/>
-      <c r="D181" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E181" s="6"/>
-      <c r="F181" s="5"/>
+      <c r="B181" s="58"/>
+      <c r="C181" s="57"/>
+      <c r="D181" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E181" s="8"/>
+      <c r="F181" s="7"/>
       <c r="G181" s="5"/>
     </row>
     <row r="182" spans="2:7">
-      <c r="B182" s="75"/>
-      <c r="C182" s="66"/>
-      <c r="D182" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E182" s="8"/>
-      <c r="F182" s="7"/>
+      <c r="B182" s="24"/>
+      <c r="C182" s="5"/>
+      <c r="D182" s="5"/>
+      <c r="E182" s="6"/>
+      <c r="F182" s="5"/>
       <c r="G182" s="5"/>
     </row>
     <row r="183" spans="2:7">
-      <c r="B183" s="26"/>
-      <c r="C183" s="5"/>
-      <c r="D183" s="5"/>
-      <c r="E183" s="6"/>
-      <c r="F183" s="5"/>
-      <c r="G183" s="5"/>
+      <c r="B183" s="53" t="s">
+        <v>169</v>
+      </c>
+      <c r="C183" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="D183" s="14"/>
+      <c r="E183" s="15"/>
+      <c r="F183" s="25" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="184" spans="2:7">
-      <c r="B184" s="65" t="s">
-        <v>169</v>
-      </c>
-      <c r="C184" s="66" t="s">
-        <v>108</v>
-      </c>
-      <c r="D184" s="16"/>
-      <c r="E184" s="17"/>
-      <c r="F184" s="27" t="s">
-        <v>239</v>
-      </c>
+      <c r="B184" s="53"/>
+      <c r="C184" s="57"/>
+      <c r="D184" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E184" s="6"/>
+      <c r="F184" s="5"/>
+      <c r="G184" s="5"/>
     </row>
     <row r="185" spans="2:7">
-      <c r="B185" s="65"/>
-      <c r="C185" s="66"/>
+      <c r="B185" s="53"/>
+      <c r="C185" s="57"/>
       <c r="D185" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E185" s="6"/>
       <c r="F185" s="5"/>
       <c r="G185" s="5"/>
     </row>
     <row r="186" spans="2:7">
-      <c r="B186" s="65"/>
-      <c r="C186" s="66"/>
+      <c r="B186" s="53"/>
+      <c r="C186" s="57"/>
       <c r="D186" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E186" s="6"/>
       <c r="F186" s="5"/>
       <c r="G186" s="5"/>
     </row>
     <row r="187" spans="2:7">
-      <c r="B187" s="65"/>
-      <c r="C187" s="66"/>
+      <c r="B187" s="53"/>
+      <c r="C187" s="57"/>
       <c r="D187" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E187" s="6"/>
       <c r="F187" s="5"/>
       <c r="G187" s="5"/>
     </row>
     <row r="188" spans="2:7">
-      <c r="B188" s="65"/>
-      <c r="C188" s="66"/>
+      <c r="B188" s="53"/>
+      <c r="C188" s="57"/>
       <c r="D188" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E188" s="6"/>
       <c r="F188" s="5"/>
       <c r="G188" s="5"/>
     </row>
     <row r="189" spans="2:7">
-      <c r="B189" s="65"/>
-      <c r="C189" s="66"/>
+      <c r="B189" s="53"/>
+      <c r="C189" s="57"/>
       <c r="D189" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E189" s="6"/>
       <c r="F189" s="5"/>
       <c r="G189" s="5"/>
     </row>
     <row r="190" spans="2:7">
-      <c r="B190" s="65"/>
-      <c r="C190" s="66"/>
+      <c r="B190" s="53"/>
+      <c r="C190" s="57"/>
       <c r="D190" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E190" s="6"/>
       <c r="F190" s="5"/>
       <c r="G190" s="5"/>
     </row>
     <row r="191" spans="2:7">
-      <c r="B191" s="65"/>
-      <c r="C191" s="66"/>
+      <c r="B191" s="53"/>
+      <c r="C191" s="57"/>
       <c r="D191" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E191" s="6"/>
       <c r="F191" s="5"/>
       <c r="G191" s="5"/>
     </row>
     <row r="192" spans="2:7">
-      <c r="B192" s="65"/>
-      <c r="C192" s="66"/>
+      <c r="B192" s="53"/>
+      <c r="C192" s="57"/>
       <c r="D192" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E192" s="6"/>
       <c r="F192" s="5"/>
       <c r="G192" s="5"/>
     </row>
     <row r="193" spans="2:7">
-      <c r="B193" s="65"/>
-      <c r="C193" s="66"/>
+      <c r="B193" s="53"/>
+      <c r="C193" s="57"/>
       <c r="D193" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E193" s="6"/>
       <c r="F193" s="5"/>
       <c r="G193" s="5"/>
     </row>
-    <row r="194" spans="2:7">
-      <c r="B194" s="65"/>
-      <c r="C194" s="66"/>
+    <row r="194" spans="2:7" ht="32.25">
+      <c r="B194" s="53"/>
+      <c r="C194" s="57"/>
       <c r="D194" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E194" s="6"/>
       <c r="F194" s="5"/>
       <c r="G194" s="5"/>
     </row>
-    <row r="195" spans="2:7" ht="31.2">
-      <c r="B195" s="65"/>
-      <c r="C195" s="66"/>
+    <row r="195" spans="2:7">
+      <c r="B195" s="53"/>
+      <c r="C195" s="57"/>
       <c r="D195" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E195" s="6"/>
       <c r="F195" s="5"/>
       <c r="G195" s="5"/>
     </row>
-    <row r="196" spans="2:7">
-      <c r="B196" s="65"/>
-      <c r="C196" s="66"/>
-      <c r="D196" s="5" t="s">
-        <v>120</v>
+    <row r="196" spans="2:7" ht="32.25">
+      <c r="B196" s="53"/>
+      <c r="C196" s="57"/>
+      <c r="D196" s="33" t="s">
+        <v>209</v>
       </c>
       <c r="E196" s="6"/>
-      <c r="F196" s="5"/>
-      <c r="G196" s="5"/>
-    </row>
-    <row r="197" spans="2:7" ht="31.2">
-      <c r="B197" s="65"/>
-      <c r="C197" s="66"/>
-      <c r="D197" s="36" t="s">
-        <v>212</v>
+      <c r="F196" s="43"/>
+      <c r="G196" s="40" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="197" spans="2:7">
+      <c r="B197" s="53"/>
+      <c r="C197" s="57"/>
+      <c r="D197" s="33" t="s">
+        <v>271</v>
       </c>
       <c r="E197" s="6"/>
-      <c r="F197" s="46"/>
-      <c r="G197" s="43" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="198" spans="2:7" ht="31.2">
-      <c r="B198" s="65"/>
-      <c r="C198" s="66"/>
-      <c r="D198" s="36" t="s">
-        <v>280</v>
+      <c r="F197" s="5"/>
+      <c r="G197" s="5"/>
+    </row>
+    <row r="198" spans="2:7">
+      <c r="B198" s="53"/>
+      <c r="C198" s="57"/>
+      <c r="D198" s="33" t="s">
+        <v>269</v>
       </c>
       <c r="E198" s="6"/>
-      <c r="F198" s="5"/>
-      <c r="G198" s="5"/>
+      <c r="F198" s="43"/>
+      <c r="G198" s="43"/>
     </row>
     <row r="199" spans="2:7">
-      <c r="B199" s="65"/>
-      <c r="C199" s="66"/>
-      <c r="D199" s="36" t="s">
-        <v>278</v>
+      <c r="B199" s="53"/>
+      <c r="C199" s="57"/>
+      <c r="D199" s="5" t="s">
+        <v>121</v>
       </c>
       <c r="E199" s="6"/>
-      <c r="F199" s="46"/>
-      <c r="G199" s="46"/>
+      <c r="F199" s="5"/>
+      <c r="G199" s="5"/>
     </row>
     <row r="200" spans="2:7">
-      <c r="B200" s="65"/>
-      <c r="C200" s="66"/>
+      <c r="B200" s="53"/>
+      <c r="C200" s="57"/>
       <c r="D200" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E200" s="6"/>
       <c r="F200" s="5"/>
       <c r="G200" s="5"/>
     </row>
     <row r="201" spans="2:7">
-      <c r="B201" s="65"/>
-      <c r="C201" s="66"/>
+      <c r="B201" s="53"/>
+      <c r="C201" s="57"/>
       <c r="D201" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E201" s="6"/>
       <c r="F201" s="5"/>
       <c r="G201" s="5"/>
     </row>
     <row r="202" spans="2:7">
-      <c r="B202" s="65"/>
-      <c r="C202" s="66"/>
+      <c r="B202" s="53"/>
+      <c r="C202" s="57"/>
       <c r="D202" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E202" s="6"/>
       <c r="F202" s="5"/>
       <c r="G202" s="5"/>
     </row>
     <row r="203" spans="2:7">
-      <c r="B203" s="65"/>
-      <c r="C203" s="66"/>
+      <c r="B203" s="53"/>
+      <c r="C203" s="57"/>
       <c r="D203" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E203" s="6"/>
       <c r="F203" s="5"/>
       <c r="G203" s="5"/>
     </row>
     <row r="204" spans="2:7">
-      <c r="B204" s="65"/>
-      <c r="C204" s="66"/>
+      <c r="B204" s="53"/>
+      <c r="C204" s="57"/>
       <c r="D204" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E204" s="6"/>
       <c r="F204" s="5"/>
       <c r="G204" s="5"/>
     </row>
     <row r="205" spans="2:7">
-      <c r="B205" s="65"/>
-      <c r="C205" s="66"/>
+      <c r="B205" s="53"/>
+      <c r="C205" s="57"/>
       <c r="D205" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E205" s="6"/>
       <c r="F205" s="5"/>
       <c r="G205" s="5"/>
     </row>
     <row r="206" spans="2:7">
-      <c r="B206" s="65"/>
-      <c r="C206" s="66"/>
-      <c r="D206" s="5" t="s">
-        <v>127</v>
-      </c>
+      <c r="B206" s="53"/>
+      <c r="C206" s="5"/>
+      <c r="D206" s="5"/>
       <c r="E206" s="6"/>
       <c r="F206" s="5"/>
       <c r="G206" s="5"/>
     </row>
     <row r="207" spans="2:7">
-      <c r="B207" s="65"/>
-      <c r="C207" s="5"/>
-      <c r="D207" s="5"/>
+      <c r="B207" s="53"/>
+      <c r="C207" s="57" t="s">
+        <v>128</v>
+      </c>
+      <c r="D207" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="E207" s="6"/>
       <c r="F207" s="5"/>
       <c r="G207" s="5"/>
     </row>
     <row r="208" spans="2:7">
-      <c r="B208" s="65"/>
-      <c r="C208" s="66" t="s">
-        <v>128</v>
-      </c>
+      <c r="B208" s="53"/>
+      <c r="C208" s="57"/>
       <c r="D208" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E208" s="6"/>
       <c r="F208" s="5"/>
       <c r="G208" s="5"/>
     </row>
     <row r="209" spans="2:7">
-      <c r="B209" s="65"/>
-      <c r="C209" s="66"/>
+      <c r="B209" s="53"/>
+      <c r="C209" s="57"/>
       <c r="D209" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E209" s="6"/>
       <c r="F209" s="5"/>
       <c r="G209" s="5"/>
     </row>
     <row r="210" spans="2:7">
-      <c r="B210" s="65"/>
-      <c r="C210" s="66"/>
+      <c r="B210" s="53"/>
+      <c r="C210" s="57"/>
       <c r="D210" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E210" s="6"/>
       <c r="F210" s="5"/>
       <c r="G210" s="5"/>
     </row>
     <row r="211" spans="2:7">
-      <c r="B211" s="65"/>
-      <c r="C211" s="66"/>
+      <c r="B211" s="53"/>
+      <c r="C211" s="57"/>
       <c r="D211" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E211" s="6"/>
       <c r="F211" s="5"/>
       <c r="G211" s="5"/>
     </row>
     <row r="212" spans="2:7">
-      <c r="B212" s="65"/>
-      <c r="C212" s="66"/>
+      <c r="B212" s="53"/>
+      <c r="C212" s="57"/>
       <c r="D212" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E212" s="6"/>
       <c r="F212" s="5"/>
       <c r="G212" s="5"/>
     </row>
     <row r="213" spans="2:7">
-      <c r="B213" s="65"/>
-      <c r="C213" s="66"/>
+      <c r="B213" s="53"/>
+      <c r="C213" s="57"/>
       <c r="D213" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E213" s="6"/>
       <c r="F213" s="5"/>
       <c r="G213" s="5"/>
     </row>
     <row r="214" spans="2:7">
-      <c r="B214" s="65"/>
-      <c r="C214" s="66"/>
-      <c r="D214" s="5" t="s">
-        <v>135</v>
-      </c>
+      <c r="B214" s="24"/>
+      <c r="C214" s="5"/>
+      <c r="D214" s="5"/>
       <c r="E214" s="6"/>
       <c r="F214" s="5"/>
       <c r="G214" s="5"/>
     </row>
-    <row r="215" spans="2:7">
-      <c r="B215" s="26"/>
+    <row r="215" spans="2:7" ht="32.25">
+      <c r="B215" s="52" t="s">
+        <v>139</v>
+      </c>
       <c r="C215" s="5"/>
-      <c r="D215" s="5"/>
-      <c r="E215" s="6"/>
-      <c r="F215" s="5"/>
-      <c r="G215" s="5"/>
-    </row>
-    <row r="216" spans="2:7" ht="31.2">
-      <c r="B216" s="67" t="s">
-        <v>139</v>
-      </c>
+      <c r="D215" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="E215" s="46"/>
+      <c r="F215" s="47" t="s">
+        <v>256</v>
+      </c>
+      <c r="G215" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="216" spans="2:7">
+      <c r="B216" s="52"/>
       <c r="C216" s="5"/>
-      <c r="D216" s="36" t="s">
-        <v>140</v>
-      </c>
-      <c r="E216" s="49"/>
-      <c r="F216" s="50" t="s">
-        <v>265</v>
-      </c>
-      <c r="G216" s="11" t="s">
-        <v>238</v>
-      </c>
+      <c r="D216" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E216" s="6"/>
+      <c r="F216" s="5"/>
+      <c r="G216" s="5"/>
     </row>
     <row r="217" spans="2:7">
-      <c r="B217" s="67"/>
+      <c r="B217" s="52"/>
       <c r="C217" s="5"/>
       <c r="D217" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E217" s="6"/>
       <c r="F217" s="5"/>
       <c r="G217" s="5"/>
     </row>
     <row r="218" spans="2:7">
-      <c r="B218" s="67"/>
+      <c r="B218" s="52"/>
       <c r="C218" s="5"/>
       <c r="D218" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E218" s="6"/>
       <c r="F218" s="5"/>
       <c r="G218" s="5"/>
     </row>
     <row r="219" spans="2:7">
-      <c r="B219" s="67"/>
+      <c r="B219" s="52"/>
       <c r="C219" s="5"/>
       <c r="D219" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E219" s="6"/>
       <c r="F219" s="5"/>
       <c r="G219" s="5"/>
     </row>
     <row r="220" spans="2:7">
-      <c r="B220" s="67"/>
+      <c r="B220" s="52"/>
       <c r="C220" s="5"/>
       <c r="D220" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E220" s="6"/>
       <c r="F220" s="5"/>
       <c r="G220" s="5"/>
     </row>
     <row r="221" spans="2:7">
-      <c r="B221" s="67"/>
+      <c r="B221" s="52"/>
       <c r="C221" s="5"/>
       <c r="D221" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E221" s="6"/>
       <c r="F221" s="5"/>
       <c r="G221" s="5"/>
     </row>
     <row r="222" spans="2:7">
-      <c r="B222" s="67"/>
+      <c r="B222" s="24"/>
       <c r="C222" s="5"/>
-      <c r="D222" s="5" t="s">
-        <v>146</v>
-      </c>
+      <c r="D222" s="5"/>
       <c r="E222" s="6"/>
       <c r="F222" s="5"/>
       <c r="G222" s="5"/>
     </row>
     <row r="223" spans="2:7">
-      <c r="B223" s="26"/>
+      <c r="B223" s="59" t="s">
+        <v>185</v>
+      </c>
       <c r="C223" s="5"/>
-      <c r="D223" s="5"/>
-      <c r="E223" s="6"/>
-      <c r="F223" s="5"/>
+      <c r="D223" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="E223" s="13"/>
+      <c r="F223" s="12"/>
       <c r="G223" s="5"/>
     </row>
     <row r="224" spans="2:7">
-      <c r="B224" s="63" t="s">
-        <v>185</v>
-      </c>
+      <c r="B224" s="60"/>
       <c r="C224" s="5"/>
-      <c r="D224" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="E224" s="15"/>
-      <c r="F224" s="14"/>
+      <c r="D224" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="E224" s="13"/>
+      <c r="F224" s="12"/>
       <c r="G224" s="5"/>
     </row>
     <row r="225" spans="2:7">
-      <c r="B225" s="76"/>
+      <c r="B225" s="60"/>
       <c r="C225" s="5"/>
-      <c r="D225" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="E225" s="15"/>
-      <c r="F225" s="14"/>
+      <c r="D225" s="32"/>
+      <c r="E225" s="6"/>
+      <c r="F225" s="32"/>
       <c r="G225" s="5"/>
     </row>
     <row r="226" spans="2:7">
-      <c r="B226" s="76"/>
+      <c r="B226" s="60"/>
       <c r="C226" s="5"/>
-      <c r="D226" s="35"/>
+      <c r="D226" s="5"/>
       <c r="E226" s="6"/>
-      <c r="F226" s="35"/>
+      <c r="F226" s="5"/>
       <c r="G226" s="5"/>
     </row>
     <row r="227" spans="2:7">
-      <c r="B227" s="76"/>
+      <c r="B227" s="60"/>
       <c r="C227" s="5"/>
       <c r="D227" s="5"/>
       <c r="E227" s="6"/>
@@ -4687,7 +4762,7 @@
       <c r="G227" s="5"/>
     </row>
     <row r="228" spans="2:7">
-      <c r="B228" s="76"/>
+      <c r="B228" s="60"/>
       <c r="C228" s="5"/>
       <c r="D228" s="5"/>
       <c r="E228" s="6"/>
@@ -4695,7 +4770,7 @@
       <c r="G228" s="5"/>
     </row>
     <row r="229" spans="2:7">
-      <c r="B229" s="76"/>
+      <c r="B229" s="60"/>
       <c r="C229" s="5"/>
       <c r="D229" s="5"/>
       <c r="E229" s="6"/>
@@ -4703,7 +4778,7 @@
       <c r="G229" s="5"/>
     </row>
     <row r="230" spans="2:7">
-      <c r="B230" s="76"/>
+      <c r="B230" s="60"/>
       <c r="C230" s="5"/>
       <c r="D230" s="5"/>
       <c r="E230" s="6"/>
@@ -4711,7 +4786,7 @@
       <c r="G230" s="5"/>
     </row>
     <row r="231" spans="2:7">
-      <c r="B231" s="76"/>
+      <c r="B231" s="60"/>
       <c r="C231" s="5"/>
       <c r="D231" s="5"/>
       <c r="E231" s="6"/>
@@ -4719,7 +4794,7 @@
       <c r="G231" s="5"/>
     </row>
     <row r="232" spans="2:7">
-      <c r="B232" s="76"/>
+      <c r="B232" s="60"/>
       <c r="C232" s="5"/>
       <c r="D232" s="5"/>
       <c r="E232" s="6"/>
@@ -4727,7 +4802,7 @@
       <c r="G232" s="5"/>
     </row>
     <row r="233" spans="2:7">
-      <c r="B233" s="76"/>
+      <c r="B233" s="60"/>
       <c r="C233" s="5"/>
       <c r="D233" s="5"/>
       <c r="E233" s="6"/>
@@ -4735,7 +4810,7 @@
       <c r="G233" s="5"/>
     </row>
     <row r="234" spans="2:7">
-      <c r="B234" s="76"/>
+      <c r="B234" s="60"/>
       <c r="C234" s="5"/>
       <c r="D234" s="5"/>
       <c r="E234" s="6"/>
@@ -4743,7 +4818,7 @@
       <c r="G234" s="5"/>
     </row>
     <row r="235" spans="2:7">
-      <c r="B235" s="76"/>
+      <c r="B235" s="60"/>
       <c r="C235" s="5"/>
       <c r="D235" s="5"/>
       <c r="E235" s="6"/>
@@ -4751,7 +4826,7 @@
       <c r="G235" s="5"/>
     </row>
     <row r="236" spans="2:7">
-      <c r="B236" s="76"/>
+      <c r="B236" s="60"/>
       <c r="C236" s="5"/>
       <c r="D236" s="5"/>
       <c r="E236" s="6"/>
@@ -4759,7 +4834,7 @@
       <c r="G236" s="5"/>
     </row>
     <row r="237" spans="2:7">
-      <c r="B237" s="76"/>
+      <c r="B237" s="61"/>
       <c r="C237" s="5"/>
       <c r="D237" s="5"/>
       <c r="E237" s="6"/>
@@ -4767,7 +4842,7 @@
       <c r="G237" s="5"/>
     </row>
     <row r="238" spans="2:7">
-      <c r="B238" s="64"/>
+      <c r="B238" s="24"/>
       <c r="C238" s="5"/>
       <c r="D238" s="5"/>
       <c r="E238" s="6"/>
@@ -4775,29 +4850,29 @@
       <c r="G238" s="5"/>
     </row>
     <row r="239" spans="2:7">
-      <c r="B239" s="26"/>
-      <c r="C239" s="5"/>
+      <c r="B239" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="C239" s="22" t="s">
+        <v>245</v>
+      </c>
       <c r="D239" s="5"/>
       <c r="E239" s="6"/>
-      <c r="F239" s="5"/>
+      <c r="F239" s="5" t="s">
+        <v>246</v>
+      </c>
       <c r="G239" s="5"/>
     </row>
     <row r="240" spans="2:7">
-      <c r="B240" s="68" t="s">
-        <v>253</v>
-      </c>
-      <c r="C240" s="24" t="s">
-        <v>254</v>
-      </c>
+      <c r="B240" s="63"/>
+      <c r="C240" s="5"/>
       <c r="D240" s="5"/>
       <c r="E240" s="6"/>
-      <c r="F240" s="5" t="s">
-        <v>255</v>
-      </c>
+      <c r="F240" s="5"/>
       <c r="G240" s="5"/>
     </row>
     <row r="241" spans="2:7">
-      <c r="B241" s="69"/>
+      <c r="B241" s="64"/>
       <c r="C241" s="5"/>
       <c r="D241" s="5"/>
       <c r="E241" s="6"/>
@@ -4805,7 +4880,7 @@
       <c r="G241" s="5"/>
     </row>
     <row r="242" spans="2:7">
-      <c r="B242" s="70"/>
+      <c r="B242" s="64"/>
       <c r="C242" s="5"/>
       <c r="D242" s="5"/>
       <c r="E242" s="6"/>
@@ -4813,7 +4888,7 @@
       <c r="G242" s="5"/>
     </row>
     <row r="243" spans="2:7">
-      <c r="B243" s="70"/>
+      <c r="B243" s="65"/>
       <c r="C243" s="5"/>
       <c r="D243" s="5"/>
       <c r="E243" s="6"/>
@@ -4821,230 +4896,216 @@
       <c r="G243" s="5"/>
     </row>
     <row r="244" spans="2:7">
-      <c r="B244" s="71"/>
+      <c r="B244" s="21"/>
       <c r="C244" s="5"/>
       <c r="D244" s="5"/>
       <c r="E244" s="6"/>
       <c r="F244" s="5"/>
       <c r="G244" s="5"/>
     </row>
-    <row r="245" spans="2:7">
-      <c r="B245" s="23"/>
+    <row r="245" spans="2:7" ht="48.4">
+      <c r="B245" s="59" t="s">
+        <v>191</v>
+      </c>
       <c r="C245" s="5"/>
-      <c r="D245" s="5"/>
-      <c r="E245" s="6"/>
-      <c r="F245" s="5"/>
+      <c r="D245" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="E245" s="16"/>
+      <c r="F245" s="11"/>
       <c r="G245" s="5"/>
     </row>
-    <row r="246" spans="2:7" ht="46.8">
-      <c r="B246" s="63" t="s">
-        <v>191</v>
-      </c>
+    <row r="246" spans="2:7" ht="32.25">
+      <c r="B246" s="61"/>
       <c r="C246" s="5"/>
       <c r="D246" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="E246" s="18"/>
+        <v>190</v>
+      </c>
+      <c r="E246" s="16"/>
       <c r="F246" s="11"/>
       <c r="G246" s="5"/>
     </row>
-    <row r="247" spans="2:7" ht="31.2">
-      <c r="B247" s="64"/>
+    <row r="247" spans="2:7">
+      <c r="B247" s="24"/>
       <c r="C247" s="5"/>
-      <c r="D247" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="E247" s="18"/>
-      <c r="F247" s="11"/>
+      <c r="D247" s="5"/>
+      <c r="E247" s="6"/>
+      <c r="F247" s="5"/>
       <c r="G247" s="5"/>
     </row>
     <row r="248" spans="2:7">
-      <c r="B248" s="26"/>
+      <c r="B248" s="52" t="s">
+        <v>147</v>
+      </c>
       <c r="C248" s="5"/>
-      <c r="D248" s="5"/>
+      <c r="D248" s="5" t="s">
+        <v>148</v>
+      </c>
       <c r="E248" s="6"/>
       <c r="F248" s="5"/>
       <c r="G248" s="5"/>
     </row>
     <row r="249" spans="2:7">
-      <c r="B249" s="67" t="s">
-        <v>147</v>
-      </c>
+      <c r="B249" s="52"/>
       <c r="C249" s="5"/>
       <c r="D249" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E249" s="6"/>
       <c r="F249" s="5"/>
       <c r="G249" s="5"/>
     </row>
     <row r="250" spans="2:7">
-      <c r="B250" s="67"/>
+      <c r="B250" s="52"/>
       <c r="C250" s="5"/>
       <c r="D250" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E250" s="6"/>
       <c r="F250" s="5"/>
       <c r="G250" s="5"/>
     </row>
     <row r="251" spans="2:7">
-      <c r="B251" s="67"/>
+      <c r="B251" s="52"/>
       <c r="C251" s="5"/>
       <c r="D251" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E251" s="6"/>
       <c r="F251" s="5"/>
       <c r="G251" s="5"/>
     </row>
     <row r="252" spans="2:7">
-      <c r="B252" s="67"/>
+      <c r="B252" s="52"/>
       <c r="C252" s="5"/>
       <c r="D252" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E252" s="6"/>
       <c r="F252" s="5"/>
       <c r="G252" s="5"/>
     </row>
-    <row r="253" spans="2:7">
-      <c r="B253" s="67"/>
+    <row r="253" spans="2:7" ht="32.25">
+      <c r="B253" s="52"/>
       <c r="C253" s="5"/>
       <c r="D253" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E253" s="6"/>
       <c r="F253" s="5"/>
       <c r="G253" s="5"/>
     </row>
-    <row r="254" spans="2:7" ht="46.8">
-      <c r="B254" s="67"/>
+    <row r="254" spans="2:7" ht="32.25">
+      <c r="B254" s="52"/>
       <c r="C254" s="5"/>
       <c r="D254" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E254" s="6"/>
       <c r="F254" s="5"/>
       <c r="G254" s="5"/>
     </row>
-    <row r="255" spans="2:7" ht="31.2">
-      <c r="B255" s="67"/>
+    <row r="255" spans="2:7">
+      <c r="B255" s="52"/>
       <c r="C255" s="5"/>
       <c r="D255" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E255" s="6"/>
       <c r="F255" s="5"/>
       <c r="G255" s="5"/>
     </row>
     <row r="256" spans="2:7">
-      <c r="B256" s="67"/>
+      <c r="B256" s="52"/>
       <c r="C256" s="5"/>
       <c r="D256" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E256" s="6"/>
       <c r="F256" s="5"/>
       <c r="G256" s="5"/>
     </row>
     <row r="257" spans="2:7">
-      <c r="B257" s="67"/>
+      <c r="B257" s="52"/>
       <c r="C257" s="5"/>
       <c r="D257" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E257" s="6"/>
       <c r="F257" s="5"/>
       <c r="G257" s="5"/>
     </row>
-    <row r="258" spans="2:7">
-      <c r="B258" s="67"/>
+    <row r="258" spans="2:7" ht="32.25">
+      <c r="B258" s="52"/>
       <c r="C258" s="5"/>
       <c r="D258" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E258" s="6"/>
       <c r="F258" s="5"/>
       <c r="G258" s="5"/>
     </row>
-    <row r="259" spans="2:7" ht="31.2">
-      <c r="B259" s="67"/>
+    <row r="259" spans="2:7" ht="32.25">
+      <c r="B259" s="52"/>
       <c r="C259" s="5"/>
       <c r="D259" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E259" s="6"/>
       <c r="F259" s="5"/>
       <c r="G259" s="5"/>
     </row>
-    <row r="260" spans="2:7" ht="31.2">
-      <c r="B260" s="67"/>
+    <row r="260" spans="2:7" ht="32.25">
+      <c r="B260" s="52"/>
       <c r="C260" s="5"/>
       <c r="D260" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E260" s="6"/>
       <c r="F260" s="5"/>
       <c r="G260" s="5"/>
     </row>
-    <row r="261" spans="2:7" ht="31.2">
-      <c r="B261" s="67"/>
+    <row r="261" spans="2:7" ht="32.25">
+      <c r="B261" s="52"/>
       <c r="C261" s="5"/>
       <c r="D261" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E261" s="6"/>
       <c r="F261" s="5"/>
       <c r="G261" s="5"/>
     </row>
-    <row r="262" spans="2:7" ht="31.2">
-      <c r="B262" s="67"/>
+    <row r="262" spans="2:7">
+      <c r="B262" s="52"/>
       <c r="C262" s="5"/>
       <c r="D262" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E262" s="6"/>
       <c r="F262" s="5"/>
       <c r="G262" s="5"/>
     </row>
-    <row r="263" spans="2:7">
-      <c r="B263" s="67"/>
-      <c r="C263" s="5"/>
-      <c r="D263" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="E263" s="6"/>
-      <c r="F263" s="5"/>
-      <c r="G263" s="5"/>
-    </row>
-    <row r="268" spans="2:7" ht="31.2">
-      <c r="E268" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="F268" s="22" t="s">
-        <v>293</v>
+    <row r="267" spans="2:7">
+      <c r="E267" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="F267" s="20" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B249:B263"/>
-    <mergeCell ref="B98:B106"/>
-    <mergeCell ref="C57:C66"/>
-    <mergeCell ref="C68:C82"/>
-    <mergeCell ref="B57:B82"/>
-    <mergeCell ref="B84:B96"/>
-    <mergeCell ref="B108:B109"/>
-    <mergeCell ref="B184:B214"/>
-    <mergeCell ref="C184:C206"/>
-    <mergeCell ref="C208:C214"/>
-    <mergeCell ref="B115:B182"/>
-    <mergeCell ref="C115:C118"/>
-    <mergeCell ref="C120:C128"/>
-    <mergeCell ref="C130:C143"/>
-    <mergeCell ref="B224:B238"/>
-    <mergeCell ref="C161:C167"/>
-    <mergeCell ref="B246:B247"/>
+    <mergeCell ref="D104:D105"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="D92:D93"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D68:D70"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="D80:D81"/>
+    <mergeCell ref="B245:B246"/>
     <mergeCell ref="B4:B55"/>
     <mergeCell ref="C4:C23"/>
     <mergeCell ref="C25:C29"/>
@@ -5052,47 +5113,53 @@
     <mergeCell ref="C40:C49"/>
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="C54:C55"/>
-    <mergeCell ref="B111:B113"/>
-    <mergeCell ref="B216:B222"/>
-    <mergeCell ref="C169:C182"/>
-    <mergeCell ref="B240:B244"/>
-    <mergeCell ref="C145:C149"/>
-    <mergeCell ref="C151:C152"/>
-    <mergeCell ref="C154:C155"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D68:D70"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="D80:D81"/>
-    <mergeCell ref="D105:D106"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="D93:D94"/>
-    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="B110:B112"/>
+    <mergeCell ref="B215:B221"/>
+    <mergeCell ref="C168:C181"/>
+    <mergeCell ref="B239:B243"/>
+    <mergeCell ref="C144:C148"/>
+    <mergeCell ref="C150:C151"/>
+    <mergeCell ref="C153:C154"/>
+    <mergeCell ref="B248:B262"/>
+    <mergeCell ref="B97:B105"/>
+    <mergeCell ref="C57:C66"/>
+    <mergeCell ref="C68:C81"/>
+    <mergeCell ref="B57:B81"/>
+    <mergeCell ref="B83:B95"/>
+    <mergeCell ref="B107:B108"/>
+    <mergeCell ref="B183:B213"/>
+    <mergeCell ref="C183:C205"/>
+    <mergeCell ref="C207:C213"/>
+    <mergeCell ref="B114:B181"/>
+    <mergeCell ref="C114:C117"/>
+    <mergeCell ref="C119:C127"/>
+    <mergeCell ref="C129:C142"/>
+    <mergeCell ref="B223:B237"/>
+    <mergeCell ref="C160:C166"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D246" r:id="rId1"/>
-    <hyperlink ref="D247" r:id="rId2"/>
+    <hyperlink ref="D245" r:id="rId1"/>
+    <hyperlink ref="D246" r:id="rId2"/>
     <hyperlink ref="G68" r:id="rId3"/>
     <hyperlink ref="G69" r:id="rId4"/>
-    <hyperlink ref="G99" r:id="rId5"/>
+    <hyperlink ref="G98" r:id="rId5"/>
     <hyperlink ref="G73" r:id="rId6"/>
     <hyperlink ref="G63" r:id="rId7"/>
     <hyperlink ref="G71" r:id="rId8"/>
     <hyperlink ref="G8" r:id="rId9" display="https://www.youtube.com/watch?v=7HCd074v8g8"/>
     <hyperlink ref="G4" r:id="rId10" location="1039525" display="https://math.stackexchange.com/questions/1039519/finding-prime-factors-by-taking-the-square-root/1039525#1039525"/>
-    <hyperlink ref="G216" r:id="rId11"/>
-    <hyperlink ref="F184" r:id="rId12"/>
+    <hyperlink ref="G215" r:id="rId11"/>
+    <hyperlink ref="F183" r:id="rId12"/>
     <hyperlink ref="F57" r:id="rId13" display="https://www.geeksforgeeks.org/advanced-data-structures/"/>
     <hyperlink ref="G77" r:id="rId14"/>
     <hyperlink ref="G76" r:id="rId15" display="https://www.youtube.com/watch?v=uxA__b23t2w"/>
     <hyperlink ref="G80" r:id="rId16"/>
-    <hyperlink ref="G96" r:id="rId17"/>
-    <hyperlink ref="G93" r:id="rId18"/>
-    <hyperlink ref="G101" r:id="rId19"/>
-    <hyperlink ref="G197" r:id="rId20"/>
-    <hyperlink ref="G105" r:id="rId21"/>
-    <hyperlink ref="G64" r:id="rId22"/>
+    <hyperlink ref="G95" r:id="rId17"/>
+    <hyperlink ref="G92" r:id="rId18"/>
+    <hyperlink ref="G100" r:id="rId19"/>
+    <hyperlink ref="G196" r:id="rId20"/>
+    <hyperlink ref="G104" r:id="rId21"/>
+    <hyperlink ref="G64" r:id="rId22" display="https://stackoverflow.com/questions/36814088/understanding-how-rolling-hash-works-with-modulus-in-rabin-karp-algorithm"/>
     <hyperlink ref="G32" r:id="rId23"/>
     <hyperlink ref="G11" r:id="rId24"/>
   </hyperlinks>
@@ -5103,77 +5170,67 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:D9"/>
+  <dimension ref="B2:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="16.149999999999999"/>
   <cols>
-    <col min="1" max="1" width="7.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="56.21875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="7.19921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.8984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="46.19921875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="56.19921875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
-      <c r="B2" s="77" t="s">
-        <v>211</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>210</v>
+    <row r="2" spans="2:4" s="3" customFormat="1">
+      <c r="B2" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="2:4">
-      <c r="B3" s="78"/>
+      <c r="B3" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="78"/>
-    </row>
-    <row r="5" spans="2:4" ht="31.2">
-      <c r="B5" s="78"/>
-      <c r="C5" s="1" t="s">
-        <v>212</v>
+      <c r="B4" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="1" t="s">
+        <v>301</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="28.8">
-      <c r="B6" s="78"/>
-      <c r="C6" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="78"/>
-      <c r="C7" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="78"/>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="78"/>
+        <v>302</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:B9"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1"/>
-    <hyperlink ref="D5" r:id="rId2" display="https://www.geeksforgeeks.org/maximum-size-rectangle-binary-sub-matrix-1s/"/>
-    <hyperlink ref="D7" r:id="rId3"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>